<commit_message>
ASK-41 Also read temporal results for common sections
</commit_message>
<xml_diff>
--- a/benchmarktests/testdefinitions/Benchmartktest_traject 13-2.xlsx
+++ b/benchmarktests/testdefinitions/Benchmartktest_traject 13-2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\src\wbi-assemblage-rekenkern\benchmarktests\testdefinitions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32BD9E56-E684-4F8C-836A-7A7F63919F33}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA4447A6-DE8A-4B9B-8F9B-07C27E9443C0}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3855" yWindow="3855" windowWidth="28800" windowHeight="15435" firstSheet="1" activeTab="1" xr2:uid="{0831170E-5124-493D-8FBC-5E58312EFD65}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="1" activeTab="10" xr2:uid="{0831170E-5124-493D-8FBC-5E58312EFD65}"/>
   </bookViews>
   <sheets>
     <sheet name="Informatiepagina" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="476" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="477" uniqueCount="137">
   <si>
     <t>Vaknaam</t>
   </si>
@@ -449,6 +449,9 @@
   </si>
   <si>
     <t>Lengte-effect</t>
+  </si>
+  <si>
+    <t>Gecombineerd (tussentijds)</t>
   </si>
 </sst>
 </file>
@@ -2477,51 +2480,55 @@
   <sheetPr>
     <tabColor rgb="FF9900FF"/>
   </sheetPr>
-  <dimension ref="B1:K135"/>
+  <dimension ref="B1:L135"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D3" sqref="D3:D40"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3:E40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="3.28515625" customWidth="1"/>
     <col min="4" max="4" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.28515625" customWidth="1"/>
+    <col min="8" max="8" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C1" s="9"/>
     </row>
-    <row r="2" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B2" s="9"/>
       <c r="C2" s="14"/>
       <c r="D2" s="63" t="s">
         <v>114</v>
       </c>
-      <c r="E2" s="47" t="s">
+      <c r="E2" s="63" t="s">
+        <v>136</v>
+      </c>
+      <c r="F2" s="48" t="s">
         <v>77</v>
       </c>
-      <c r="F2" s="48" t="s">
+      <c r="G2" s="48" t="s">
         <v>78</v>
       </c>
-      <c r="G2" s="48" t="s">
+      <c r="H2" s="48" t="s">
         <v>79</v>
       </c>
-      <c r="H2" s="48" t="s">
+      <c r="I2" s="48" t="s">
         <v>80</v>
       </c>
-      <c r="I2" s="48" t="s">
+      <c r="J2" s="48" t="s">
         <v>81</v>
       </c>
-      <c r="J2" s="48" t="s">
+      <c r="K2" s="48" t="s">
         <v>101</v>
       </c>
-      <c r="K2" s="49" t="s">
+      <c r="L2" s="49" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="3" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B3" s="3">
         <v>0</v>
       </c>
@@ -2529,39 +2536,43 @@
         <v>0.27700000000000002</v>
       </c>
       <c r="D3" s="22" t="str">
-        <f t="shared" ref="D3:D40" si="0">IF(COUNTIF(E3:K3,"D")&gt;0,"D",IF(COUNTIF(E3:K3,"-III")&gt;0,"-III",IF(COUNTIF(E3:K3,"-II")&gt;0,"-II",IF(COUNTIF(E3:K3,"-I")&gt;0,"-I",IF(COUNTIF(E3:K3,"+0")&gt;0,"+0",IF(COUNTIF(E3:K3,"+I")&gt;0,"+I",IF(COUNTIF(E3:K3,"+II")&gt;0,"+II",IF(COUNTIF(E3:K3,"+III")&gt;0,"+III","ND"))))))))</f>
+        <f t="shared" ref="D3:D40" si="0">IF(COUNTIF(F3:L3,"D")&gt;0,"D",IF(COUNTIF(F3:L3,"-III")&gt;0,"-III",IF(COUNTIF(F3:L3,"-II")&gt;0,"-II",IF(COUNTIF(F3:L3,"-I")&gt;0,"-I",IF(COUNTIF(F3:L3,"+0")&gt;0,"+0",IF(COUNTIF(F3:L3,"+I")&gt;0,"+I",IF(COUNTIF(F3:L3,"+II")&gt;0,"+II",IF(COUNTIF(F3:L3,"+III")&gt;0,"+III","ND"))))))))</f>
         <v>+0</v>
       </c>
-      <c r="E3" s="4" t="str">
-        <f t="array" ref="E3">INDEX(STPH!$O$11:$O$30,IFERROR(MATCH(MIN(IF(STPH!$D$11:$D$30&gt;AVERAGE(B3,C3),STPH!$D$11:$D$30)),STPH!$D$11:$D$30),1))</f>
-        <v>+III</v>
+      <c r="E3" s="22" t="str">
+        <f t="shared" ref="E3:E40" si="1">IF(COUNTIF(F3:L3,"-III")&gt;0,"-III",IF(COUNTIF(F3:L3,"-II")&gt;0,"-II",IF(COUNTIF(F3:L3,"-I")&gt;0,"-I",IF(COUNTIF(F3:L3,"+0")&gt;0,"+0",IF(COUNTIF(F3:L3,"+I")&gt;0,"+I",IF(COUNTIF(F3:L3,"+II")&gt;0,"+II",IF(COUNTIF(F3:L3,"+III")&gt;0,"+III","ND")))))))</f>
+        <v>+0</v>
       </c>
       <c r="F3" s="4" t="str">
-        <f t="array" ref="F3">INDEX(STBI!$O$11:$O$30,IFERROR(MATCH(MIN(IF(STBI!$D$11:$D$30&gt;AVERAGE(B3,C3),STBI!$D$11:$D$30)),STBI!$D$11:$D$30),1))</f>
+        <f t="array" ref="F3">INDEX(STPH!$O$11:$O$30,IFERROR(MATCH(MIN(IF(STPH!$D$11:$D$30&gt;AVERAGE(B3,C3),STPH!$D$11:$D$30)),STPH!$D$11:$D$30),1))</f>
         <v>+III</v>
       </c>
       <c r="G3" s="4" t="str">
-        <f t="array" ref="G3">INDEX(GEKB!$K$11:$K$30,IFERROR(MATCH(MIN(IF(GEKB!$D$11:$D$30&gt;AVERAGE(B3,C3),GEKB!$D$11:$D$30)),GEKB!$D$11:$D$30),1))</f>
-        <v>+III</v>
-      </c>
-      <c r="H3" s="4">
-        <f t="array" ref="H3">INDEX(DA!$K$50:$K$71,IFERROR(MATCH(MIN(IF(DA!$D$50:$D$71&gt;AVERAGE(B3,C3),DA!$D$50:$D$71)),DA!$D$50:$D$71),1))</f>
-        <v>0</v>
-      </c>
-      <c r="I3" s="4" t="str">
-        <f t="array" ref="I3">INDEX(STKWp!$K$11:$K$30,IFERROR(MATCH(MIN(IF(STKWp!$D$11:$D$30&gt;AVERAGE(B3,C3),STKWp!$D$11:$D$30)),STKWp!$D$11:$D$30),1))</f>
-        <v>+III</v>
+        <f t="array" ref="G3">INDEX(STBI!$O$11:$O$30,IFERROR(MATCH(MIN(IF(STBI!$D$11:$D$30&gt;AVERAGE(B3,C3),STBI!$D$11:$D$30)),STBI!$D$11:$D$30),1))</f>
+        <v>+III</v>
+      </c>
+      <c r="H3" s="4" t="str">
+        <f t="array" ref="H3">INDEX(GEKB!$K$11:$K$30,IFERROR(MATCH(MIN(IF(GEKB!$D$11:$D$30&gt;AVERAGE(B3,C3),GEKB!$D$11:$D$30)),GEKB!$D$11:$D$30),1))</f>
+        <v>+III</v>
+      </c>
+      <c r="I3" s="4">
+        <f t="array" ref="I3">INDEX(DA!$K$50:$K$71,IFERROR(MATCH(MIN(IF(DA!$D$50:$D$71&gt;AVERAGE(B3,C3),DA!$D$50:$D$71)),DA!$D$50:$D$71),1))</f>
+        <v>0</v>
       </c>
       <c r="J3" s="4" t="str">
-        <f t="array" ref="J3">INDEX(BSKW!$K$11:$K$30,IFERROR(MATCH(MIN(IF(BSKW!$D$11:$D$30&gt;AVERAGE(B3,C3),BSKW!$D$11:$D$30)),BSKW!$D$11:$D$30),1))</f>
-        <v>+III</v>
-      </c>
-      <c r="K3" s="7" t="str">
-        <f t="array" ref="K3">INDEX(HTKW!$K$11:$K$30,IFERROR(MATCH(MIN(IF(HTKW!$D$11:$D$30&gt;AVERAGE(B3,C3),HTKW!$D$11:$D$30)),HTKW!$D$11:$D$30),1))</f>
-        <v>+III</v>
-      </c>
-    </row>
-    <row r="4" spans="2:11" x14ac:dyDescent="0.25">
+        <f t="array" ref="J3">INDEX(STKWp!$K$11:$K$30,IFERROR(MATCH(MIN(IF(STKWp!$D$11:$D$30&gt;AVERAGE(B3,C3),STKWp!$D$11:$D$30)),STKWp!$D$11:$D$30),1))</f>
+        <v>+III</v>
+      </c>
+      <c r="K3" s="4" t="str">
+        <f t="array" ref="K3">INDEX(BSKW!$K$11:$K$30,IFERROR(MATCH(MIN(IF(BSKW!$D$11:$D$30&gt;AVERAGE(B3,C3),BSKW!$D$11:$D$30)),BSKW!$D$11:$D$30),1))</f>
+        <v>+III</v>
+      </c>
+      <c r="L3" s="7" t="str">
+        <f t="array" ref="L3">INDEX(HTKW!$K$11:$K$30,IFERROR(MATCH(MIN(IF(HTKW!$D$11:$D$30&gt;AVERAGE(B3,C3),HTKW!$D$11:$D$30)),HTKW!$D$11:$D$30),1))</f>
+        <v>+III</v>
+      </c>
+    </row>
+    <row r="4" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B4" s="8">
         <v>0.27700000000000002</v>
       </c>
@@ -2572,36 +2583,40 @@
         <f t="shared" si="0"/>
         <v>+0</v>
       </c>
-      <c r="E4" s="9" t="str">
-        <f t="array" ref="E4">INDEX(STPH!$O$11:$O$30,IFERROR(MATCH(MIN(IF(STPH!$D$11:$D$30&gt;AVERAGE(B4,C4),STPH!$D$11:$D$30)),STPH!$D$11:$D$30),1))</f>
-        <v>+III</v>
+      <c r="E4" s="23" t="str">
+        <f t="shared" si="1"/>
+        <v>+0</v>
       </c>
       <c r="F4" s="9" t="str">
-        <f t="array" ref="F4">INDEX(STBI!$O$11:$O$30,IFERROR(MATCH(MIN(IF(STBI!$D$11:$D$30&gt;AVERAGE(B4,C4),STBI!$D$11:$D$30)),STBI!$D$11:$D$30),1))</f>
+        <f t="array" ref="F4">INDEX(STPH!$O$11:$O$30,IFERROR(MATCH(MIN(IF(STPH!$D$11:$D$30&gt;AVERAGE(B4,C4),STPH!$D$11:$D$30)),STPH!$D$11:$D$30),1))</f>
         <v>+III</v>
       </c>
       <c r="G4" s="9" t="str">
-        <f t="array" ref="G4">INDEX(GEKB!$K$11:$K$30,IFERROR(MATCH(MIN(IF(GEKB!$D$11:$D$30&gt;AVERAGE(B4,C4),GEKB!$D$11:$D$30)),GEKB!$D$11:$D$30),1))</f>
-        <v>+III</v>
-      </c>
-      <c r="H4" s="9">
-        <f t="array" ref="H4">INDEX(DA!$K$50:$K$71,IFERROR(MATCH(MIN(IF(DA!$D$50:$D$71&gt;AVERAGE(B4,C4),DA!$D$50:$D$71)),DA!$D$50:$D$71),1))</f>
-        <v>0</v>
-      </c>
-      <c r="I4" s="9" t="str">
-        <f t="array" ref="I4">INDEX(STKWp!$K$11:$K$30,IFERROR(MATCH(MIN(IF(STKWp!$D$11:$D$30&gt;AVERAGE(B4,C4),STKWp!$D$11:$D$30)),STKWp!$D$11:$D$30),1))</f>
-        <v>+III</v>
+        <f t="array" ref="G4">INDEX(STBI!$O$11:$O$30,IFERROR(MATCH(MIN(IF(STBI!$D$11:$D$30&gt;AVERAGE(B4,C4),STBI!$D$11:$D$30)),STBI!$D$11:$D$30),1))</f>
+        <v>+III</v>
+      </c>
+      <c r="H4" s="9" t="str">
+        <f t="array" ref="H4">INDEX(GEKB!$K$11:$K$30,IFERROR(MATCH(MIN(IF(GEKB!$D$11:$D$30&gt;AVERAGE(B4,C4),GEKB!$D$11:$D$30)),GEKB!$D$11:$D$30),1))</f>
+        <v>+III</v>
+      </c>
+      <c r="I4" s="9">
+        <f t="array" ref="I4">INDEX(DA!$K$50:$K$71,IFERROR(MATCH(MIN(IF(DA!$D$50:$D$71&gt;AVERAGE(B4,C4),DA!$D$50:$D$71)),DA!$D$50:$D$71),1))</f>
+        <v>0</v>
       </c>
       <c r="J4" s="9" t="str">
-        <f t="array" ref="J4">INDEX(BSKW!$K$11:$K$30,IFERROR(MATCH(MIN(IF(BSKW!$D$11:$D$30&gt;AVERAGE(B4,C4),BSKW!$D$11:$D$30)),BSKW!$D$11:$D$30),1))</f>
-        <v>+III</v>
-      </c>
-      <c r="K4" s="12" t="str">
-        <f t="array" ref="K4">INDEX(HTKW!$K$11:$K$30,IFERROR(MATCH(MIN(IF(HTKW!$D$11:$D$30&gt;AVERAGE(B4,C4),HTKW!$D$11:$D$30)),HTKW!$D$11:$D$30),1))</f>
-        <v>+III</v>
-      </c>
-    </row>
-    <row r="5" spans="2:11" x14ac:dyDescent="0.25">
+        <f t="array" ref="J4">INDEX(STKWp!$K$11:$K$30,IFERROR(MATCH(MIN(IF(STKWp!$D$11:$D$30&gt;AVERAGE(B4,C4),STKWp!$D$11:$D$30)),STKWp!$D$11:$D$30),1))</f>
+        <v>+III</v>
+      </c>
+      <c r="K4" s="9" t="str">
+        <f t="array" ref="K4">INDEX(BSKW!$K$11:$K$30,IFERROR(MATCH(MIN(IF(BSKW!$D$11:$D$30&gt;AVERAGE(B4,C4),BSKW!$D$11:$D$30)),BSKW!$D$11:$D$30),1))</f>
+        <v>+III</v>
+      </c>
+      <c r="L4" s="12" t="str">
+        <f t="array" ref="L4">INDEX(HTKW!$K$11:$K$30,IFERROR(MATCH(MIN(IF(HTKW!$D$11:$D$30&gt;AVERAGE(B4,C4),HTKW!$D$11:$D$30)),HTKW!$D$11:$D$30),1))</f>
+        <v>+III</v>
+      </c>
+    </row>
+    <row r="5" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B5" s="8">
         <v>0.53200000000000003</v>
       </c>
@@ -2612,36 +2627,40 @@
         <f t="shared" si="0"/>
         <v>+0</v>
       </c>
-      <c r="E5" s="9" t="str">
-        <f t="array" ref="E5">INDEX(STPH!$O$11:$O$30,IFERROR(MATCH(MIN(IF(STPH!$D$11:$D$30&gt;AVERAGE(B5,C5),STPH!$D$11:$D$30)),STPH!$D$11:$D$30),1))</f>
-        <v>+III</v>
+      <c r="E5" s="23" t="str">
+        <f t="shared" si="1"/>
+        <v>+0</v>
       </c>
       <c r="F5" s="9" t="str">
-        <f t="array" ref="F5">INDEX(STBI!$O$11:$O$30,IFERROR(MATCH(MIN(IF(STBI!$D$11:$D$30&gt;AVERAGE(B5,C5),STBI!$D$11:$D$30)),STBI!$D$11:$D$30),1))</f>
+        <f t="array" ref="F5">INDEX(STPH!$O$11:$O$30,IFERROR(MATCH(MIN(IF(STPH!$D$11:$D$30&gt;AVERAGE(B5,C5),STPH!$D$11:$D$30)),STPH!$D$11:$D$30),1))</f>
         <v>+III</v>
       </c>
       <c r="G5" s="9" t="str">
-        <f t="array" ref="G5">INDEX(GEKB!$K$11:$K$30,IFERROR(MATCH(MIN(IF(GEKB!$D$11:$D$30&gt;AVERAGE(B5,C5),GEKB!$D$11:$D$30)),GEKB!$D$11:$D$30),1))</f>
-        <v>+III</v>
-      </c>
-      <c r="H5" s="9">
-        <f t="array" ref="H5">INDEX(DA!$K$50:$K$71,IFERROR(MATCH(MIN(IF(DA!$D$50:$D$71&gt;AVERAGE(B5,C5),DA!$D$50:$D$71)),DA!$D$50:$D$71),1))</f>
-        <v>0</v>
-      </c>
-      <c r="I5" s="9" t="str">
-        <f t="array" ref="I5">INDEX(STKWp!$K$11:$K$30,IFERROR(MATCH(MIN(IF(STKWp!$D$11:$D$30&gt;AVERAGE(B5,C5),STKWp!$D$11:$D$30)),STKWp!$D$11:$D$30),1))</f>
-        <v>+III</v>
+        <f t="array" ref="G5">INDEX(STBI!$O$11:$O$30,IFERROR(MATCH(MIN(IF(STBI!$D$11:$D$30&gt;AVERAGE(B5,C5),STBI!$D$11:$D$30)),STBI!$D$11:$D$30),1))</f>
+        <v>+III</v>
+      </c>
+      <c r="H5" s="9" t="str">
+        <f t="array" ref="H5">INDEX(GEKB!$K$11:$K$30,IFERROR(MATCH(MIN(IF(GEKB!$D$11:$D$30&gt;AVERAGE(B5,C5),GEKB!$D$11:$D$30)),GEKB!$D$11:$D$30),1))</f>
+        <v>+III</v>
+      </c>
+      <c r="I5" s="9">
+        <f t="array" ref="I5">INDEX(DA!$K$50:$K$71,IFERROR(MATCH(MIN(IF(DA!$D$50:$D$71&gt;AVERAGE(B5,C5),DA!$D$50:$D$71)),DA!$D$50:$D$71),1))</f>
+        <v>0</v>
       </c>
       <c r="J5" s="9" t="str">
-        <f t="array" ref="J5">INDEX(BSKW!$K$11:$K$30,IFERROR(MATCH(MIN(IF(BSKW!$D$11:$D$30&gt;AVERAGE(B5,C5),BSKW!$D$11:$D$30)),BSKW!$D$11:$D$30),1))</f>
-        <v>+III</v>
-      </c>
-      <c r="K5" s="12" t="str">
-        <f t="array" ref="K5">INDEX(HTKW!$K$11:$K$30,IFERROR(MATCH(MIN(IF(HTKW!$D$11:$D$30&gt;AVERAGE(B5,C5),HTKW!$D$11:$D$30)),HTKW!$D$11:$D$30),1))</f>
-        <v>+III</v>
-      </c>
-    </row>
-    <row r="6" spans="2:11" x14ac:dyDescent="0.25">
+        <f t="array" ref="J5">INDEX(STKWp!$K$11:$K$30,IFERROR(MATCH(MIN(IF(STKWp!$D$11:$D$30&gt;AVERAGE(B5,C5),STKWp!$D$11:$D$30)),STKWp!$D$11:$D$30),1))</f>
+        <v>+III</v>
+      </c>
+      <c r="K5" s="9" t="str">
+        <f t="array" ref="K5">INDEX(BSKW!$K$11:$K$30,IFERROR(MATCH(MIN(IF(BSKW!$D$11:$D$30&gt;AVERAGE(B5,C5),BSKW!$D$11:$D$30)),BSKW!$D$11:$D$30),1))</f>
+        <v>+III</v>
+      </c>
+      <c r="L5" s="12" t="str">
+        <f t="array" ref="L5">INDEX(HTKW!$K$11:$K$30,IFERROR(MATCH(MIN(IF(HTKW!$D$11:$D$30&gt;AVERAGE(B5,C5),HTKW!$D$11:$D$30)),HTKW!$D$11:$D$30),1))</f>
+        <v>+III</v>
+      </c>
+    </row>
+    <row r="6" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B6" s="8">
         <v>0.755</v>
       </c>
@@ -2652,36 +2671,40 @@
         <f t="shared" si="0"/>
         <v>+0</v>
       </c>
-      <c r="E6" s="9" t="str">
-        <f t="array" ref="E6">INDEX(STPH!$O$11:$O$30,IFERROR(MATCH(MIN(IF(STPH!$D$11:$D$30&gt;AVERAGE(B6,C6),STPH!$D$11:$D$30)),STPH!$D$11:$D$30),1))</f>
-        <v>+III</v>
+      <c r="E6" s="23" t="str">
+        <f t="shared" si="1"/>
+        <v>+0</v>
       </c>
       <c r="F6" s="9" t="str">
-        <f t="array" ref="F6">INDEX(STBI!$O$11:$O$30,IFERROR(MATCH(MIN(IF(STBI!$D$11:$D$30&gt;AVERAGE(B6,C6),STBI!$D$11:$D$30)),STBI!$D$11:$D$30),1))</f>
+        <f t="array" ref="F6">INDEX(STPH!$O$11:$O$30,IFERROR(MATCH(MIN(IF(STPH!$D$11:$D$30&gt;AVERAGE(B6,C6),STPH!$D$11:$D$30)),STPH!$D$11:$D$30),1))</f>
         <v>+III</v>
       </c>
       <c r="G6" s="9" t="str">
-        <f t="array" ref="G6">INDEX(GEKB!$K$11:$K$30,IFERROR(MATCH(MIN(IF(GEKB!$D$11:$D$30&gt;AVERAGE(B6,C6),GEKB!$D$11:$D$30)),GEKB!$D$11:$D$30),1))</f>
-        <v>+III</v>
-      </c>
-      <c r="H6" s="9">
-        <f t="array" ref="H6">INDEX(DA!$K$50:$K$71,IFERROR(MATCH(MIN(IF(DA!$D$50:$D$71&gt;AVERAGE(B6,C6),DA!$D$50:$D$71)),DA!$D$50:$D$71),1))</f>
-        <v>0</v>
-      </c>
-      <c r="I6" s="9" t="str">
-        <f t="array" ref="I6">INDEX(STKWp!$K$11:$K$30,IFERROR(MATCH(MIN(IF(STKWp!$D$11:$D$30&gt;AVERAGE(B6,C6),STKWp!$D$11:$D$30)),STKWp!$D$11:$D$30),1))</f>
-        <v>+III</v>
+        <f t="array" ref="G6">INDEX(STBI!$O$11:$O$30,IFERROR(MATCH(MIN(IF(STBI!$D$11:$D$30&gt;AVERAGE(B6,C6),STBI!$D$11:$D$30)),STBI!$D$11:$D$30),1))</f>
+        <v>+III</v>
+      </c>
+      <c r="H6" s="9" t="str">
+        <f t="array" ref="H6">INDEX(GEKB!$K$11:$K$30,IFERROR(MATCH(MIN(IF(GEKB!$D$11:$D$30&gt;AVERAGE(B6,C6),GEKB!$D$11:$D$30)),GEKB!$D$11:$D$30),1))</f>
+        <v>+III</v>
+      </c>
+      <c r="I6" s="9">
+        <f t="array" ref="I6">INDEX(DA!$K$50:$K$71,IFERROR(MATCH(MIN(IF(DA!$D$50:$D$71&gt;AVERAGE(B6,C6),DA!$D$50:$D$71)),DA!$D$50:$D$71),1))</f>
+        <v>0</v>
       </c>
       <c r="J6" s="9" t="str">
-        <f t="array" ref="J6">INDEX(BSKW!$K$11:$K$30,IFERROR(MATCH(MIN(IF(BSKW!$D$11:$D$30&gt;AVERAGE(B6,C6),BSKW!$D$11:$D$30)),BSKW!$D$11:$D$30),1))</f>
-        <v>+III</v>
-      </c>
-      <c r="K6" s="12" t="str">
-        <f t="array" ref="K6">INDEX(HTKW!$K$11:$K$30,IFERROR(MATCH(MIN(IF(HTKW!$D$11:$D$30&gt;AVERAGE(B6,C6),HTKW!$D$11:$D$30)),HTKW!$D$11:$D$30),1))</f>
-        <v>+III</v>
-      </c>
-    </row>
-    <row r="7" spans="2:11" x14ac:dyDescent="0.25">
+        <f t="array" ref="J6">INDEX(STKWp!$K$11:$K$30,IFERROR(MATCH(MIN(IF(STKWp!$D$11:$D$30&gt;AVERAGE(B6,C6),STKWp!$D$11:$D$30)),STKWp!$D$11:$D$30),1))</f>
+        <v>+III</v>
+      </c>
+      <c r="K6" s="9" t="str">
+        <f t="array" ref="K6">INDEX(BSKW!$K$11:$K$30,IFERROR(MATCH(MIN(IF(BSKW!$D$11:$D$30&gt;AVERAGE(B6,C6),BSKW!$D$11:$D$30)),BSKW!$D$11:$D$30),1))</f>
+        <v>+III</v>
+      </c>
+      <c r="L6" s="12" t="str">
+        <f t="array" ref="L6">INDEX(HTKW!$K$11:$K$30,IFERROR(MATCH(MIN(IF(HTKW!$D$11:$D$30&gt;AVERAGE(B6,C6),HTKW!$D$11:$D$30)),HTKW!$D$11:$D$30),1))</f>
+        <v>+III</v>
+      </c>
+    </row>
+    <row r="7" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B7" s="8">
         <v>0.91300000000000003</v>
       </c>
@@ -2692,36 +2715,40 @@
         <f t="shared" si="0"/>
         <v>+0</v>
       </c>
-      <c r="E7" s="9" t="str">
-        <f t="array" ref="E7">INDEX(STPH!$O$11:$O$30,IFERROR(MATCH(MIN(IF(STPH!$D$11:$D$30&gt;AVERAGE(B7,C7),STPH!$D$11:$D$30)),STPH!$D$11:$D$30),1))</f>
-        <v>+III</v>
+      <c r="E7" s="23" t="str">
+        <f t="shared" si="1"/>
+        <v>+0</v>
       </c>
       <c r="F7" s="9" t="str">
-        <f t="array" ref="F7">INDEX(STBI!$O$11:$O$30,IFERROR(MATCH(MIN(IF(STBI!$D$11:$D$30&gt;AVERAGE(B7,C7),STBI!$D$11:$D$30)),STBI!$D$11:$D$30),1))</f>
+        <f t="array" ref="F7">INDEX(STPH!$O$11:$O$30,IFERROR(MATCH(MIN(IF(STPH!$D$11:$D$30&gt;AVERAGE(B7,C7),STPH!$D$11:$D$30)),STPH!$D$11:$D$30),1))</f>
         <v>+III</v>
       </c>
       <c r="G7" s="9" t="str">
-        <f t="array" ref="G7">INDEX(GEKB!$K$11:$K$30,IFERROR(MATCH(MIN(IF(GEKB!$D$11:$D$30&gt;AVERAGE(B7,C7),GEKB!$D$11:$D$30)),GEKB!$D$11:$D$30),1))</f>
-        <v>+III</v>
-      </c>
-      <c r="H7" s="9">
-        <f t="array" ref="H7">INDEX(DA!$K$50:$K$71,IFERROR(MATCH(MIN(IF(DA!$D$50:$D$71&gt;AVERAGE(B7,C7),DA!$D$50:$D$71)),DA!$D$50:$D$71),1))</f>
-        <v>0</v>
-      </c>
-      <c r="I7" s="9" t="str">
-        <f t="array" ref="I7">INDEX(STKWp!$K$11:$K$30,IFERROR(MATCH(MIN(IF(STKWp!$D$11:$D$30&gt;AVERAGE(B7,C7),STKWp!$D$11:$D$30)),STKWp!$D$11:$D$30),1))</f>
-        <v>+III</v>
+        <f t="array" ref="G7">INDEX(STBI!$O$11:$O$30,IFERROR(MATCH(MIN(IF(STBI!$D$11:$D$30&gt;AVERAGE(B7,C7),STBI!$D$11:$D$30)),STBI!$D$11:$D$30),1))</f>
+        <v>+III</v>
+      </c>
+      <c r="H7" s="9" t="str">
+        <f t="array" ref="H7">INDEX(GEKB!$K$11:$K$30,IFERROR(MATCH(MIN(IF(GEKB!$D$11:$D$30&gt;AVERAGE(B7,C7),GEKB!$D$11:$D$30)),GEKB!$D$11:$D$30),1))</f>
+        <v>+III</v>
+      </c>
+      <c r="I7" s="9">
+        <f t="array" ref="I7">INDEX(DA!$K$50:$K$71,IFERROR(MATCH(MIN(IF(DA!$D$50:$D$71&gt;AVERAGE(B7,C7),DA!$D$50:$D$71)),DA!$D$50:$D$71),1))</f>
+        <v>0</v>
       </c>
       <c r="J7" s="9" t="str">
-        <f t="array" ref="J7">INDEX(BSKW!$K$11:$K$30,IFERROR(MATCH(MIN(IF(BSKW!$D$11:$D$30&gt;AVERAGE(B7,C7),BSKW!$D$11:$D$30)),BSKW!$D$11:$D$30),1))</f>
-        <v>+III</v>
-      </c>
-      <c r="K7" s="12" t="str">
-        <f t="array" ref="K7">INDEX(HTKW!$K$11:$K$30,IFERROR(MATCH(MIN(IF(HTKW!$D$11:$D$30&gt;AVERAGE(B7,C7),HTKW!$D$11:$D$30)),HTKW!$D$11:$D$30),1))</f>
-        <v>+III</v>
-      </c>
-    </row>
-    <row r="8" spans="2:11" x14ac:dyDescent="0.25">
+        <f t="array" ref="J7">INDEX(STKWp!$K$11:$K$30,IFERROR(MATCH(MIN(IF(STKWp!$D$11:$D$30&gt;AVERAGE(B7,C7),STKWp!$D$11:$D$30)),STKWp!$D$11:$D$30),1))</f>
+        <v>+III</v>
+      </c>
+      <c r="K7" s="9" t="str">
+        <f t="array" ref="K7">INDEX(BSKW!$K$11:$K$30,IFERROR(MATCH(MIN(IF(BSKW!$D$11:$D$30&gt;AVERAGE(B7,C7),BSKW!$D$11:$D$30)),BSKW!$D$11:$D$30),1))</f>
+        <v>+III</v>
+      </c>
+      <c r="L7" s="12" t="str">
+        <f t="array" ref="L7">INDEX(HTKW!$K$11:$K$30,IFERROR(MATCH(MIN(IF(HTKW!$D$11:$D$30&gt;AVERAGE(B7,C7),HTKW!$D$11:$D$30)),HTKW!$D$11:$D$30),1))</f>
+        <v>+III</v>
+      </c>
+    </row>
+    <row r="8" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B8" s="8">
         <v>1.0509999999999999</v>
       </c>
@@ -2732,36 +2759,40 @@
         <f t="shared" si="0"/>
         <v>+0</v>
       </c>
-      <c r="E8" s="9" t="str">
-        <f t="array" ref="E8">INDEX(STPH!$O$11:$O$30,IFERROR(MATCH(MIN(IF(STPH!$D$11:$D$30&gt;AVERAGE(B8,C8),STPH!$D$11:$D$30)),STPH!$D$11:$D$30),1))</f>
-        <v>+III</v>
+      <c r="E8" s="23" t="str">
+        <f t="shared" si="1"/>
+        <v>+0</v>
       </c>
       <c r="F8" s="9" t="str">
-        <f t="array" ref="F8">INDEX(STBI!$O$11:$O$30,IFERROR(MATCH(MIN(IF(STBI!$D$11:$D$30&gt;AVERAGE(B8,C8),STBI!$D$11:$D$30)),STBI!$D$11:$D$30),1))</f>
+        <f t="array" ref="F8">INDEX(STPH!$O$11:$O$30,IFERROR(MATCH(MIN(IF(STPH!$D$11:$D$30&gt;AVERAGE(B8,C8),STPH!$D$11:$D$30)),STPH!$D$11:$D$30),1))</f>
         <v>+III</v>
       </c>
       <c r="G8" s="9" t="str">
-        <f t="array" ref="G8">INDEX(GEKB!$K$11:$K$30,IFERROR(MATCH(MIN(IF(GEKB!$D$11:$D$30&gt;AVERAGE(B8,C8),GEKB!$D$11:$D$30)),GEKB!$D$11:$D$30),1))</f>
-        <v>+III</v>
-      </c>
-      <c r="H8" s="9">
-        <f t="array" ref="H8">INDEX(DA!$K$50:$K$71,IFERROR(MATCH(MIN(IF(DA!$D$50:$D$71&gt;AVERAGE(B8,C8),DA!$D$50:$D$71)),DA!$D$50:$D$71),1))</f>
-        <v>0</v>
-      </c>
-      <c r="I8" s="9" t="str">
-        <f t="array" ref="I8">INDEX(STKWp!$K$11:$K$30,IFERROR(MATCH(MIN(IF(STKWp!$D$11:$D$30&gt;AVERAGE(B8,C8),STKWp!$D$11:$D$30)),STKWp!$D$11:$D$30),1))</f>
-        <v>+III</v>
+        <f t="array" ref="G8">INDEX(STBI!$O$11:$O$30,IFERROR(MATCH(MIN(IF(STBI!$D$11:$D$30&gt;AVERAGE(B8,C8),STBI!$D$11:$D$30)),STBI!$D$11:$D$30),1))</f>
+        <v>+III</v>
+      </c>
+      <c r="H8" s="9" t="str">
+        <f t="array" ref="H8">INDEX(GEKB!$K$11:$K$30,IFERROR(MATCH(MIN(IF(GEKB!$D$11:$D$30&gt;AVERAGE(B8,C8),GEKB!$D$11:$D$30)),GEKB!$D$11:$D$30),1))</f>
+        <v>+III</v>
+      </c>
+      <c r="I8" s="9">
+        <f t="array" ref="I8">INDEX(DA!$K$50:$K$71,IFERROR(MATCH(MIN(IF(DA!$D$50:$D$71&gt;AVERAGE(B8,C8),DA!$D$50:$D$71)),DA!$D$50:$D$71),1))</f>
+        <v>0</v>
       </c>
       <c r="J8" s="9" t="str">
-        <f t="array" ref="J8">INDEX(BSKW!$K$11:$K$30,IFERROR(MATCH(MIN(IF(BSKW!$D$11:$D$30&gt;AVERAGE(B8,C8),BSKW!$D$11:$D$30)),BSKW!$D$11:$D$30),1))</f>
-        <v>+III</v>
-      </c>
-      <c r="K8" s="12" t="str">
-        <f t="array" ref="K8">INDEX(HTKW!$K$11:$K$30,IFERROR(MATCH(MIN(IF(HTKW!$D$11:$D$30&gt;AVERAGE(B8,C8),HTKW!$D$11:$D$30)),HTKW!$D$11:$D$30),1))</f>
-        <v>+III</v>
-      </c>
-    </row>
-    <row r="9" spans="2:11" x14ac:dyDescent="0.25">
+        <f t="array" ref="J8">INDEX(STKWp!$K$11:$K$30,IFERROR(MATCH(MIN(IF(STKWp!$D$11:$D$30&gt;AVERAGE(B8,C8),STKWp!$D$11:$D$30)),STKWp!$D$11:$D$30),1))</f>
+        <v>+III</v>
+      </c>
+      <c r="K8" s="9" t="str">
+        <f t="array" ref="K8">INDEX(BSKW!$K$11:$K$30,IFERROR(MATCH(MIN(IF(BSKW!$D$11:$D$30&gt;AVERAGE(B8,C8),BSKW!$D$11:$D$30)),BSKW!$D$11:$D$30),1))</f>
+        <v>+III</v>
+      </c>
+      <c r="L8" s="12" t="str">
+        <f t="array" ref="L8">INDEX(HTKW!$K$11:$K$30,IFERROR(MATCH(MIN(IF(HTKW!$D$11:$D$30&gt;AVERAGE(B8,C8),HTKW!$D$11:$D$30)),HTKW!$D$11:$D$30),1))</f>
+        <v>+III</v>
+      </c>
+    </row>
+    <row r="9" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B9" s="8">
         <v>1.214</v>
       </c>
@@ -2772,36 +2803,40 @@
         <f t="shared" si="0"/>
         <v>+0</v>
       </c>
-      <c r="E9" s="9" t="str">
-        <f t="array" ref="E9">INDEX(STPH!$O$11:$O$30,IFERROR(MATCH(MIN(IF(STPH!$D$11:$D$30&gt;AVERAGE(B9,C9),STPH!$D$11:$D$30)),STPH!$D$11:$D$30),1))</f>
-        <v>+III</v>
+      <c r="E9" s="23" t="str">
+        <f t="shared" si="1"/>
+        <v>+0</v>
       </c>
       <c r="F9" s="9" t="str">
-        <f t="array" ref="F9">INDEX(STBI!$O$11:$O$30,IFERROR(MATCH(MIN(IF(STBI!$D$11:$D$30&gt;AVERAGE(B9,C9),STBI!$D$11:$D$30)),STBI!$D$11:$D$30),1))</f>
+        <f t="array" ref="F9">INDEX(STPH!$O$11:$O$30,IFERROR(MATCH(MIN(IF(STPH!$D$11:$D$30&gt;AVERAGE(B9,C9),STPH!$D$11:$D$30)),STPH!$D$11:$D$30),1))</f>
         <v>+III</v>
       </c>
       <c r="G9" s="9" t="str">
-        <f t="array" ref="G9">INDEX(GEKB!$K$11:$K$30,IFERROR(MATCH(MIN(IF(GEKB!$D$11:$D$30&gt;AVERAGE(B9,C9),GEKB!$D$11:$D$30)),GEKB!$D$11:$D$30),1))</f>
-        <v>+III</v>
-      </c>
-      <c r="H9" s="9">
-        <f t="array" ref="H9">INDEX(DA!$K$50:$K$71,IFERROR(MATCH(MIN(IF(DA!$D$50:$D$71&gt;AVERAGE(B9,C9),DA!$D$50:$D$71)),DA!$D$50:$D$71),1))</f>
-        <v>0</v>
-      </c>
-      <c r="I9" s="9" t="str">
-        <f t="array" ref="I9">INDEX(STKWp!$K$11:$K$30,IFERROR(MATCH(MIN(IF(STKWp!$D$11:$D$30&gt;AVERAGE(B9,C9),STKWp!$D$11:$D$30)),STKWp!$D$11:$D$30),1))</f>
-        <v>+III</v>
+        <f t="array" ref="G9">INDEX(STBI!$O$11:$O$30,IFERROR(MATCH(MIN(IF(STBI!$D$11:$D$30&gt;AVERAGE(B9,C9),STBI!$D$11:$D$30)),STBI!$D$11:$D$30),1))</f>
+        <v>+III</v>
+      </c>
+      <c r="H9" s="9" t="str">
+        <f t="array" ref="H9">INDEX(GEKB!$K$11:$K$30,IFERROR(MATCH(MIN(IF(GEKB!$D$11:$D$30&gt;AVERAGE(B9,C9),GEKB!$D$11:$D$30)),GEKB!$D$11:$D$30),1))</f>
+        <v>+III</v>
+      </c>
+      <c r="I9" s="9">
+        <f t="array" ref="I9">INDEX(DA!$K$50:$K$71,IFERROR(MATCH(MIN(IF(DA!$D$50:$D$71&gt;AVERAGE(B9,C9),DA!$D$50:$D$71)),DA!$D$50:$D$71),1))</f>
+        <v>0</v>
       </c>
       <c r="J9" s="9" t="str">
-        <f t="array" ref="J9">INDEX(BSKW!$K$11:$K$30,IFERROR(MATCH(MIN(IF(BSKW!$D$11:$D$30&gt;AVERAGE(B9,C9),BSKW!$D$11:$D$30)),BSKW!$D$11:$D$30),1))</f>
-        <v>+III</v>
-      </c>
-      <c r="K9" s="12" t="str">
-        <f t="array" ref="K9">INDEX(HTKW!$K$11:$K$30,IFERROR(MATCH(MIN(IF(HTKW!$D$11:$D$30&gt;AVERAGE(B9,C9),HTKW!$D$11:$D$30)),HTKW!$D$11:$D$30),1))</f>
-        <v>+III</v>
-      </c>
-    </row>
-    <row r="10" spans="2:11" x14ac:dyDescent="0.25">
+        <f t="array" ref="J9">INDEX(STKWp!$K$11:$K$30,IFERROR(MATCH(MIN(IF(STKWp!$D$11:$D$30&gt;AVERAGE(B9,C9),STKWp!$D$11:$D$30)),STKWp!$D$11:$D$30),1))</f>
+        <v>+III</v>
+      </c>
+      <c r="K9" s="9" t="str">
+        <f t="array" ref="K9">INDEX(BSKW!$K$11:$K$30,IFERROR(MATCH(MIN(IF(BSKW!$D$11:$D$30&gt;AVERAGE(B9,C9),BSKW!$D$11:$D$30)),BSKW!$D$11:$D$30),1))</f>
+        <v>+III</v>
+      </c>
+      <c r="L9" s="12" t="str">
+        <f t="array" ref="L9">INDEX(HTKW!$K$11:$K$30,IFERROR(MATCH(MIN(IF(HTKW!$D$11:$D$30&gt;AVERAGE(B9,C9),HTKW!$D$11:$D$30)),HTKW!$D$11:$D$30),1))</f>
+        <v>+III</v>
+      </c>
+    </row>
+    <row r="10" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B10" s="8">
         <v>1.383</v>
       </c>
@@ -2812,36 +2847,40 @@
         <f t="shared" si="0"/>
         <v>+0</v>
       </c>
-      <c r="E10" s="9" t="str">
-        <f t="array" ref="E10">INDEX(STPH!$O$11:$O$30,IFERROR(MATCH(MIN(IF(STPH!$D$11:$D$30&gt;AVERAGE(B10,C10),STPH!$D$11:$D$30)),STPH!$D$11:$D$30),1))</f>
-        <v>+III</v>
+      <c r="E10" s="23" t="str">
+        <f t="shared" si="1"/>
+        <v>+0</v>
       </c>
       <c r="F10" s="9" t="str">
-        <f t="array" ref="F10">INDEX(STBI!$O$11:$O$30,IFERROR(MATCH(MIN(IF(STBI!$D$11:$D$30&gt;AVERAGE(B10,C10),STBI!$D$11:$D$30)),STBI!$D$11:$D$30),1))</f>
+        <f t="array" ref="F10">INDEX(STPH!$O$11:$O$30,IFERROR(MATCH(MIN(IF(STPH!$D$11:$D$30&gt;AVERAGE(B10,C10),STPH!$D$11:$D$30)),STPH!$D$11:$D$30),1))</f>
         <v>+III</v>
       </c>
       <c r="G10" s="9" t="str">
-        <f t="array" ref="G10">INDEX(GEKB!$K$11:$K$30,IFERROR(MATCH(MIN(IF(GEKB!$D$11:$D$30&gt;AVERAGE(B10,C10),GEKB!$D$11:$D$30)),GEKB!$D$11:$D$30),1))</f>
-        <v>+III</v>
-      </c>
-      <c r="H10" s="9">
-        <f t="array" ref="H10">INDEX(DA!$K$50:$K$71,IFERROR(MATCH(MIN(IF(DA!$D$50:$D$71&gt;AVERAGE(B10,C10),DA!$D$50:$D$71)),DA!$D$50:$D$71),1))</f>
-        <v>0</v>
-      </c>
-      <c r="I10" s="9" t="str">
-        <f t="array" ref="I10">INDEX(STKWp!$K$11:$K$30,IFERROR(MATCH(MIN(IF(STKWp!$D$11:$D$30&gt;AVERAGE(B10,C10),STKWp!$D$11:$D$30)),STKWp!$D$11:$D$30),1))</f>
-        <v>+III</v>
+        <f t="array" ref="G10">INDEX(STBI!$O$11:$O$30,IFERROR(MATCH(MIN(IF(STBI!$D$11:$D$30&gt;AVERAGE(B10,C10),STBI!$D$11:$D$30)),STBI!$D$11:$D$30),1))</f>
+        <v>+III</v>
+      </c>
+      <c r="H10" s="9" t="str">
+        <f t="array" ref="H10">INDEX(GEKB!$K$11:$K$30,IFERROR(MATCH(MIN(IF(GEKB!$D$11:$D$30&gt;AVERAGE(B10,C10),GEKB!$D$11:$D$30)),GEKB!$D$11:$D$30),1))</f>
+        <v>+III</v>
+      </c>
+      <c r="I10" s="9">
+        <f t="array" ref="I10">INDEX(DA!$K$50:$K$71,IFERROR(MATCH(MIN(IF(DA!$D$50:$D$71&gt;AVERAGE(B10,C10),DA!$D$50:$D$71)),DA!$D$50:$D$71),1))</f>
+        <v>0</v>
       </c>
       <c r="J10" s="9" t="str">
-        <f t="array" ref="J10">INDEX(BSKW!$K$11:$K$30,IFERROR(MATCH(MIN(IF(BSKW!$D$11:$D$30&gt;AVERAGE(B10,C10),BSKW!$D$11:$D$30)),BSKW!$D$11:$D$30),1))</f>
-        <v>+III</v>
-      </c>
-      <c r="K10" s="12" t="str">
-        <f t="array" ref="K10">INDEX(HTKW!$K$11:$K$30,IFERROR(MATCH(MIN(IF(HTKW!$D$11:$D$30&gt;AVERAGE(B10,C10),HTKW!$D$11:$D$30)),HTKW!$D$11:$D$30),1))</f>
-        <v>+III</v>
-      </c>
-    </row>
-    <row r="11" spans="2:11" x14ac:dyDescent="0.25">
+        <f t="array" ref="J10">INDEX(STKWp!$K$11:$K$30,IFERROR(MATCH(MIN(IF(STKWp!$D$11:$D$30&gt;AVERAGE(B10,C10),STKWp!$D$11:$D$30)),STKWp!$D$11:$D$30),1))</f>
+        <v>+III</v>
+      </c>
+      <c r="K10" s="9" t="str">
+        <f t="array" ref="K10">INDEX(BSKW!$K$11:$K$30,IFERROR(MATCH(MIN(IF(BSKW!$D$11:$D$30&gt;AVERAGE(B10,C10),BSKW!$D$11:$D$30)),BSKW!$D$11:$D$30),1))</f>
+        <v>+III</v>
+      </c>
+      <c r="L10" s="12" t="str">
+        <f t="array" ref="L10">INDEX(HTKW!$K$11:$K$30,IFERROR(MATCH(MIN(IF(HTKW!$D$11:$D$30&gt;AVERAGE(B10,C10),HTKW!$D$11:$D$30)),HTKW!$D$11:$D$30),1))</f>
+        <v>+III</v>
+      </c>
+    </row>
+    <row r="11" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B11" s="8">
         <v>1.5289999999999999</v>
       </c>
@@ -2852,36 +2891,40 @@
         <f t="shared" si="0"/>
         <v>+0</v>
       </c>
-      <c r="E11" s="9" t="str">
-        <f t="array" ref="E11">INDEX(STPH!$O$11:$O$30,IFERROR(MATCH(MIN(IF(STPH!$D$11:$D$30&gt;AVERAGE(B11,C11),STPH!$D$11:$D$30)),STPH!$D$11:$D$30),1))</f>
-        <v>+III</v>
+      <c r="E11" s="23" t="str">
+        <f t="shared" si="1"/>
+        <v>+0</v>
       </c>
       <c r="F11" s="9" t="str">
-        <f t="array" ref="F11">INDEX(STBI!$O$11:$O$30,IFERROR(MATCH(MIN(IF(STBI!$D$11:$D$30&gt;AVERAGE(B11,C11),STBI!$D$11:$D$30)),STBI!$D$11:$D$30),1))</f>
+        <f t="array" ref="F11">INDEX(STPH!$O$11:$O$30,IFERROR(MATCH(MIN(IF(STPH!$D$11:$D$30&gt;AVERAGE(B11,C11),STPH!$D$11:$D$30)),STPH!$D$11:$D$30),1))</f>
         <v>+III</v>
       </c>
       <c r="G11" s="9" t="str">
-        <f t="array" ref="G11">INDEX(GEKB!$K$11:$K$30,IFERROR(MATCH(MIN(IF(GEKB!$D$11:$D$30&gt;AVERAGE(B11,C11),GEKB!$D$11:$D$30)),GEKB!$D$11:$D$30),1))</f>
-        <v>+III</v>
-      </c>
-      <c r="H11" s="9">
-        <f t="array" ref="H11">INDEX(DA!$K$50:$K$71,IFERROR(MATCH(MIN(IF(DA!$D$50:$D$71&gt;AVERAGE(B11,C11),DA!$D$50:$D$71)),DA!$D$50:$D$71),1))</f>
-        <v>0</v>
-      </c>
-      <c r="I11" s="9" t="str">
-        <f t="array" ref="I11">INDEX(STKWp!$K$11:$K$30,IFERROR(MATCH(MIN(IF(STKWp!$D$11:$D$30&gt;AVERAGE(B11,C11),STKWp!$D$11:$D$30)),STKWp!$D$11:$D$30),1))</f>
-        <v>+III</v>
+        <f t="array" ref="G11">INDEX(STBI!$O$11:$O$30,IFERROR(MATCH(MIN(IF(STBI!$D$11:$D$30&gt;AVERAGE(B11,C11),STBI!$D$11:$D$30)),STBI!$D$11:$D$30),1))</f>
+        <v>+III</v>
+      </c>
+      <c r="H11" s="9" t="str">
+        <f t="array" ref="H11">INDEX(GEKB!$K$11:$K$30,IFERROR(MATCH(MIN(IF(GEKB!$D$11:$D$30&gt;AVERAGE(B11,C11),GEKB!$D$11:$D$30)),GEKB!$D$11:$D$30),1))</f>
+        <v>+III</v>
+      </c>
+      <c r="I11" s="9">
+        <f t="array" ref="I11">INDEX(DA!$K$50:$K$71,IFERROR(MATCH(MIN(IF(DA!$D$50:$D$71&gt;AVERAGE(B11,C11),DA!$D$50:$D$71)),DA!$D$50:$D$71),1))</f>
+        <v>0</v>
       </c>
       <c r="J11" s="9" t="str">
-        <f t="array" ref="J11">INDEX(BSKW!$K$11:$K$30,IFERROR(MATCH(MIN(IF(BSKW!$D$11:$D$30&gt;AVERAGE(B11,C11),BSKW!$D$11:$D$30)),BSKW!$D$11:$D$30),1))</f>
-        <v>+III</v>
-      </c>
-      <c r="K11" s="12" t="str">
-        <f t="array" ref="K11">INDEX(HTKW!$K$11:$K$30,IFERROR(MATCH(MIN(IF(HTKW!$D$11:$D$30&gt;AVERAGE(B11,C11),HTKW!$D$11:$D$30)),HTKW!$D$11:$D$30),1))</f>
-        <v>+III</v>
-      </c>
-    </row>
-    <row r="12" spans="2:11" x14ac:dyDescent="0.25">
+        <f t="array" ref="J11">INDEX(STKWp!$K$11:$K$30,IFERROR(MATCH(MIN(IF(STKWp!$D$11:$D$30&gt;AVERAGE(B11,C11),STKWp!$D$11:$D$30)),STKWp!$D$11:$D$30),1))</f>
+        <v>+III</v>
+      </c>
+      <c r="K11" s="9" t="str">
+        <f t="array" ref="K11">INDEX(BSKW!$K$11:$K$30,IFERROR(MATCH(MIN(IF(BSKW!$D$11:$D$30&gt;AVERAGE(B11,C11),BSKW!$D$11:$D$30)),BSKW!$D$11:$D$30),1))</f>
+        <v>+III</v>
+      </c>
+      <c r="L11" s="12" t="str">
+        <f t="array" ref="L11">INDEX(HTKW!$K$11:$K$30,IFERROR(MATCH(MIN(IF(HTKW!$D$11:$D$30&gt;AVERAGE(B11,C11),HTKW!$D$11:$D$30)),HTKW!$D$11:$D$30),1))</f>
+        <v>+III</v>
+      </c>
+    </row>
+    <row r="12" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B12" s="8">
         <v>1.661</v>
       </c>
@@ -2892,36 +2935,40 @@
         <f t="shared" si="0"/>
         <v>+0</v>
       </c>
-      <c r="E12" s="9" t="str">
-        <f t="array" ref="E12">INDEX(STPH!$O$11:$O$30,IFERROR(MATCH(MIN(IF(STPH!$D$11:$D$30&gt;AVERAGE(B12,C12),STPH!$D$11:$D$30)),STPH!$D$11:$D$30),1))</f>
-        <v>+III</v>
+      <c r="E12" s="23" t="str">
+        <f t="shared" si="1"/>
+        <v>+0</v>
       </c>
       <c r="F12" s="9" t="str">
-        <f t="array" ref="F12">INDEX(STBI!$O$11:$O$30,IFERROR(MATCH(MIN(IF(STBI!$D$11:$D$30&gt;AVERAGE(B12,C12),STBI!$D$11:$D$30)),STBI!$D$11:$D$30),1))</f>
+        <f t="array" ref="F12">INDEX(STPH!$O$11:$O$30,IFERROR(MATCH(MIN(IF(STPH!$D$11:$D$30&gt;AVERAGE(B12,C12),STPH!$D$11:$D$30)),STPH!$D$11:$D$30),1))</f>
         <v>+III</v>
       </c>
       <c r="G12" s="9" t="str">
-        <f t="array" ref="G12">INDEX(GEKB!$K$11:$K$30,IFERROR(MATCH(MIN(IF(GEKB!$D$11:$D$30&gt;AVERAGE(B12,C12),GEKB!$D$11:$D$30)),GEKB!$D$11:$D$30),1))</f>
-        <v>+III</v>
-      </c>
-      <c r="H12" s="9">
-        <f t="array" ref="H12">INDEX(DA!$K$50:$K$71,IFERROR(MATCH(MIN(IF(DA!$D$50:$D$71&gt;AVERAGE(B12,C12),DA!$D$50:$D$71)),DA!$D$50:$D$71),1))</f>
-        <v>0</v>
-      </c>
-      <c r="I12" s="9" t="str">
-        <f t="array" ref="I12">INDEX(STKWp!$K$11:$K$30,IFERROR(MATCH(MIN(IF(STKWp!$D$11:$D$30&gt;AVERAGE(B12,C12),STKWp!$D$11:$D$30)),STKWp!$D$11:$D$30),1))</f>
-        <v>+III</v>
+        <f t="array" ref="G12">INDEX(STBI!$O$11:$O$30,IFERROR(MATCH(MIN(IF(STBI!$D$11:$D$30&gt;AVERAGE(B12,C12),STBI!$D$11:$D$30)),STBI!$D$11:$D$30),1))</f>
+        <v>+III</v>
+      </c>
+      <c r="H12" s="9" t="str">
+        <f t="array" ref="H12">INDEX(GEKB!$K$11:$K$30,IFERROR(MATCH(MIN(IF(GEKB!$D$11:$D$30&gt;AVERAGE(B12,C12),GEKB!$D$11:$D$30)),GEKB!$D$11:$D$30),1))</f>
+        <v>+III</v>
+      </c>
+      <c r="I12" s="9">
+        <f t="array" ref="I12">INDEX(DA!$K$50:$K$71,IFERROR(MATCH(MIN(IF(DA!$D$50:$D$71&gt;AVERAGE(B12,C12),DA!$D$50:$D$71)),DA!$D$50:$D$71),1))</f>
+        <v>0</v>
       </c>
       <c r="J12" s="9" t="str">
-        <f t="array" ref="J12">INDEX(BSKW!$K$11:$K$30,IFERROR(MATCH(MIN(IF(BSKW!$D$11:$D$30&gt;AVERAGE(B12,C12),BSKW!$D$11:$D$30)),BSKW!$D$11:$D$30),1))</f>
-        <v>+III</v>
-      </c>
-      <c r="K12" s="12" t="str">
-        <f t="array" ref="K12">INDEX(HTKW!$K$11:$K$30,IFERROR(MATCH(MIN(IF(HTKW!$D$11:$D$30&gt;AVERAGE(B12,C12),HTKW!$D$11:$D$30)),HTKW!$D$11:$D$30),1))</f>
-        <v>+III</v>
-      </c>
-    </row>
-    <row r="13" spans="2:11" x14ac:dyDescent="0.25">
+        <f t="array" ref="J12">INDEX(STKWp!$K$11:$K$30,IFERROR(MATCH(MIN(IF(STKWp!$D$11:$D$30&gt;AVERAGE(B12,C12),STKWp!$D$11:$D$30)),STKWp!$D$11:$D$30),1))</f>
+        <v>+III</v>
+      </c>
+      <c r="K12" s="9" t="str">
+        <f t="array" ref="K12">INDEX(BSKW!$K$11:$K$30,IFERROR(MATCH(MIN(IF(BSKW!$D$11:$D$30&gt;AVERAGE(B12,C12),BSKW!$D$11:$D$30)),BSKW!$D$11:$D$30),1))</f>
+        <v>+III</v>
+      </c>
+      <c r="L12" s="12" t="str">
+        <f t="array" ref="L12">INDEX(HTKW!$K$11:$K$30,IFERROR(MATCH(MIN(IF(HTKW!$D$11:$D$30&gt;AVERAGE(B12,C12),HTKW!$D$11:$D$30)),HTKW!$D$11:$D$30),1))</f>
+        <v>+III</v>
+      </c>
+    </row>
+    <row r="13" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B13" s="8">
         <v>1.79</v>
       </c>
@@ -2932,36 +2979,40 @@
         <f t="shared" si="0"/>
         <v>+0</v>
       </c>
-      <c r="E13" s="9" t="str">
-        <f t="array" ref="E13">INDEX(STPH!$O$11:$O$30,IFERROR(MATCH(MIN(IF(STPH!$D$11:$D$30&gt;AVERAGE(B13,C13),STPH!$D$11:$D$30)),STPH!$D$11:$D$30),1))</f>
-        <v>+III</v>
+      <c r="E13" s="23" t="str">
+        <f t="shared" si="1"/>
+        <v>+0</v>
       </c>
       <c r="F13" s="9" t="str">
-        <f t="array" ref="F13">INDEX(STBI!$O$11:$O$30,IFERROR(MATCH(MIN(IF(STBI!$D$11:$D$30&gt;AVERAGE(B13,C13),STBI!$D$11:$D$30)),STBI!$D$11:$D$30),1))</f>
+        <f t="array" ref="F13">INDEX(STPH!$O$11:$O$30,IFERROR(MATCH(MIN(IF(STPH!$D$11:$D$30&gt;AVERAGE(B13,C13),STPH!$D$11:$D$30)),STPH!$D$11:$D$30),1))</f>
         <v>+III</v>
       </c>
       <c r="G13" s="9" t="str">
-        <f t="array" ref="G13">INDEX(GEKB!$K$11:$K$30,IFERROR(MATCH(MIN(IF(GEKB!$D$11:$D$30&gt;AVERAGE(B13,C13),GEKB!$D$11:$D$30)),GEKB!$D$11:$D$30),1))</f>
-        <v>+III</v>
-      </c>
-      <c r="H13" s="9">
-        <f t="array" ref="H13">INDEX(DA!$K$50:$K$71,IFERROR(MATCH(MIN(IF(DA!$D$50:$D$71&gt;AVERAGE(B13,C13),DA!$D$50:$D$71)),DA!$D$50:$D$71),1))</f>
-        <v>0</v>
-      </c>
-      <c r="I13" s="9" t="str">
-        <f t="array" ref="I13">INDEX(STKWp!$K$11:$K$30,IFERROR(MATCH(MIN(IF(STKWp!$D$11:$D$30&gt;AVERAGE(B13,C13),STKWp!$D$11:$D$30)),STKWp!$D$11:$D$30),1))</f>
-        <v>+III</v>
+        <f t="array" ref="G13">INDEX(STBI!$O$11:$O$30,IFERROR(MATCH(MIN(IF(STBI!$D$11:$D$30&gt;AVERAGE(B13,C13),STBI!$D$11:$D$30)),STBI!$D$11:$D$30),1))</f>
+        <v>+III</v>
+      </c>
+      <c r="H13" s="9" t="str">
+        <f t="array" ref="H13">INDEX(GEKB!$K$11:$K$30,IFERROR(MATCH(MIN(IF(GEKB!$D$11:$D$30&gt;AVERAGE(B13,C13),GEKB!$D$11:$D$30)),GEKB!$D$11:$D$30),1))</f>
+        <v>+III</v>
+      </c>
+      <c r="I13" s="9">
+        <f t="array" ref="I13">INDEX(DA!$K$50:$K$71,IFERROR(MATCH(MIN(IF(DA!$D$50:$D$71&gt;AVERAGE(B13,C13),DA!$D$50:$D$71)),DA!$D$50:$D$71),1))</f>
+        <v>0</v>
       </c>
       <c r="J13" s="9" t="str">
-        <f t="array" ref="J13">INDEX(BSKW!$K$11:$K$30,IFERROR(MATCH(MIN(IF(BSKW!$D$11:$D$30&gt;AVERAGE(B13,C13),BSKW!$D$11:$D$30)),BSKW!$D$11:$D$30),1))</f>
-        <v>+III</v>
-      </c>
-      <c r="K13" s="12" t="str">
-        <f t="array" ref="K13">INDEX(HTKW!$K$11:$K$30,IFERROR(MATCH(MIN(IF(HTKW!$D$11:$D$30&gt;AVERAGE(B13,C13),HTKW!$D$11:$D$30)),HTKW!$D$11:$D$30),1))</f>
-        <v>+III</v>
-      </c>
-    </row>
-    <row r="14" spans="2:11" x14ac:dyDescent="0.25">
+        <f t="array" ref="J13">INDEX(STKWp!$K$11:$K$30,IFERROR(MATCH(MIN(IF(STKWp!$D$11:$D$30&gt;AVERAGE(B13,C13),STKWp!$D$11:$D$30)),STKWp!$D$11:$D$30),1))</f>
+        <v>+III</v>
+      </c>
+      <c r="K13" s="9" t="str">
+        <f t="array" ref="K13">INDEX(BSKW!$K$11:$K$30,IFERROR(MATCH(MIN(IF(BSKW!$D$11:$D$30&gt;AVERAGE(B13,C13),BSKW!$D$11:$D$30)),BSKW!$D$11:$D$30),1))</f>
+        <v>+III</v>
+      </c>
+      <c r="L13" s="12" t="str">
+        <f t="array" ref="L13">INDEX(HTKW!$K$11:$K$30,IFERROR(MATCH(MIN(IF(HTKW!$D$11:$D$30&gt;AVERAGE(B13,C13),HTKW!$D$11:$D$30)),HTKW!$D$11:$D$30),1))</f>
+        <v>+III</v>
+      </c>
+    </row>
+    <row r="14" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B14" s="8">
         <v>1.929</v>
       </c>
@@ -2972,36 +3023,40 @@
         <f t="shared" si="0"/>
         <v>+0</v>
       </c>
-      <c r="E14" s="9" t="str">
-        <f t="array" ref="E14">INDEX(STPH!$O$11:$O$30,IFERROR(MATCH(MIN(IF(STPH!$D$11:$D$30&gt;AVERAGE(B14,C14),STPH!$D$11:$D$30)),STPH!$D$11:$D$30),1))</f>
-        <v>+III</v>
+      <c r="E14" s="23" t="str">
+        <f t="shared" si="1"/>
+        <v>+0</v>
       </c>
       <c r="F14" s="9" t="str">
-        <f t="array" ref="F14">INDEX(STBI!$O$11:$O$30,IFERROR(MATCH(MIN(IF(STBI!$D$11:$D$30&gt;AVERAGE(B14,C14),STBI!$D$11:$D$30)),STBI!$D$11:$D$30),1))</f>
+        <f t="array" ref="F14">INDEX(STPH!$O$11:$O$30,IFERROR(MATCH(MIN(IF(STPH!$D$11:$D$30&gt;AVERAGE(B14,C14),STPH!$D$11:$D$30)),STPH!$D$11:$D$30),1))</f>
         <v>+III</v>
       </c>
       <c r="G14" s="9" t="str">
-        <f t="array" ref="G14">INDEX(GEKB!$K$11:$K$30,IFERROR(MATCH(MIN(IF(GEKB!$D$11:$D$30&gt;AVERAGE(B14,C14),GEKB!$D$11:$D$30)),GEKB!$D$11:$D$30),1))</f>
-        <v>+III</v>
-      </c>
-      <c r="H14" s="9">
-        <f t="array" ref="H14">INDEX(DA!$K$50:$K$71,IFERROR(MATCH(MIN(IF(DA!$D$50:$D$71&gt;AVERAGE(B14,C14),DA!$D$50:$D$71)),DA!$D$50:$D$71),1))</f>
-        <v>0</v>
-      </c>
-      <c r="I14" s="9" t="str">
-        <f t="array" ref="I14">INDEX(STKWp!$K$11:$K$30,IFERROR(MATCH(MIN(IF(STKWp!$D$11:$D$30&gt;AVERAGE(B14,C14),STKWp!$D$11:$D$30)),STKWp!$D$11:$D$30),1))</f>
-        <v>+III</v>
+        <f t="array" ref="G14">INDEX(STBI!$O$11:$O$30,IFERROR(MATCH(MIN(IF(STBI!$D$11:$D$30&gt;AVERAGE(B14,C14),STBI!$D$11:$D$30)),STBI!$D$11:$D$30),1))</f>
+        <v>+III</v>
+      </c>
+      <c r="H14" s="9" t="str">
+        <f t="array" ref="H14">INDEX(GEKB!$K$11:$K$30,IFERROR(MATCH(MIN(IF(GEKB!$D$11:$D$30&gt;AVERAGE(B14,C14),GEKB!$D$11:$D$30)),GEKB!$D$11:$D$30),1))</f>
+        <v>+III</v>
+      </c>
+      <c r="I14" s="9">
+        <f t="array" ref="I14">INDEX(DA!$K$50:$K$71,IFERROR(MATCH(MIN(IF(DA!$D$50:$D$71&gt;AVERAGE(B14,C14),DA!$D$50:$D$71)),DA!$D$50:$D$71),1))</f>
+        <v>0</v>
       </c>
       <c r="J14" s="9" t="str">
-        <f t="array" ref="J14">INDEX(BSKW!$K$11:$K$30,IFERROR(MATCH(MIN(IF(BSKW!$D$11:$D$30&gt;AVERAGE(B14,C14),BSKW!$D$11:$D$30)),BSKW!$D$11:$D$30),1))</f>
-        <v>+III</v>
-      </c>
-      <c r="K14" s="12" t="str">
-        <f t="array" ref="K14">INDEX(HTKW!$K$11:$K$30,IFERROR(MATCH(MIN(IF(HTKW!$D$11:$D$30&gt;AVERAGE(B14,C14),HTKW!$D$11:$D$30)),HTKW!$D$11:$D$30),1))</f>
-        <v>+III</v>
-      </c>
-    </row>
-    <row r="15" spans="2:11" x14ac:dyDescent="0.25">
+        <f t="array" ref="J14">INDEX(STKWp!$K$11:$K$30,IFERROR(MATCH(MIN(IF(STKWp!$D$11:$D$30&gt;AVERAGE(B14,C14),STKWp!$D$11:$D$30)),STKWp!$D$11:$D$30),1))</f>
+        <v>+III</v>
+      </c>
+      <c r="K14" s="9" t="str">
+        <f t="array" ref="K14">INDEX(BSKW!$K$11:$K$30,IFERROR(MATCH(MIN(IF(BSKW!$D$11:$D$30&gt;AVERAGE(B14,C14),BSKW!$D$11:$D$30)),BSKW!$D$11:$D$30),1))</f>
+        <v>+III</v>
+      </c>
+      <c r="L14" s="12" t="str">
+        <f t="array" ref="L14">INDEX(HTKW!$K$11:$K$30,IFERROR(MATCH(MIN(IF(HTKW!$D$11:$D$30&gt;AVERAGE(B14,C14),HTKW!$D$11:$D$30)),HTKW!$D$11:$D$30),1))</f>
+        <v>+III</v>
+      </c>
+    </row>
+    <row r="15" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B15" s="8">
         <v>2.0910000000000002</v>
       </c>
@@ -3012,36 +3067,40 @@
         <f t="shared" si="0"/>
         <v>+0</v>
       </c>
-      <c r="E15" s="9" t="str">
-        <f t="array" ref="E15">INDEX(STPH!$O$11:$O$30,IFERROR(MATCH(MIN(IF(STPH!$D$11:$D$30&gt;AVERAGE(B15,C15),STPH!$D$11:$D$30)),STPH!$D$11:$D$30),1))</f>
-        <v>+III</v>
+      <c r="E15" s="23" t="str">
+        <f t="shared" si="1"/>
+        <v>+0</v>
       </c>
       <c r="F15" s="9" t="str">
-        <f t="array" ref="F15">INDEX(STBI!$O$11:$O$30,IFERROR(MATCH(MIN(IF(STBI!$D$11:$D$30&gt;AVERAGE(B15,C15),STBI!$D$11:$D$30)),STBI!$D$11:$D$30),1))</f>
+        <f t="array" ref="F15">INDEX(STPH!$O$11:$O$30,IFERROR(MATCH(MIN(IF(STPH!$D$11:$D$30&gt;AVERAGE(B15,C15),STPH!$D$11:$D$30)),STPH!$D$11:$D$30),1))</f>
         <v>+III</v>
       </c>
       <c r="G15" s="9" t="str">
-        <f t="array" ref="G15">INDEX(GEKB!$K$11:$K$30,IFERROR(MATCH(MIN(IF(GEKB!$D$11:$D$30&gt;AVERAGE(B15,C15),GEKB!$D$11:$D$30)),GEKB!$D$11:$D$30),1))</f>
-        <v>+III</v>
-      </c>
-      <c r="H15" s="9">
-        <f t="array" ref="H15">INDEX(DA!$K$50:$K$71,IFERROR(MATCH(MIN(IF(DA!$D$50:$D$71&gt;AVERAGE(B15,C15),DA!$D$50:$D$71)),DA!$D$50:$D$71),1))</f>
-        <v>0</v>
-      </c>
-      <c r="I15" s="9" t="str">
-        <f t="array" ref="I15">INDEX(STKWp!$K$11:$K$30,IFERROR(MATCH(MIN(IF(STKWp!$D$11:$D$30&gt;AVERAGE(B15,C15),STKWp!$D$11:$D$30)),STKWp!$D$11:$D$30),1))</f>
-        <v>+III</v>
+        <f t="array" ref="G15">INDEX(STBI!$O$11:$O$30,IFERROR(MATCH(MIN(IF(STBI!$D$11:$D$30&gt;AVERAGE(B15,C15),STBI!$D$11:$D$30)),STBI!$D$11:$D$30),1))</f>
+        <v>+III</v>
+      </c>
+      <c r="H15" s="9" t="str">
+        <f t="array" ref="H15">INDEX(GEKB!$K$11:$K$30,IFERROR(MATCH(MIN(IF(GEKB!$D$11:$D$30&gt;AVERAGE(B15,C15),GEKB!$D$11:$D$30)),GEKB!$D$11:$D$30),1))</f>
+        <v>+III</v>
+      </c>
+      <c r="I15" s="9">
+        <f t="array" ref="I15">INDEX(DA!$K$50:$K$71,IFERROR(MATCH(MIN(IF(DA!$D$50:$D$71&gt;AVERAGE(B15,C15),DA!$D$50:$D$71)),DA!$D$50:$D$71),1))</f>
+        <v>0</v>
       </c>
       <c r="J15" s="9" t="str">
-        <f t="array" ref="J15">INDEX(BSKW!$K$11:$K$30,IFERROR(MATCH(MIN(IF(BSKW!$D$11:$D$30&gt;AVERAGE(B15,C15),BSKW!$D$11:$D$30)),BSKW!$D$11:$D$30),1))</f>
-        <v>+III</v>
-      </c>
-      <c r="K15" s="12" t="str">
-        <f t="array" ref="K15">INDEX(HTKW!$K$11:$K$30,IFERROR(MATCH(MIN(IF(HTKW!$D$11:$D$30&gt;AVERAGE(B15,C15),HTKW!$D$11:$D$30)),HTKW!$D$11:$D$30),1))</f>
-        <v>+III</v>
-      </c>
-    </row>
-    <row r="16" spans="2:11" x14ac:dyDescent="0.25">
+        <f t="array" ref="J15">INDEX(STKWp!$K$11:$K$30,IFERROR(MATCH(MIN(IF(STKWp!$D$11:$D$30&gt;AVERAGE(B15,C15),STKWp!$D$11:$D$30)),STKWp!$D$11:$D$30),1))</f>
+        <v>+III</v>
+      </c>
+      <c r="K15" s="9" t="str">
+        <f t="array" ref="K15">INDEX(BSKW!$K$11:$K$30,IFERROR(MATCH(MIN(IF(BSKW!$D$11:$D$30&gt;AVERAGE(B15,C15),BSKW!$D$11:$D$30)),BSKW!$D$11:$D$30),1))</f>
+        <v>+III</v>
+      </c>
+      <c r="L15" s="12" t="str">
+        <f t="array" ref="L15">INDEX(HTKW!$K$11:$K$30,IFERROR(MATCH(MIN(IF(HTKW!$D$11:$D$30&gt;AVERAGE(B15,C15),HTKW!$D$11:$D$30)),HTKW!$D$11:$D$30),1))</f>
+        <v>+III</v>
+      </c>
+    </row>
+    <row r="16" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B16" s="8">
         <v>2.254</v>
       </c>
@@ -3052,36 +3111,40 @@
         <f t="shared" si="0"/>
         <v>+0</v>
       </c>
-      <c r="E16" s="9" t="str">
-        <f t="array" ref="E16">INDEX(STPH!$O$11:$O$30,IFERROR(MATCH(MIN(IF(STPH!$D$11:$D$30&gt;AVERAGE(B16,C16),STPH!$D$11:$D$30)),STPH!$D$11:$D$30),1))</f>
-        <v>+III</v>
+      <c r="E16" s="23" t="str">
+        <f t="shared" si="1"/>
+        <v>+0</v>
       </c>
       <c r="F16" s="9" t="str">
-        <f t="array" ref="F16">INDEX(STBI!$O$11:$O$30,IFERROR(MATCH(MIN(IF(STBI!$D$11:$D$30&gt;AVERAGE(B16,C16),STBI!$D$11:$D$30)),STBI!$D$11:$D$30),1))</f>
+        <f t="array" ref="F16">INDEX(STPH!$O$11:$O$30,IFERROR(MATCH(MIN(IF(STPH!$D$11:$D$30&gt;AVERAGE(B16,C16),STPH!$D$11:$D$30)),STPH!$D$11:$D$30),1))</f>
         <v>+III</v>
       </c>
       <c r="G16" s="9" t="str">
-        <f t="array" ref="G16">INDEX(GEKB!$K$11:$K$30,IFERROR(MATCH(MIN(IF(GEKB!$D$11:$D$30&gt;AVERAGE(B16,C16),GEKB!$D$11:$D$30)),GEKB!$D$11:$D$30),1))</f>
-        <v>+III</v>
-      </c>
-      <c r="H16" s="9">
-        <f t="array" ref="H16">INDEX(DA!$K$50:$K$71,IFERROR(MATCH(MIN(IF(DA!$D$50:$D$71&gt;AVERAGE(B16,C16),DA!$D$50:$D$71)),DA!$D$50:$D$71),1))</f>
-        <v>0</v>
-      </c>
-      <c r="I16" s="9" t="str">
-        <f t="array" ref="I16">INDEX(STKWp!$K$11:$K$30,IFERROR(MATCH(MIN(IF(STKWp!$D$11:$D$30&gt;AVERAGE(B16,C16),STKWp!$D$11:$D$30)),STKWp!$D$11:$D$30),1))</f>
-        <v>+III</v>
+        <f t="array" ref="G16">INDEX(STBI!$O$11:$O$30,IFERROR(MATCH(MIN(IF(STBI!$D$11:$D$30&gt;AVERAGE(B16,C16),STBI!$D$11:$D$30)),STBI!$D$11:$D$30),1))</f>
+        <v>+III</v>
+      </c>
+      <c r="H16" s="9" t="str">
+        <f t="array" ref="H16">INDEX(GEKB!$K$11:$K$30,IFERROR(MATCH(MIN(IF(GEKB!$D$11:$D$30&gt;AVERAGE(B16,C16),GEKB!$D$11:$D$30)),GEKB!$D$11:$D$30),1))</f>
+        <v>+III</v>
+      </c>
+      <c r="I16" s="9">
+        <f t="array" ref="I16">INDEX(DA!$K$50:$K$71,IFERROR(MATCH(MIN(IF(DA!$D$50:$D$71&gt;AVERAGE(B16,C16),DA!$D$50:$D$71)),DA!$D$50:$D$71),1))</f>
+        <v>0</v>
       </c>
       <c r="J16" s="9" t="str">
-        <f t="array" ref="J16">INDEX(BSKW!$K$11:$K$30,IFERROR(MATCH(MIN(IF(BSKW!$D$11:$D$30&gt;AVERAGE(B16,C16),BSKW!$D$11:$D$30)),BSKW!$D$11:$D$30),1))</f>
-        <v>+III</v>
-      </c>
-      <c r="K16" s="12" t="str">
-        <f t="array" ref="K16">INDEX(HTKW!$K$11:$K$30,IFERROR(MATCH(MIN(IF(HTKW!$D$11:$D$30&gt;AVERAGE(B16,C16),HTKW!$D$11:$D$30)),HTKW!$D$11:$D$30),1))</f>
-        <v>+III</v>
-      </c>
-    </row>
-    <row r="17" spans="2:11" x14ac:dyDescent="0.25">
+        <f t="array" ref="J16">INDEX(STKWp!$K$11:$K$30,IFERROR(MATCH(MIN(IF(STKWp!$D$11:$D$30&gt;AVERAGE(B16,C16),STKWp!$D$11:$D$30)),STKWp!$D$11:$D$30),1))</f>
+        <v>+III</v>
+      </c>
+      <c r="K16" s="9" t="str">
+        <f t="array" ref="K16">INDEX(BSKW!$K$11:$K$30,IFERROR(MATCH(MIN(IF(BSKW!$D$11:$D$30&gt;AVERAGE(B16,C16),BSKW!$D$11:$D$30)),BSKW!$D$11:$D$30),1))</f>
+        <v>+III</v>
+      </c>
+      <c r="L16" s="12" t="str">
+        <f t="array" ref="L16">INDEX(HTKW!$K$11:$K$30,IFERROR(MATCH(MIN(IF(HTKW!$D$11:$D$30&gt;AVERAGE(B16,C16),HTKW!$D$11:$D$30)),HTKW!$D$11:$D$30),1))</f>
+        <v>+III</v>
+      </c>
+    </row>
+    <row r="17" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B17" s="8">
         <v>2.395</v>
       </c>
@@ -3092,36 +3155,40 @@
         <f t="shared" si="0"/>
         <v>+0</v>
       </c>
-      <c r="E17" s="9" t="str">
-        <f t="array" ref="E17">INDEX(STPH!$O$11:$O$30,IFERROR(MATCH(MIN(IF(STPH!$D$11:$D$30&gt;AVERAGE(B17,C17),STPH!$D$11:$D$30)),STPH!$D$11:$D$30),1))</f>
-        <v>+III</v>
+      <c r="E17" s="23" t="str">
+        <f t="shared" si="1"/>
+        <v>+0</v>
       </c>
       <c r="F17" s="9" t="str">
-        <f t="array" ref="F17">INDEX(STBI!$O$11:$O$30,IFERROR(MATCH(MIN(IF(STBI!$D$11:$D$30&gt;AVERAGE(B17,C17),STBI!$D$11:$D$30)),STBI!$D$11:$D$30),1))</f>
+        <f t="array" ref="F17">INDEX(STPH!$O$11:$O$30,IFERROR(MATCH(MIN(IF(STPH!$D$11:$D$30&gt;AVERAGE(B17,C17),STPH!$D$11:$D$30)),STPH!$D$11:$D$30),1))</f>
         <v>+III</v>
       </c>
       <c r="G17" s="9" t="str">
-        <f t="array" ref="G17">INDEX(GEKB!$K$11:$K$30,IFERROR(MATCH(MIN(IF(GEKB!$D$11:$D$30&gt;AVERAGE(B17,C17),GEKB!$D$11:$D$30)),GEKB!$D$11:$D$30),1))</f>
-        <v>+III</v>
-      </c>
-      <c r="H17" s="9">
-        <f t="array" ref="H17">INDEX(DA!$K$50:$K$71,IFERROR(MATCH(MIN(IF(DA!$D$50:$D$71&gt;AVERAGE(B17,C17),DA!$D$50:$D$71)),DA!$D$50:$D$71),1))</f>
-        <v>0</v>
-      </c>
-      <c r="I17" s="9" t="str">
-        <f t="array" ref="I17">INDEX(STKWp!$K$11:$K$30,IFERROR(MATCH(MIN(IF(STKWp!$D$11:$D$30&gt;AVERAGE(B17,C17),STKWp!$D$11:$D$30)),STKWp!$D$11:$D$30),1))</f>
-        <v>+III</v>
+        <f t="array" ref="G17">INDEX(STBI!$O$11:$O$30,IFERROR(MATCH(MIN(IF(STBI!$D$11:$D$30&gt;AVERAGE(B17,C17),STBI!$D$11:$D$30)),STBI!$D$11:$D$30),1))</f>
+        <v>+III</v>
+      </c>
+      <c r="H17" s="9" t="str">
+        <f t="array" ref="H17">INDEX(GEKB!$K$11:$K$30,IFERROR(MATCH(MIN(IF(GEKB!$D$11:$D$30&gt;AVERAGE(B17,C17),GEKB!$D$11:$D$30)),GEKB!$D$11:$D$30),1))</f>
+        <v>+III</v>
+      </c>
+      <c r="I17" s="9">
+        <f t="array" ref="I17">INDEX(DA!$K$50:$K$71,IFERROR(MATCH(MIN(IF(DA!$D$50:$D$71&gt;AVERAGE(B17,C17),DA!$D$50:$D$71)),DA!$D$50:$D$71),1))</f>
+        <v>0</v>
       </c>
       <c r="J17" s="9" t="str">
-        <f t="array" ref="J17">INDEX(BSKW!$K$11:$K$30,IFERROR(MATCH(MIN(IF(BSKW!$D$11:$D$30&gt;AVERAGE(B17,C17),BSKW!$D$11:$D$30)),BSKW!$D$11:$D$30),1))</f>
-        <v>+III</v>
-      </c>
-      <c r="K17" s="12" t="str">
-        <f t="array" ref="K17">INDEX(HTKW!$K$11:$K$30,IFERROR(MATCH(MIN(IF(HTKW!$D$11:$D$30&gt;AVERAGE(B17,C17),HTKW!$D$11:$D$30)),HTKW!$D$11:$D$30),1))</f>
-        <v>+III</v>
-      </c>
-    </row>
-    <row r="18" spans="2:11" x14ac:dyDescent="0.25">
+        <f t="array" ref="J17">INDEX(STKWp!$K$11:$K$30,IFERROR(MATCH(MIN(IF(STKWp!$D$11:$D$30&gt;AVERAGE(B17,C17),STKWp!$D$11:$D$30)),STKWp!$D$11:$D$30),1))</f>
+        <v>+III</v>
+      </c>
+      <c r="K17" s="9" t="str">
+        <f t="array" ref="K17">INDEX(BSKW!$K$11:$K$30,IFERROR(MATCH(MIN(IF(BSKW!$D$11:$D$30&gt;AVERAGE(B17,C17),BSKW!$D$11:$D$30)),BSKW!$D$11:$D$30),1))</f>
+        <v>+III</v>
+      </c>
+      <c r="L17" s="12" t="str">
+        <f t="array" ref="L17">INDEX(HTKW!$K$11:$K$30,IFERROR(MATCH(MIN(IF(HTKW!$D$11:$D$30&gt;AVERAGE(B17,C17),HTKW!$D$11:$D$30)),HTKW!$D$11:$D$30),1))</f>
+        <v>+III</v>
+      </c>
+    </row>
+    <row r="18" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B18" s="8">
         <v>2.524</v>
       </c>
@@ -3132,36 +3199,40 @@
         <f t="shared" si="0"/>
         <v>+0</v>
       </c>
-      <c r="E18" s="9" t="str">
-        <f t="array" ref="E18">INDEX(STPH!$O$11:$O$30,IFERROR(MATCH(MIN(IF(STPH!$D$11:$D$30&gt;AVERAGE(B18,C18),STPH!$D$11:$D$30)),STPH!$D$11:$D$30),1))</f>
-        <v>+III</v>
+      <c r="E18" s="23" t="str">
+        <f t="shared" si="1"/>
+        <v>+0</v>
       </c>
       <c r="F18" s="9" t="str">
-        <f t="array" ref="F18">INDEX(STBI!$O$11:$O$30,IFERROR(MATCH(MIN(IF(STBI!$D$11:$D$30&gt;AVERAGE(B18,C18),STBI!$D$11:$D$30)),STBI!$D$11:$D$30),1))</f>
+        <f t="array" ref="F18">INDEX(STPH!$O$11:$O$30,IFERROR(MATCH(MIN(IF(STPH!$D$11:$D$30&gt;AVERAGE(B18,C18),STPH!$D$11:$D$30)),STPH!$D$11:$D$30),1))</f>
         <v>+III</v>
       </c>
       <c r="G18" s="9" t="str">
-        <f t="array" ref="G18">INDEX(GEKB!$K$11:$K$30,IFERROR(MATCH(MIN(IF(GEKB!$D$11:$D$30&gt;AVERAGE(B18,C18),GEKB!$D$11:$D$30)),GEKB!$D$11:$D$30),1))</f>
-        <v>+III</v>
-      </c>
-      <c r="H18" s="9">
-        <f t="array" ref="H18">INDEX(DA!$K$50:$K$71,IFERROR(MATCH(MIN(IF(DA!$D$50:$D$71&gt;AVERAGE(B18,C18),DA!$D$50:$D$71)),DA!$D$50:$D$71),1))</f>
-        <v>0</v>
-      </c>
-      <c r="I18" s="9" t="str">
-        <f t="array" ref="I18">INDEX(STKWp!$K$11:$K$30,IFERROR(MATCH(MIN(IF(STKWp!$D$11:$D$30&gt;AVERAGE(B18,C18),STKWp!$D$11:$D$30)),STKWp!$D$11:$D$30),1))</f>
-        <v>+III</v>
+        <f t="array" ref="G18">INDEX(STBI!$O$11:$O$30,IFERROR(MATCH(MIN(IF(STBI!$D$11:$D$30&gt;AVERAGE(B18,C18),STBI!$D$11:$D$30)),STBI!$D$11:$D$30),1))</f>
+        <v>+III</v>
+      </c>
+      <c r="H18" s="9" t="str">
+        <f t="array" ref="H18">INDEX(GEKB!$K$11:$K$30,IFERROR(MATCH(MIN(IF(GEKB!$D$11:$D$30&gt;AVERAGE(B18,C18),GEKB!$D$11:$D$30)),GEKB!$D$11:$D$30),1))</f>
+        <v>+III</v>
+      </c>
+      <c r="I18" s="9">
+        <f t="array" ref="I18">INDEX(DA!$K$50:$K$71,IFERROR(MATCH(MIN(IF(DA!$D$50:$D$71&gt;AVERAGE(B18,C18),DA!$D$50:$D$71)),DA!$D$50:$D$71),1))</f>
+        <v>0</v>
       </c>
       <c r="J18" s="9" t="str">
-        <f t="array" ref="J18">INDEX(BSKW!$K$11:$K$30,IFERROR(MATCH(MIN(IF(BSKW!$D$11:$D$30&gt;AVERAGE(B18,C18),BSKW!$D$11:$D$30)),BSKW!$D$11:$D$30),1))</f>
-        <v>+III</v>
-      </c>
-      <c r="K18" s="12" t="str">
-        <f t="array" ref="K18">INDEX(HTKW!$K$11:$K$30,IFERROR(MATCH(MIN(IF(HTKW!$D$11:$D$30&gt;AVERAGE(B18,C18),HTKW!$D$11:$D$30)),HTKW!$D$11:$D$30),1))</f>
-        <v>+III</v>
-      </c>
-    </row>
-    <row r="19" spans="2:11" x14ac:dyDescent="0.25">
+        <f t="array" ref="J18">INDEX(STKWp!$K$11:$K$30,IFERROR(MATCH(MIN(IF(STKWp!$D$11:$D$30&gt;AVERAGE(B18,C18),STKWp!$D$11:$D$30)),STKWp!$D$11:$D$30),1))</f>
+        <v>+III</v>
+      </c>
+      <c r="K18" s="9" t="str">
+        <f t="array" ref="K18">INDEX(BSKW!$K$11:$K$30,IFERROR(MATCH(MIN(IF(BSKW!$D$11:$D$30&gt;AVERAGE(B18,C18),BSKW!$D$11:$D$30)),BSKW!$D$11:$D$30),1))</f>
+        <v>+III</v>
+      </c>
+      <c r="L18" s="12" t="str">
+        <f t="array" ref="L18">INDEX(HTKW!$K$11:$K$30,IFERROR(MATCH(MIN(IF(HTKW!$D$11:$D$30&gt;AVERAGE(B18,C18),HTKW!$D$11:$D$30)),HTKW!$D$11:$D$30),1))</f>
+        <v>+III</v>
+      </c>
+    </row>
+    <row r="19" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B19" s="8">
         <v>2.6560000000000001</v>
       </c>
@@ -3172,36 +3243,40 @@
         <f t="shared" si="0"/>
         <v>+0</v>
       </c>
-      <c r="E19" s="9" t="str">
-        <f t="array" ref="E19">INDEX(STPH!$O$11:$O$30,IFERROR(MATCH(MIN(IF(STPH!$D$11:$D$30&gt;AVERAGE(B19,C19),STPH!$D$11:$D$30)),STPH!$D$11:$D$30),1))</f>
-        <v>+III</v>
+      <c r="E19" s="23" t="str">
+        <f t="shared" si="1"/>
+        <v>+0</v>
       </c>
       <c r="F19" s="9" t="str">
-        <f t="array" ref="F19">INDEX(STBI!$O$11:$O$30,IFERROR(MATCH(MIN(IF(STBI!$D$11:$D$30&gt;AVERAGE(B19,C19),STBI!$D$11:$D$30)),STBI!$D$11:$D$30),1))</f>
+        <f t="array" ref="F19">INDEX(STPH!$O$11:$O$30,IFERROR(MATCH(MIN(IF(STPH!$D$11:$D$30&gt;AVERAGE(B19,C19),STPH!$D$11:$D$30)),STPH!$D$11:$D$30),1))</f>
         <v>+III</v>
       </c>
       <c r="G19" s="9" t="str">
-        <f t="array" ref="G19">INDEX(GEKB!$K$11:$K$30,IFERROR(MATCH(MIN(IF(GEKB!$D$11:$D$30&gt;AVERAGE(B19,C19),GEKB!$D$11:$D$30)),GEKB!$D$11:$D$30),1))</f>
-        <v>+III</v>
-      </c>
-      <c r="H19" s="9">
-        <f t="array" ref="H19">INDEX(DA!$K$50:$K$71,IFERROR(MATCH(MIN(IF(DA!$D$50:$D$71&gt;AVERAGE(B19,C19),DA!$D$50:$D$71)),DA!$D$50:$D$71),1))</f>
-        <v>0</v>
-      </c>
-      <c r="I19" s="9" t="str">
-        <f t="array" ref="I19">INDEX(STKWp!$K$11:$K$30,IFERROR(MATCH(MIN(IF(STKWp!$D$11:$D$30&gt;AVERAGE(B19,C19),STKWp!$D$11:$D$30)),STKWp!$D$11:$D$30),1))</f>
-        <v>+III</v>
+        <f t="array" ref="G19">INDEX(STBI!$O$11:$O$30,IFERROR(MATCH(MIN(IF(STBI!$D$11:$D$30&gt;AVERAGE(B19,C19),STBI!$D$11:$D$30)),STBI!$D$11:$D$30),1))</f>
+        <v>+III</v>
+      </c>
+      <c r="H19" s="9" t="str">
+        <f t="array" ref="H19">INDEX(GEKB!$K$11:$K$30,IFERROR(MATCH(MIN(IF(GEKB!$D$11:$D$30&gt;AVERAGE(B19,C19),GEKB!$D$11:$D$30)),GEKB!$D$11:$D$30),1))</f>
+        <v>+III</v>
+      </c>
+      <c r="I19" s="9">
+        <f t="array" ref="I19">INDEX(DA!$K$50:$K$71,IFERROR(MATCH(MIN(IF(DA!$D$50:$D$71&gt;AVERAGE(B19,C19),DA!$D$50:$D$71)),DA!$D$50:$D$71),1))</f>
+        <v>0</v>
       </c>
       <c r="J19" s="9" t="str">
-        <f t="array" ref="J19">INDEX(BSKW!$K$11:$K$30,IFERROR(MATCH(MIN(IF(BSKW!$D$11:$D$30&gt;AVERAGE(B19,C19),BSKW!$D$11:$D$30)),BSKW!$D$11:$D$30),1))</f>
-        <v>+III</v>
-      </c>
-      <c r="K19" s="12" t="str">
-        <f t="array" ref="K19">INDEX(HTKW!$K$11:$K$30,IFERROR(MATCH(MIN(IF(HTKW!$D$11:$D$30&gt;AVERAGE(B19,C19),HTKW!$D$11:$D$30)),HTKW!$D$11:$D$30),1))</f>
-        <v>+III</v>
-      </c>
-    </row>
-    <row r="20" spans="2:11" x14ac:dyDescent="0.25">
+        <f t="array" ref="J19">INDEX(STKWp!$K$11:$K$30,IFERROR(MATCH(MIN(IF(STKWp!$D$11:$D$30&gt;AVERAGE(B19,C19),STKWp!$D$11:$D$30)),STKWp!$D$11:$D$30),1))</f>
+        <v>+III</v>
+      </c>
+      <c r="K19" s="9" t="str">
+        <f t="array" ref="K19">INDEX(BSKW!$K$11:$K$30,IFERROR(MATCH(MIN(IF(BSKW!$D$11:$D$30&gt;AVERAGE(B19,C19),BSKW!$D$11:$D$30)),BSKW!$D$11:$D$30),1))</f>
+        <v>+III</v>
+      </c>
+      <c r="L19" s="12" t="str">
+        <f t="array" ref="L19">INDEX(HTKW!$K$11:$K$30,IFERROR(MATCH(MIN(IF(HTKW!$D$11:$D$30&gt;AVERAGE(B19,C19),HTKW!$D$11:$D$30)),HTKW!$D$11:$D$30),1))</f>
+        <v>+III</v>
+      </c>
+    </row>
+    <row r="20" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B20" s="8">
         <v>2.7959999999999998</v>
       </c>
@@ -3212,36 +3287,40 @@
         <f t="shared" si="0"/>
         <v>+0</v>
       </c>
-      <c r="E20" s="9" t="str">
-        <f t="array" ref="E20">INDEX(STPH!$O$11:$O$30,IFERROR(MATCH(MIN(IF(STPH!$D$11:$D$30&gt;AVERAGE(B20,C20),STPH!$D$11:$D$30)),STPH!$D$11:$D$30),1))</f>
-        <v>+III</v>
+      <c r="E20" s="23" t="str">
+        <f t="shared" si="1"/>
+        <v>+0</v>
       </c>
       <c r="F20" s="9" t="str">
-        <f t="array" ref="F20">INDEX(STBI!$O$11:$O$30,IFERROR(MATCH(MIN(IF(STBI!$D$11:$D$30&gt;AVERAGE(B20,C20),STBI!$D$11:$D$30)),STBI!$D$11:$D$30),1))</f>
+        <f t="array" ref="F20">INDEX(STPH!$O$11:$O$30,IFERROR(MATCH(MIN(IF(STPH!$D$11:$D$30&gt;AVERAGE(B20,C20),STPH!$D$11:$D$30)),STPH!$D$11:$D$30),1))</f>
         <v>+III</v>
       </c>
       <c r="G20" s="9" t="str">
-        <f t="array" ref="G20">INDEX(GEKB!$K$11:$K$30,IFERROR(MATCH(MIN(IF(GEKB!$D$11:$D$30&gt;AVERAGE(B20,C20),GEKB!$D$11:$D$30)),GEKB!$D$11:$D$30),1))</f>
-        <v>+III</v>
-      </c>
-      <c r="H20" s="9">
-        <f t="array" ref="H20">INDEX(DA!$K$50:$K$71,IFERROR(MATCH(MIN(IF(DA!$D$50:$D$71&gt;AVERAGE(B20,C20),DA!$D$50:$D$71)),DA!$D$50:$D$71),1))</f>
-        <v>0</v>
-      </c>
-      <c r="I20" s="9" t="str">
-        <f t="array" ref="I20">INDEX(STKWp!$K$11:$K$30,IFERROR(MATCH(MIN(IF(STKWp!$D$11:$D$30&gt;AVERAGE(B20,C20),STKWp!$D$11:$D$30)),STKWp!$D$11:$D$30),1))</f>
-        <v>+III</v>
+        <f t="array" ref="G20">INDEX(STBI!$O$11:$O$30,IFERROR(MATCH(MIN(IF(STBI!$D$11:$D$30&gt;AVERAGE(B20,C20),STBI!$D$11:$D$30)),STBI!$D$11:$D$30),1))</f>
+        <v>+III</v>
+      </c>
+      <c r="H20" s="9" t="str">
+        <f t="array" ref="H20">INDEX(GEKB!$K$11:$K$30,IFERROR(MATCH(MIN(IF(GEKB!$D$11:$D$30&gt;AVERAGE(B20,C20),GEKB!$D$11:$D$30)),GEKB!$D$11:$D$30),1))</f>
+        <v>+III</v>
+      </c>
+      <c r="I20" s="9">
+        <f t="array" ref="I20">INDEX(DA!$K$50:$K$71,IFERROR(MATCH(MIN(IF(DA!$D$50:$D$71&gt;AVERAGE(B20,C20),DA!$D$50:$D$71)),DA!$D$50:$D$71),1))</f>
+        <v>0</v>
       </c>
       <c r="J20" s="9" t="str">
-        <f t="array" ref="J20">INDEX(BSKW!$K$11:$K$30,IFERROR(MATCH(MIN(IF(BSKW!$D$11:$D$30&gt;AVERAGE(B20,C20),BSKW!$D$11:$D$30)),BSKW!$D$11:$D$30),1))</f>
-        <v>+III</v>
-      </c>
-      <c r="K20" s="12" t="str">
-        <f t="array" ref="K20">INDEX(HTKW!$K$11:$K$30,IFERROR(MATCH(MIN(IF(HTKW!$D$11:$D$30&gt;AVERAGE(B20,C20),HTKW!$D$11:$D$30)),HTKW!$D$11:$D$30),1))</f>
-        <v>+III</v>
-      </c>
-    </row>
-    <row r="21" spans="2:11" x14ac:dyDescent="0.25">
+        <f t="array" ref="J20">INDEX(STKWp!$K$11:$K$30,IFERROR(MATCH(MIN(IF(STKWp!$D$11:$D$30&gt;AVERAGE(B20,C20),STKWp!$D$11:$D$30)),STKWp!$D$11:$D$30),1))</f>
+        <v>+III</v>
+      </c>
+      <c r="K20" s="9" t="str">
+        <f t="array" ref="K20">INDEX(BSKW!$K$11:$K$30,IFERROR(MATCH(MIN(IF(BSKW!$D$11:$D$30&gt;AVERAGE(B20,C20),BSKW!$D$11:$D$30)),BSKW!$D$11:$D$30),1))</f>
+        <v>+III</v>
+      </c>
+      <c r="L20" s="12" t="str">
+        <f t="array" ref="L20">INDEX(HTKW!$K$11:$K$30,IFERROR(MATCH(MIN(IF(HTKW!$D$11:$D$30&gt;AVERAGE(B20,C20),HTKW!$D$11:$D$30)),HTKW!$D$11:$D$30),1))</f>
+        <v>+III</v>
+      </c>
+    </row>
+    <row r="21" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B21" s="8">
         <v>2.9569999999999999</v>
       </c>
@@ -3252,36 +3331,40 @@
         <f t="shared" si="0"/>
         <v>+0</v>
       </c>
-      <c r="E21" s="9" t="str">
-        <f t="array" ref="E21">INDEX(STPH!$O$11:$O$30,IFERROR(MATCH(MIN(IF(STPH!$D$11:$D$30&gt;AVERAGE(B21,C21),STPH!$D$11:$D$30)),STPH!$D$11:$D$30),1))</f>
-        <v>+III</v>
+      <c r="E21" s="23" t="str">
+        <f t="shared" si="1"/>
+        <v>+0</v>
       </c>
       <c r="F21" s="9" t="str">
-        <f t="array" ref="F21">INDEX(STBI!$O$11:$O$30,IFERROR(MATCH(MIN(IF(STBI!$D$11:$D$30&gt;AVERAGE(B21,C21),STBI!$D$11:$D$30)),STBI!$D$11:$D$30),1))</f>
+        <f t="array" ref="F21">INDEX(STPH!$O$11:$O$30,IFERROR(MATCH(MIN(IF(STPH!$D$11:$D$30&gt;AVERAGE(B21,C21),STPH!$D$11:$D$30)),STPH!$D$11:$D$30),1))</f>
         <v>+III</v>
       </c>
       <c r="G21" s="9" t="str">
-        <f t="array" ref="G21">INDEX(GEKB!$K$11:$K$30,IFERROR(MATCH(MIN(IF(GEKB!$D$11:$D$30&gt;AVERAGE(B21,C21),GEKB!$D$11:$D$30)),GEKB!$D$11:$D$30),1))</f>
-        <v>+III</v>
-      </c>
-      <c r="H21" s="9">
-        <f t="array" ref="H21">INDEX(DA!$K$50:$K$71,IFERROR(MATCH(MIN(IF(DA!$D$50:$D$71&gt;AVERAGE(B21,C21),DA!$D$50:$D$71)),DA!$D$50:$D$71),1))</f>
-        <v>0</v>
-      </c>
-      <c r="I21" s="9" t="str">
-        <f t="array" ref="I21">INDEX(STKWp!$K$11:$K$30,IFERROR(MATCH(MIN(IF(STKWp!$D$11:$D$30&gt;AVERAGE(B21,C21),STKWp!$D$11:$D$30)),STKWp!$D$11:$D$30),1))</f>
-        <v>+III</v>
+        <f t="array" ref="G21">INDEX(STBI!$O$11:$O$30,IFERROR(MATCH(MIN(IF(STBI!$D$11:$D$30&gt;AVERAGE(B21,C21),STBI!$D$11:$D$30)),STBI!$D$11:$D$30),1))</f>
+        <v>+III</v>
+      </c>
+      <c r="H21" s="9" t="str">
+        <f t="array" ref="H21">INDEX(GEKB!$K$11:$K$30,IFERROR(MATCH(MIN(IF(GEKB!$D$11:$D$30&gt;AVERAGE(B21,C21),GEKB!$D$11:$D$30)),GEKB!$D$11:$D$30),1))</f>
+        <v>+III</v>
+      </c>
+      <c r="I21" s="9">
+        <f t="array" ref="I21">INDEX(DA!$K$50:$K$71,IFERROR(MATCH(MIN(IF(DA!$D$50:$D$71&gt;AVERAGE(B21,C21),DA!$D$50:$D$71)),DA!$D$50:$D$71),1))</f>
+        <v>0</v>
       </c>
       <c r="J21" s="9" t="str">
-        <f t="array" ref="J21">INDEX(BSKW!$K$11:$K$30,IFERROR(MATCH(MIN(IF(BSKW!$D$11:$D$30&gt;AVERAGE(B21,C21),BSKW!$D$11:$D$30)),BSKW!$D$11:$D$30),1))</f>
-        <v>+III</v>
-      </c>
-      <c r="K21" s="12" t="str">
-        <f t="array" ref="K21">INDEX(HTKW!$K$11:$K$30,IFERROR(MATCH(MIN(IF(HTKW!$D$11:$D$30&gt;AVERAGE(B21,C21),HTKW!$D$11:$D$30)),HTKW!$D$11:$D$30),1))</f>
-        <v>+III</v>
-      </c>
-    </row>
-    <row r="22" spans="2:11" x14ac:dyDescent="0.25">
+        <f t="array" ref="J21">INDEX(STKWp!$K$11:$K$30,IFERROR(MATCH(MIN(IF(STKWp!$D$11:$D$30&gt;AVERAGE(B21,C21),STKWp!$D$11:$D$30)),STKWp!$D$11:$D$30),1))</f>
+        <v>+III</v>
+      </c>
+      <c r="K21" s="9" t="str">
+        <f t="array" ref="K21">INDEX(BSKW!$K$11:$K$30,IFERROR(MATCH(MIN(IF(BSKW!$D$11:$D$30&gt;AVERAGE(B21,C21),BSKW!$D$11:$D$30)),BSKW!$D$11:$D$30),1))</f>
+        <v>+III</v>
+      </c>
+      <c r="L21" s="12" t="str">
+        <f t="array" ref="L21">INDEX(HTKW!$K$11:$K$30,IFERROR(MATCH(MIN(IF(HTKW!$D$11:$D$30&gt;AVERAGE(B21,C21),HTKW!$D$11:$D$30)),HTKW!$D$11:$D$30),1))</f>
+        <v>+III</v>
+      </c>
+    </row>
+    <row r="22" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B22" s="8">
         <v>3.129</v>
       </c>
@@ -3292,36 +3375,40 @@
         <f t="shared" si="0"/>
         <v>+0</v>
       </c>
-      <c r="E22" s="9" t="str">
-        <f t="array" ref="E22">INDEX(STPH!$O$11:$O$30,IFERROR(MATCH(MIN(IF(STPH!$D$11:$D$30&gt;AVERAGE(B22,C22),STPH!$D$11:$D$30)),STPH!$D$11:$D$30),1))</f>
-        <v>+III</v>
+      <c r="E22" s="23" t="str">
+        <f t="shared" si="1"/>
+        <v>+0</v>
       </c>
       <c r="F22" s="9" t="str">
-        <f t="array" ref="F22">INDEX(STBI!$O$11:$O$30,IFERROR(MATCH(MIN(IF(STBI!$D$11:$D$30&gt;AVERAGE(B22,C22),STBI!$D$11:$D$30)),STBI!$D$11:$D$30),1))</f>
+        <f t="array" ref="F22">INDEX(STPH!$O$11:$O$30,IFERROR(MATCH(MIN(IF(STPH!$D$11:$D$30&gt;AVERAGE(B22,C22),STPH!$D$11:$D$30)),STPH!$D$11:$D$30),1))</f>
         <v>+III</v>
       </c>
       <c r="G22" s="9" t="str">
-        <f t="array" ref="G22">INDEX(GEKB!$K$11:$K$30,IFERROR(MATCH(MIN(IF(GEKB!$D$11:$D$30&gt;AVERAGE(B22,C22),GEKB!$D$11:$D$30)),GEKB!$D$11:$D$30),1))</f>
-        <v>+III</v>
-      </c>
-      <c r="H22" s="9">
-        <f t="array" ref="H22">INDEX(DA!$K$50:$K$71,IFERROR(MATCH(MIN(IF(DA!$D$50:$D$71&gt;AVERAGE(B22,C22),DA!$D$50:$D$71)),DA!$D$50:$D$71),1))</f>
-        <v>0</v>
-      </c>
-      <c r="I22" s="9" t="str">
-        <f t="array" ref="I22">INDEX(STKWp!$K$11:$K$30,IFERROR(MATCH(MIN(IF(STKWp!$D$11:$D$30&gt;AVERAGE(B22,C22),STKWp!$D$11:$D$30)),STKWp!$D$11:$D$30),1))</f>
-        <v>+III</v>
+        <f t="array" ref="G22">INDEX(STBI!$O$11:$O$30,IFERROR(MATCH(MIN(IF(STBI!$D$11:$D$30&gt;AVERAGE(B22,C22),STBI!$D$11:$D$30)),STBI!$D$11:$D$30),1))</f>
+        <v>+III</v>
+      </c>
+      <c r="H22" s="9" t="str">
+        <f t="array" ref="H22">INDEX(GEKB!$K$11:$K$30,IFERROR(MATCH(MIN(IF(GEKB!$D$11:$D$30&gt;AVERAGE(B22,C22),GEKB!$D$11:$D$30)),GEKB!$D$11:$D$30),1))</f>
+        <v>+III</v>
+      </c>
+      <c r="I22" s="9">
+        <f t="array" ref="I22">INDEX(DA!$K$50:$K$71,IFERROR(MATCH(MIN(IF(DA!$D$50:$D$71&gt;AVERAGE(B22,C22),DA!$D$50:$D$71)),DA!$D$50:$D$71),1))</f>
+        <v>0</v>
       </c>
       <c r="J22" s="9" t="str">
-        <f t="array" ref="J22">INDEX(BSKW!$K$11:$K$30,IFERROR(MATCH(MIN(IF(BSKW!$D$11:$D$30&gt;AVERAGE(B22,C22),BSKW!$D$11:$D$30)),BSKW!$D$11:$D$30),1))</f>
-        <v>+III</v>
-      </c>
-      <c r="K22" s="12" t="str">
-        <f t="array" ref="K22">INDEX(HTKW!$K$11:$K$30,IFERROR(MATCH(MIN(IF(HTKW!$D$11:$D$30&gt;AVERAGE(B22,C22),HTKW!$D$11:$D$30)),HTKW!$D$11:$D$30),1))</f>
-        <v>+III</v>
-      </c>
-    </row>
-    <row r="23" spans="2:11" x14ac:dyDescent="0.25">
+        <f t="array" ref="J22">INDEX(STKWp!$K$11:$K$30,IFERROR(MATCH(MIN(IF(STKWp!$D$11:$D$30&gt;AVERAGE(B22,C22),STKWp!$D$11:$D$30)),STKWp!$D$11:$D$30),1))</f>
+        <v>+III</v>
+      </c>
+      <c r="K22" s="9" t="str">
+        <f t="array" ref="K22">INDEX(BSKW!$K$11:$K$30,IFERROR(MATCH(MIN(IF(BSKW!$D$11:$D$30&gt;AVERAGE(B22,C22),BSKW!$D$11:$D$30)),BSKW!$D$11:$D$30),1))</f>
+        <v>+III</v>
+      </c>
+      <c r="L22" s="12" t="str">
+        <f t="array" ref="L22">INDEX(HTKW!$K$11:$K$30,IFERROR(MATCH(MIN(IF(HTKW!$D$11:$D$30&gt;AVERAGE(B22,C22),HTKW!$D$11:$D$30)),HTKW!$D$11:$D$30),1))</f>
+        <v>+III</v>
+      </c>
+    </row>
+    <row r="23" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B23" s="8">
         <v>3.302</v>
       </c>
@@ -3332,36 +3419,40 @@
         <f t="shared" si="0"/>
         <v>+0</v>
       </c>
-      <c r="E23" s="9" t="str">
-        <f t="array" ref="E23">INDEX(STPH!$O$11:$O$30,IFERROR(MATCH(MIN(IF(STPH!$D$11:$D$30&gt;AVERAGE(B23,C23),STPH!$D$11:$D$30)),STPH!$D$11:$D$30),1))</f>
-        <v>+III</v>
+      <c r="E23" s="23" t="str">
+        <f t="shared" si="1"/>
+        <v>+0</v>
       </c>
       <c r="F23" s="9" t="str">
-        <f t="array" ref="F23">INDEX(STBI!$O$11:$O$30,IFERROR(MATCH(MIN(IF(STBI!$D$11:$D$30&gt;AVERAGE(B23,C23),STBI!$D$11:$D$30)),STBI!$D$11:$D$30),1))</f>
+        <f t="array" ref="F23">INDEX(STPH!$O$11:$O$30,IFERROR(MATCH(MIN(IF(STPH!$D$11:$D$30&gt;AVERAGE(B23,C23),STPH!$D$11:$D$30)),STPH!$D$11:$D$30),1))</f>
         <v>+III</v>
       </c>
       <c r="G23" s="9" t="str">
-        <f t="array" ref="G23">INDEX(GEKB!$K$11:$K$30,IFERROR(MATCH(MIN(IF(GEKB!$D$11:$D$30&gt;AVERAGE(B23,C23),GEKB!$D$11:$D$30)),GEKB!$D$11:$D$30),1))</f>
-        <v>+III</v>
-      </c>
-      <c r="H23" s="9">
-        <f t="array" ref="H23">INDEX(DA!$K$50:$K$71,IFERROR(MATCH(MIN(IF(DA!$D$50:$D$71&gt;AVERAGE(B23,C23),DA!$D$50:$D$71)),DA!$D$50:$D$71),1))</f>
-        <v>0</v>
-      </c>
-      <c r="I23" s="9" t="str">
-        <f t="array" ref="I23">INDEX(STKWp!$K$11:$K$30,IFERROR(MATCH(MIN(IF(STKWp!$D$11:$D$30&gt;AVERAGE(B23,C23),STKWp!$D$11:$D$30)),STKWp!$D$11:$D$30),1))</f>
-        <v>+III</v>
+        <f t="array" ref="G23">INDEX(STBI!$O$11:$O$30,IFERROR(MATCH(MIN(IF(STBI!$D$11:$D$30&gt;AVERAGE(B23,C23),STBI!$D$11:$D$30)),STBI!$D$11:$D$30),1))</f>
+        <v>+III</v>
+      </c>
+      <c r="H23" s="9" t="str">
+        <f t="array" ref="H23">INDEX(GEKB!$K$11:$K$30,IFERROR(MATCH(MIN(IF(GEKB!$D$11:$D$30&gt;AVERAGE(B23,C23),GEKB!$D$11:$D$30)),GEKB!$D$11:$D$30),1))</f>
+        <v>+III</v>
+      </c>
+      <c r="I23" s="9">
+        <f t="array" ref="I23">INDEX(DA!$K$50:$K$71,IFERROR(MATCH(MIN(IF(DA!$D$50:$D$71&gt;AVERAGE(B23,C23),DA!$D$50:$D$71)),DA!$D$50:$D$71),1))</f>
+        <v>0</v>
       </c>
       <c r="J23" s="9" t="str">
-        <f t="array" ref="J23">INDEX(BSKW!$K$11:$K$30,IFERROR(MATCH(MIN(IF(BSKW!$D$11:$D$30&gt;AVERAGE(B23,C23),BSKW!$D$11:$D$30)),BSKW!$D$11:$D$30),1))</f>
-        <v>+III</v>
-      </c>
-      <c r="K23" s="12" t="str">
-        <f t="array" ref="K23">INDEX(HTKW!$K$11:$K$30,IFERROR(MATCH(MIN(IF(HTKW!$D$11:$D$30&gt;AVERAGE(B23,C23),HTKW!$D$11:$D$30)),HTKW!$D$11:$D$30),1))</f>
-        <v>+III</v>
-      </c>
-    </row>
-    <row r="24" spans="2:11" x14ac:dyDescent="0.25">
+        <f t="array" ref="J23">INDEX(STKWp!$K$11:$K$30,IFERROR(MATCH(MIN(IF(STKWp!$D$11:$D$30&gt;AVERAGE(B23,C23),STKWp!$D$11:$D$30)),STKWp!$D$11:$D$30),1))</f>
+        <v>+III</v>
+      </c>
+      <c r="K23" s="9" t="str">
+        <f t="array" ref="K23">INDEX(BSKW!$K$11:$K$30,IFERROR(MATCH(MIN(IF(BSKW!$D$11:$D$30&gt;AVERAGE(B23,C23),BSKW!$D$11:$D$30)),BSKW!$D$11:$D$30),1))</f>
+        <v>+III</v>
+      </c>
+      <c r="L23" s="12" t="str">
+        <f t="array" ref="L23">INDEX(HTKW!$K$11:$K$30,IFERROR(MATCH(MIN(IF(HTKW!$D$11:$D$30&gt;AVERAGE(B23,C23),HTKW!$D$11:$D$30)),HTKW!$D$11:$D$30),1))</f>
+        <v>+III</v>
+      </c>
+    </row>
+    <row r="24" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B24" s="8">
         <v>3.4630000000000001</v>
       </c>
@@ -3372,36 +3463,40 @@
         <f t="shared" si="0"/>
         <v>+0</v>
       </c>
-      <c r="E24" s="9" t="str">
-        <f t="array" ref="E24">INDEX(STPH!$O$11:$O$30,IFERROR(MATCH(MIN(IF(STPH!$D$11:$D$30&gt;AVERAGE(B24,C24),STPH!$D$11:$D$30)),STPH!$D$11:$D$30),1))</f>
-        <v>+III</v>
+      <c r="E24" s="23" t="str">
+        <f t="shared" si="1"/>
+        <v>+0</v>
       </c>
       <c r="F24" s="9" t="str">
-        <f t="array" ref="F24">INDEX(STBI!$O$11:$O$30,IFERROR(MATCH(MIN(IF(STBI!$D$11:$D$30&gt;AVERAGE(B24,C24),STBI!$D$11:$D$30)),STBI!$D$11:$D$30),1))</f>
+        <f t="array" ref="F24">INDEX(STPH!$O$11:$O$30,IFERROR(MATCH(MIN(IF(STPH!$D$11:$D$30&gt;AVERAGE(B24,C24),STPH!$D$11:$D$30)),STPH!$D$11:$D$30),1))</f>
         <v>+III</v>
       </c>
       <c r="G24" s="9" t="str">
-        <f t="array" ref="G24">INDEX(GEKB!$K$11:$K$30,IFERROR(MATCH(MIN(IF(GEKB!$D$11:$D$30&gt;AVERAGE(B24,C24),GEKB!$D$11:$D$30)),GEKB!$D$11:$D$30),1))</f>
-        <v>+III</v>
-      </c>
-      <c r="H24" s="9">
-        <f t="array" ref="H24">INDEX(DA!$K$50:$K$71,IFERROR(MATCH(MIN(IF(DA!$D$50:$D$71&gt;AVERAGE(B24,C24),DA!$D$50:$D$71)),DA!$D$50:$D$71),1))</f>
-        <v>0</v>
-      </c>
-      <c r="I24" s="9" t="str">
-        <f t="array" ref="I24">INDEX(STKWp!$K$11:$K$30,IFERROR(MATCH(MIN(IF(STKWp!$D$11:$D$30&gt;AVERAGE(B24,C24),STKWp!$D$11:$D$30)),STKWp!$D$11:$D$30),1))</f>
-        <v>+III</v>
+        <f t="array" ref="G24">INDEX(STBI!$O$11:$O$30,IFERROR(MATCH(MIN(IF(STBI!$D$11:$D$30&gt;AVERAGE(B24,C24),STBI!$D$11:$D$30)),STBI!$D$11:$D$30),1))</f>
+        <v>+III</v>
+      </c>
+      <c r="H24" s="9" t="str">
+        <f t="array" ref="H24">INDEX(GEKB!$K$11:$K$30,IFERROR(MATCH(MIN(IF(GEKB!$D$11:$D$30&gt;AVERAGE(B24,C24),GEKB!$D$11:$D$30)),GEKB!$D$11:$D$30),1))</f>
+        <v>+III</v>
+      </c>
+      <c r="I24" s="9">
+        <f t="array" ref="I24">INDEX(DA!$K$50:$K$71,IFERROR(MATCH(MIN(IF(DA!$D$50:$D$71&gt;AVERAGE(B24,C24),DA!$D$50:$D$71)),DA!$D$50:$D$71),1))</f>
+        <v>0</v>
       </c>
       <c r="J24" s="9" t="str">
-        <f t="array" ref="J24">INDEX(BSKW!$K$11:$K$30,IFERROR(MATCH(MIN(IF(BSKW!$D$11:$D$30&gt;AVERAGE(B24,C24),BSKW!$D$11:$D$30)),BSKW!$D$11:$D$30),1))</f>
-        <v>+III</v>
-      </c>
-      <c r="K24" s="12" t="str">
-        <f t="array" ref="K24">INDEX(HTKW!$K$11:$K$30,IFERROR(MATCH(MIN(IF(HTKW!$D$11:$D$30&gt;AVERAGE(B24,C24),HTKW!$D$11:$D$30)),HTKW!$D$11:$D$30),1))</f>
-        <v>+III</v>
-      </c>
-    </row>
-    <row r="25" spans="2:11" x14ac:dyDescent="0.25">
+        <f t="array" ref="J24">INDEX(STKWp!$K$11:$K$30,IFERROR(MATCH(MIN(IF(STKWp!$D$11:$D$30&gt;AVERAGE(B24,C24),STKWp!$D$11:$D$30)),STKWp!$D$11:$D$30),1))</f>
+        <v>+III</v>
+      </c>
+      <c r="K24" s="9" t="str">
+        <f t="array" ref="K24">INDEX(BSKW!$K$11:$K$30,IFERROR(MATCH(MIN(IF(BSKW!$D$11:$D$30&gt;AVERAGE(B24,C24),BSKW!$D$11:$D$30)),BSKW!$D$11:$D$30),1))</f>
+        <v>+III</v>
+      </c>
+      <c r="L24" s="12" t="str">
+        <f t="array" ref="L24">INDEX(HTKW!$K$11:$K$30,IFERROR(MATCH(MIN(IF(HTKW!$D$11:$D$30&gt;AVERAGE(B24,C24),HTKW!$D$11:$D$30)),HTKW!$D$11:$D$30),1))</f>
+        <v>+III</v>
+      </c>
+    </row>
+    <row r="25" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B25" s="8">
         <v>3.5960000000000001</v>
       </c>
@@ -3412,36 +3507,40 @@
         <f t="shared" si="0"/>
         <v>+0</v>
       </c>
-      <c r="E25" s="9" t="str">
-        <f t="array" ref="E25">INDEX(STPH!$O$11:$O$30,IFERROR(MATCH(MIN(IF(STPH!$D$11:$D$30&gt;AVERAGE(B25,C25),STPH!$D$11:$D$30)),STPH!$D$11:$D$30),1))</f>
-        <v>+III</v>
+      <c r="E25" s="23" t="str">
+        <f t="shared" si="1"/>
+        <v>+0</v>
       </c>
       <c r="F25" s="9" t="str">
-        <f t="array" ref="F25">INDEX(STBI!$O$11:$O$30,IFERROR(MATCH(MIN(IF(STBI!$D$11:$D$30&gt;AVERAGE(B25,C25),STBI!$D$11:$D$30)),STBI!$D$11:$D$30),1))</f>
+        <f t="array" ref="F25">INDEX(STPH!$O$11:$O$30,IFERROR(MATCH(MIN(IF(STPH!$D$11:$D$30&gt;AVERAGE(B25,C25),STPH!$D$11:$D$30)),STPH!$D$11:$D$30),1))</f>
         <v>+III</v>
       </c>
       <c r="G25" s="9" t="str">
-        <f t="array" ref="G25">INDEX(GEKB!$K$11:$K$30,IFERROR(MATCH(MIN(IF(GEKB!$D$11:$D$30&gt;AVERAGE(B25,C25),GEKB!$D$11:$D$30)),GEKB!$D$11:$D$30),1))</f>
-        <v>+III</v>
-      </c>
-      <c r="H25" s="9">
-        <f t="array" ref="H25">INDEX(DA!$K$50:$K$71,IFERROR(MATCH(MIN(IF(DA!$D$50:$D$71&gt;AVERAGE(B25,C25),DA!$D$50:$D$71)),DA!$D$50:$D$71),1))</f>
-        <v>0</v>
-      </c>
-      <c r="I25" s="9" t="str">
-        <f t="array" ref="I25">INDEX(STKWp!$K$11:$K$30,IFERROR(MATCH(MIN(IF(STKWp!$D$11:$D$30&gt;AVERAGE(B25,C25),STKWp!$D$11:$D$30)),STKWp!$D$11:$D$30),1))</f>
-        <v>+III</v>
+        <f t="array" ref="G25">INDEX(STBI!$O$11:$O$30,IFERROR(MATCH(MIN(IF(STBI!$D$11:$D$30&gt;AVERAGE(B25,C25),STBI!$D$11:$D$30)),STBI!$D$11:$D$30),1))</f>
+        <v>+III</v>
+      </c>
+      <c r="H25" s="9" t="str">
+        <f t="array" ref="H25">INDEX(GEKB!$K$11:$K$30,IFERROR(MATCH(MIN(IF(GEKB!$D$11:$D$30&gt;AVERAGE(B25,C25),GEKB!$D$11:$D$30)),GEKB!$D$11:$D$30),1))</f>
+        <v>+III</v>
+      </c>
+      <c r="I25" s="9">
+        <f t="array" ref="I25">INDEX(DA!$K$50:$K$71,IFERROR(MATCH(MIN(IF(DA!$D$50:$D$71&gt;AVERAGE(B25,C25),DA!$D$50:$D$71)),DA!$D$50:$D$71),1))</f>
+        <v>0</v>
       </c>
       <c r="J25" s="9" t="str">
-        <f t="array" ref="J25">INDEX(BSKW!$K$11:$K$30,IFERROR(MATCH(MIN(IF(BSKW!$D$11:$D$30&gt;AVERAGE(B25,C25),BSKW!$D$11:$D$30)),BSKW!$D$11:$D$30),1))</f>
-        <v>+III</v>
-      </c>
-      <c r="K25" s="12" t="str">
-        <f t="array" ref="K25">INDEX(HTKW!$K$11:$K$30,IFERROR(MATCH(MIN(IF(HTKW!$D$11:$D$30&gt;AVERAGE(B25,C25),HTKW!$D$11:$D$30)),HTKW!$D$11:$D$30),1))</f>
-        <v>+III</v>
-      </c>
-    </row>
-    <row r="26" spans="2:11" x14ac:dyDescent="0.25">
+        <f t="array" ref="J25">INDEX(STKWp!$K$11:$K$30,IFERROR(MATCH(MIN(IF(STKWp!$D$11:$D$30&gt;AVERAGE(B25,C25),STKWp!$D$11:$D$30)),STKWp!$D$11:$D$30),1))</f>
+        <v>+III</v>
+      </c>
+      <c r="K25" s="9" t="str">
+        <f t="array" ref="K25">INDEX(BSKW!$K$11:$K$30,IFERROR(MATCH(MIN(IF(BSKW!$D$11:$D$30&gt;AVERAGE(B25,C25),BSKW!$D$11:$D$30)),BSKW!$D$11:$D$30),1))</f>
+        <v>+III</v>
+      </c>
+      <c r="L25" s="12" t="str">
+        <f t="array" ref="L25">INDEX(HTKW!$K$11:$K$30,IFERROR(MATCH(MIN(IF(HTKW!$D$11:$D$30&gt;AVERAGE(B25,C25),HTKW!$D$11:$D$30)),HTKW!$D$11:$D$30),1))</f>
+        <v>+III</v>
+      </c>
+    </row>
+    <row r="26" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B26" s="8">
         <v>3.726</v>
       </c>
@@ -3452,36 +3551,40 @@
         <f t="shared" si="0"/>
         <v>+0</v>
       </c>
-      <c r="E26" s="9" t="str">
-        <f t="array" ref="E26">INDEX(STPH!$O$11:$O$30,IFERROR(MATCH(MIN(IF(STPH!$D$11:$D$30&gt;AVERAGE(B26,C26),STPH!$D$11:$D$30)),STPH!$D$11:$D$30),1))</f>
-        <v>+III</v>
+      <c r="E26" s="23" t="str">
+        <f t="shared" si="1"/>
+        <v>+0</v>
       </c>
       <c r="F26" s="9" t="str">
-        <f t="array" ref="F26">INDEX(STBI!$O$11:$O$30,IFERROR(MATCH(MIN(IF(STBI!$D$11:$D$30&gt;AVERAGE(B26,C26),STBI!$D$11:$D$30)),STBI!$D$11:$D$30),1))</f>
+        <f t="array" ref="F26">INDEX(STPH!$O$11:$O$30,IFERROR(MATCH(MIN(IF(STPH!$D$11:$D$30&gt;AVERAGE(B26,C26),STPH!$D$11:$D$30)),STPH!$D$11:$D$30),1))</f>
         <v>+III</v>
       </c>
       <c r="G26" s="9" t="str">
-        <f t="array" ref="G26">INDEX(GEKB!$K$11:$K$30,IFERROR(MATCH(MIN(IF(GEKB!$D$11:$D$30&gt;AVERAGE(B26,C26),GEKB!$D$11:$D$30)),GEKB!$D$11:$D$30),1))</f>
-        <v>+III</v>
-      </c>
-      <c r="H26" s="9">
-        <f t="array" ref="H26">INDEX(DA!$K$50:$K$71,IFERROR(MATCH(MIN(IF(DA!$D$50:$D$71&gt;AVERAGE(B26,C26),DA!$D$50:$D$71)),DA!$D$50:$D$71),1))</f>
-        <v>0</v>
-      </c>
-      <c r="I26" s="9" t="str">
-        <f t="array" ref="I26">INDEX(STKWp!$K$11:$K$30,IFERROR(MATCH(MIN(IF(STKWp!$D$11:$D$30&gt;AVERAGE(B26,C26),STKWp!$D$11:$D$30)),STKWp!$D$11:$D$30),1))</f>
-        <v>+III</v>
+        <f t="array" ref="G26">INDEX(STBI!$O$11:$O$30,IFERROR(MATCH(MIN(IF(STBI!$D$11:$D$30&gt;AVERAGE(B26,C26),STBI!$D$11:$D$30)),STBI!$D$11:$D$30),1))</f>
+        <v>+III</v>
+      </c>
+      <c r="H26" s="9" t="str">
+        <f t="array" ref="H26">INDEX(GEKB!$K$11:$K$30,IFERROR(MATCH(MIN(IF(GEKB!$D$11:$D$30&gt;AVERAGE(B26,C26),GEKB!$D$11:$D$30)),GEKB!$D$11:$D$30),1))</f>
+        <v>+III</v>
+      </c>
+      <c r="I26" s="9">
+        <f t="array" ref="I26">INDEX(DA!$K$50:$K$71,IFERROR(MATCH(MIN(IF(DA!$D$50:$D$71&gt;AVERAGE(B26,C26),DA!$D$50:$D$71)),DA!$D$50:$D$71),1))</f>
+        <v>0</v>
       </c>
       <c r="J26" s="9" t="str">
-        <f t="array" ref="J26">INDEX(BSKW!$K$11:$K$30,IFERROR(MATCH(MIN(IF(BSKW!$D$11:$D$30&gt;AVERAGE(B26,C26),BSKW!$D$11:$D$30)),BSKW!$D$11:$D$30),1))</f>
-        <v>+III</v>
-      </c>
-      <c r="K26" s="12" t="str">
-        <f t="array" ref="K26">INDEX(HTKW!$K$11:$K$30,IFERROR(MATCH(MIN(IF(HTKW!$D$11:$D$30&gt;AVERAGE(B26,C26),HTKW!$D$11:$D$30)),HTKW!$D$11:$D$30),1))</f>
-        <v>+III</v>
-      </c>
-    </row>
-    <row r="27" spans="2:11" x14ac:dyDescent="0.25">
+        <f t="array" ref="J26">INDEX(STKWp!$K$11:$K$30,IFERROR(MATCH(MIN(IF(STKWp!$D$11:$D$30&gt;AVERAGE(B26,C26),STKWp!$D$11:$D$30)),STKWp!$D$11:$D$30),1))</f>
+        <v>+III</v>
+      </c>
+      <c r="K26" s="9" t="str">
+        <f t="array" ref="K26">INDEX(BSKW!$K$11:$K$30,IFERROR(MATCH(MIN(IF(BSKW!$D$11:$D$30&gt;AVERAGE(B26,C26),BSKW!$D$11:$D$30)),BSKW!$D$11:$D$30),1))</f>
+        <v>+III</v>
+      </c>
+      <c r="L26" s="12" t="str">
+        <f t="array" ref="L26">INDEX(HTKW!$K$11:$K$30,IFERROR(MATCH(MIN(IF(HTKW!$D$11:$D$30&gt;AVERAGE(B26,C26),HTKW!$D$11:$D$30)),HTKW!$D$11:$D$30),1))</f>
+        <v>+III</v>
+      </c>
+    </row>
+    <row r="27" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B27" s="8">
         <v>3.8559999999999999</v>
       </c>
@@ -3492,36 +3595,40 @@
         <f t="shared" si="0"/>
         <v>+0</v>
       </c>
-      <c r="E27" s="9" t="str">
-        <f t="array" ref="E27">INDEX(STPH!$O$11:$O$30,IFERROR(MATCH(MIN(IF(STPH!$D$11:$D$30&gt;AVERAGE(B27,C27),STPH!$D$11:$D$30)),STPH!$D$11:$D$30),1))</f>
-        <v>+III</v>
+      <c r="E27" s="23" t="str">
+        <f t="shared" si="1"/>
+        <v>+0</v>
       </c>
       <c r="F27" s="9" t="str">
-        <f t="array" ref="F27">INDEX(STBI!$O$11:$O$30,IFERROR(MATCH(MIN(IF(STBI!$D$11:$D$30&gt;AVERAGE(B27,C27),STBI!$D$11:$D$30)),STBI!$D$11:$D$30),1))</f>
+        <f t="array" ref="F27">INDEX(STPH!$O$11:$O$30,IFERROR(MATCH(MIN(IF(STPH!$D$11:$D$30&gt;AVERAGE(B27,C27),STPH!$D$11:$D$30)),STPH!$D$11:$D$30),1))</f>
         <v>+III</v>
       </c>
       <c r="G27" s="9" t="str">
-        <f t="array" ref="G27">INDEX(GEKB!$K$11:$K$30,IFERROR(MATCH(MIN(IF(GEKB!$D$11:$D$30&gt;AVERAGE(B27,C27),GEKB!$D$11:$D$30)),GEKB!$D$11:$D$30),1))</f>
-        <v>+III</v>
-      </c>
-      <c r="H27" s="9">
-        <f t="array" ref="H27">INDEX(DA!$K$50:$K$71,IFERROR(MATCH(MIN(IF(DA!$D$50:$D$71&gt;AVERAGE(B27,C27),DA!$D$50:$D$71)),DA!$D$50:$D$71),1))</f>
-        <v>0</v>
-      </c>
-      <c r="I27" s="9" t="str">
-        <f t="array" ref="I27">INDEX(STKWp!$K$11:$K$30,IFERROR(MATCH(MIN(IF(STKWp!$D$11:$D$30&gt;AVERAGE(B27,C27),STKWp!$D$11:$D$30)),STKWp!$D$11:$D$30),1))</f>
-        <v>+III</v>
+        <f t="array" ref="G27">INDEX(STBI!$O$11:$O$30,IFERROR(MATCH(MIN(IF(STBI!$D$11:$D$30&gt;AVERAGE(B27,C27),STBI!$D$11:$D$30)),STBI!$D$11:$D$30),1))</f>
+        <v>+III</v>
+      </c>
+      <c r="H27" s="9" t="str">
+        <f t="array" ref="H27">INDEX(GEKB!$K$11:$K$30,IFERROR(MATCH(MIN(IF(GEKB!$D$11:$D$30&gt;AVERAGE(B27,C27),GEKB!$D$11:$D$30)),GEKB!$D$11:$D$30),1))</f>
+        <v>+III</v>
+      </c>
+      <c r="I27" s="9">
+        <f t="array" ref="I27">INDEX(DA!$K$50:$K$71,IFERROR(MATCH(MIN(IF(DA!$D$50:$D$71&gt;AVERAGE(B27,C27),DA!$D$50:$D$71)),DA!$D$50:$D$71),1))</f>
+        <v>0</v>
       </c>
       <c r="J27" s="9" t="str">
-        <f t="array" ref="J27">INDEX(BSKW!$K$11:$K$30,IFERROR(MATCH(MIN(IF(BSKW!$D$11:$D$30&gt;AVERAGE(B27,C27),BSKW!$D$11:$D$30)),BSKW!$D$11:$D$30),1))</f>
-        <v>+III</v>
-      </c>
-      <c r="K27" s="12" t="str">
-        <f t="array" ref="K27">INDEX(HTKW!$K$11:$K$30,IFERROR(MATCH(MIN(IF(HTKW!$D$11:$D$30&gt;AVERAGE(B27,C27),HTKW!$D$11:$D$30)),HTKW!$D$11:$D$30),1))</f>
-        <v>+III</v>
-      </c>
-    </row>
-    <row r="28" spans="2:11" x14ac:dyDescent="0.25">
+        <f t="array" ref="J27">INDEX(STKWp!$K$11:$K$30,IFERROR(MATCH(MIN(IF(STKWp!$D$11:$D$30&gt;AVERAGE(B27,C27),STKWp!$D$11:$D$30)),STKWp!$D$11:$D$30),1))</f>
+        <v>+III</v>
+      </c>
+      <c r="K27" s="9" t="str">
+        <f t="array" ref="K27">INDEX(BSKW!$K$11:$K$30,IFERROR(MATCH(MIN(IF(BSKW!$D$11:$D$30&gt;AVERAGE(B27,C27),BSKW!$D$11:$D$30)),BSKW!$D$11:$D$30),1))</f>
+        <v>+III</v>
+      </c>
+      <c r="L27" s="12" t="str">
+        <f t="array" ref="L27">INDEX(HTKW!$K$11:$K$30,IFERROR(MATCH(MIN(IF(HTKW!$D$11:$D$30&gt;AVERAGE(B27,C27),HTKW!$D$11:$D$30)),HTKW!$D$11:$D$30),1))</f>
+        <v>+III</v>
+      </c>
+    </row>
+    <row r="28" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B28" s="8">
         <v>3.9809999999999999</v>
       </c>
@@ -3532,36 +3639,40 @@
         <f t="shared" si="0"/>
         <v>+0</v>
       </c>
-      <c r="E28" s="9" t="str">
-        <f t="array" ref="E28">INDEX(STPH!$O$11:$O$30,IFERROR(MATCH(MIN(IF(STPH!$D$11:$D$30&gt;AVERAGE(B28,C28),STPH!$D$11:$D$30)),STPH!$D$11:$D$30),1))</f>
-        <v>+III</v>
+      <c r="E28" s="23" t="str">
+        <f t="shared" si="1"/>
+        <v>+0</v>
       </c>
       <c r="F28" s="9" t="str">
-        <f t="array" ref="F28">INDEX(STBI!$O$11:$O$30,IFERROR(MATCH(MIN(IF(STBI!$D$11:$D$30&gt;AVERAGE(B28,C28),STBI!$D$11:$D$30)),STBI!$D$11:$D$30),1))</f>
+        <f t="array" ref="F28">INDEX(STPH!$O$11:$O$30,IFERROR(MATCH(MIN(IF(STPH!$D$11:$D$30&gt;AVERAGE(B28,C28),STPH!$D$11:$D$30)),STPH!$D$11:$D$30),1))</f>
         <v>+III</v>
       </c>
       <c r="G28" s="9" t="str">
-        <f t="array" ref="G28">INDEX(GEKB!$K$11:$K$30,IFERROR(MATCH(MIN(IF(GEKB!$D$11:$D$30&gt;AVERAGE(B28,C28),GEKB!$D$11:$D$30)),GEKB!$D$11:$D$30),1))</f>
-        <v>+III</v>
-      </c>
-      <c r="H28" s="9">
-        <f t="array" ref="H28">INDEX(DA!$K$50:$K$71,IFERROR(MATCH(MIN(IF(DA!$D$50:$D$71&gt;AVERAGE(B28,C28),DA!$D$50:$D$71)),DA!$D$50:$D$71),1))</f>
-        <v>0</v>
-      </c>
-      <c r="I28" s="9" t="str">
-        <f t="array" ref="I28">INDEX(STKWp!$K$11:$K$30,IFERROR(MATCH(MIN(IF(STKWp!$D$11:$D$30&gt;AVERAGE(B28,C28),STKWp!$D$11:$D$30)),STKWp!$D$11:$D$30),1))</f>
-        <v>+III</v>
+        <f t="array" ref="G28">INDEX(STBI!$O$11:$O$30,IFERROR(MATCH(MIN(IF(STBI!$D$11:$D$30&gt;AVERAGE(B28,C28),STBI!$D$11:$D$30)),STBI!$D$11:$D$30),1))</f>
+        <v>+III</v>
+      </c>
+      <c r="H28" s="9" t="str">
+        <f t="array" ref="H28">INDEX(GEKB!$K$11:$K$30,IFERROR(MATCH(MIN(IF(GEKB!$D$11:$D$30&gt;AVERAGE(B28,C28),GEKB!$D$11:$D$30)),GEKB!$D$11:$D$30),1))</f>
+        <v>+III</v>
+      </c>
+      <c r="I28" s="9">
+        <f t="array" ref="I28">INDEX(DA!$K$50:$K$71,IFERROR(MATCH(MIN(IF(DA!$D$50:$D$71&gt;AVERAGE(B28,C28),DA!$D$50:$D$71)),DA!$D$50:$D$71),1))</f>
+        <v>0</v>
       </c>
       <c r="J28" s="9" t="str">
-        <f t="array" ref="J28">INDEX(BSKW!$K$11:$K$30,IFERROR(MATCH(MIN(IF(BSKW!$D$11:$D$30&gt;AVERAGE(B28,C28),BSKW!$D$11:$D$30)),BSKW!$D$11:$D$30),1))</f>
-        <v>+III</v>
-      </c>
-      <c r="K28" s="12" t="str">
-        <f t="array" ref="K28">INDEX(HTKW!$K$11:$K$30,IFERROR(MATCH(MIN(IF(HTKW!$D$11:$D$30&gt;AVERAGE(B28,C28),HTKW!$D$11:$D$30)),HTKW!$D$11:$D$30),1))</f>
-        <v>+III</v>
-      </c>
-    </row>
-    <row r="29" spans="2:11" x14ac:dyDescent="0.25">
+        <f t="array" ref="J28">INDEX(STKWp!$K$11:$K$30,IFERROR(MATCH(MIN(IF(STKWp!$D$11:$D$30&gt;AVERAGE(B28,C28),STKWp!$D$11:$D$30)),STKWp!$D$11:$D$30),1))</f>
+        <v>+III</v>
+      </c>
+      <c r="K28" s="9" t="str">
+        <f t="array" ref="K28">INDEX(BSKW!$K$11:$K$30,IFERROR(MATCH(MIN(IF(BSKW!$D$11:$D$30&gt;AVERAGE(B28,C28),BSKW!$D$11:$D$30)),BSKW!$D$11:$D$30),1))</f>
+        <v>+III</v>
+      </c>
+      <c r="L28" s="12" t="str">
+        <f t="array" ref="L28">INDEX(HTKW!$K$11:$K$30,IFERROR(MATCH(MIN(IF(HTKW!$D$11:$D$30&gt;AVERAGE(B28,C28),HTKW!$D$11:$D$30)),HTKW!$D$11:$D$30),1))</f>
+        <v>+III</v>
+      </c>
+    </row>
+    <row r="29" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B29" s="8">
         <v>4.1050000000000004</v>
       </c>
@@ -3572,36 +3683,40 @@
         <f t="shared" si="0"/>
         <v>+0</v>
       </c>
-      <c r="E29" s="9" t="str">
-        <f t="array" ref="E29">INDEX(STPH!$O$11:$O$30,IFERROR(MATCH(MIN(IF(STPH!$D$11:$D$30&gt;AVERAGE(B29,C29),STPH!$D$11:$D$30)),STPH!$D$11:$D$30),1))</f>
-        <v>+III</v>
+      <c r="E29" s="23" t="str">
+        <f t="shared" si="1"/>
+        <v>+0</v>
       </c>
       <c r="F29" s="9" t="str">
-        <f t="array" ref="F29">INDEX(STBI!$O$11:$O$30,IFERROR(MATCH(MIN(IF(STBI!$D$11:$D$30&gt;AVERAGE(B29,C29),STBI!$D$11:$D$30)),STBI!$D$11:$D$30),1))</f>
+        <f t="array" ref="F29">INDEX(STPH!$O$11:$O$30,IFERROR(MATCH(MIN(IF(STPH!$D$11:$D$30&gt;AVERAGE(B29,C29),STPH!$D$11:$D$30)),STPH!$D$11:$D$30),1))</f>
         <v>+III</v>
       </c>
       <c r="G29" s="9" t="str">
-        <f t="array" ref="G29">INDEX(GEKB!$K$11:$K$30,IFERROR(MATCH(MIN(IF(GEKB!$D$11:$D$30&gt;AVERAGE(B29,C29),GEKB!$D$11:$D$30)),GEKB!$D$11:$D$30),1))</f>
-        <v>+III</v>
-      </c>
-      <c r="H29" s="9">
-        <f t="array" ref="H29">INDEX(DA!$K$50:$K$71,IFERROR(MATCH(MIN(IF(DA!$D$50:$D$71&gt;AVERAGE(B29,C29),DA!$D$50:$D$71)),DA!$D$50:$D$71),1))</f>
-        <v>0</v>
-      </c>
-      <c r="I29" s="9" t="str">
-        <f t="array" ref="I29">INDEX(STKWp!$K$11:$K$30,IFERROR(MATCH(MIN(IF(STKWp!$D$11:$D$30&gt;AVERAGE(B29,C29),STKWp!$D$11:$D$30)),STKWp!$D$11:$D$30),1))</f>
-        <v>+III</v>
+        <f t="array" ref="G29">INDEX(STBI!$O$11:$O$30,IFERROR(MATCH(MIN(IF(STBI!$D$11:$D$30&gt;AVERAGE(B29,C29),STBI!$D$11:$D$30)),STBI!$D$11:$D$30),1))</f>
+        <v>+III</v>
+      </c>
+      <c r="H29" s="9" t="str">
+        <f t="array" ref="H29">INDEX(GEKB!$K$11:$K$30,IFERROR(MATCH(MIN(IF(GEKB!$D$11:$D$30&gt;AVERAGE(B29,C29),GEKB!$D$11:$D$30)),GEKB!$D$11:$D$30),1))</f>
+        <v>+III</v>
+      </c>
+      <c r="I29" s="9">
+        <f t="array" ref="I29">INDEX(DA!$K$50:$K$71,IFERROR(MATCH(MIN(IF(DA!$D$50:$D$71&gt;AVERAGE(B29,C29),DA!$D$50:$D$71)),DA!$D$50:$D$71),1))</f>
+        <v>0</v>
       </c>
       <c r="J29" s="9" t="str">
-        <f t="array" ref="J29">INDEX(BSKW!$K$11:$K$30,IFERROR(MATCH(MIN(IF(BSKW!$D$11:$D$30&gt;AVERAGE(B29,C29),BSKW!$D$11:$D$30)),BSKW!$D$11:$D$30),1))</f>
-        <v>+III</v>
-      </c>
-      <c r="K29" s="12" t="str">
-        <f t="array" ref="K29">INDEX(HTKW!$K$11:$K$30,IFERROR(MATCH(MIN(IF(HTKW!$D$11:$D$30&gt;AVERAGE(B29,C29),HTKW!$D$11:$D$30)),HTKW!$D$11:$D$30),1))</f>
-        <v>+III</v>
-      </c>
-    </row>
-    <row r="30" spans="2:11" x14ac:dyDescent="0.25">
+        <f t="array" ref="J29">INDEX(STKWp!$K$11:$K$30,IFERROR(MATCH(MIN(IF(STKWp!$D$11:$D$30&gt;AVERAGE(B29,C29),STKWp!$D$11:$D$30)),STKWp!$D$11:$D$30),1))</f>
+        <v>+III</v>
+      </c>
+      <c r="K29" s="9" t="str">
+        <f t="array" ref="K29">INDEX(BSKW!$K$11:$K$30,IFERROR(MATCH(MIN(IF(BSKW!$D$11:$D$30&gt;AVERAGE(B29,C29),BSKW!$D$11:$D$30)),BSKW!$D$11:$D$30),1))</f>
+        <v>+III</v>
+      </c>
+      <c r="L29" s="12" t="str">
+        <f t="array" ref="L29">INDEX(HTKW!$K$11:$K$30,IFERROR(MATCH(MIN(IF(HTKW!$D$11:$D$30&gt;AVERAGE(B29,C29),HTKW!$D$11:$D$30)),HTKW!$D$11:$D$30),1))</f>
+        <v>+III</v>
+      </c>
+    </row>
+    <row r="30" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B30" s="8">
         <v>4.2359999999999998</v>
       </c>
@@ -3612,36 +3727,40 @@
         <f t="shared" si="0"/>
         <v>+0</v>
       </c>
-      <c r="E30" s="9" t="str">
-        <f t="array" ref="E30">INDEX(STPH!$O$11:$O$30,IFERROR(MATCH(MIN(IF(STPH!$D$11:$D$30&gt;AVERAGE(B30,C30),STPH!$D$11:$D$30)),STPH!$D$11:$D$30),1))</f>
-        <v>+III</v>
+      <c r="E30" s="23" t="str">
+        <f t="shared" si="1"/>
+        <v>+0</v>
       </c>
       <c r="F30" s="9" t="str">
-        <f t="array" ref="F30">INDEX(STBI!$O$11:$O$30,IFERROR(MATCH(MIN(IF(STBI!$D$11:$D$30&gt;AVERAGE(B30,C30),STBI!$D$11:$D$30)),STBI!$D$11:$D$30),1))</f>
+        <f t="array" ref="F30">INDEX(STPH!$O$11:$O$30,IFERROR(MATCH(MIN(IF(STPH!$D$11:$D$30&gt;AVERAGE(B30,C30),STPH!$D$11:$D$30)),STPH!$D$11:$D$30),1))</f>
         <v>+III</v>
       </c>
       <c r="G30" s="9" t="str">
-        <f t="array" ref="G30">INDEX(GEKB!$K$11:$K$30,IFERROR(MATCH(MIN(IF(GEKB!$D$11:$D$30&gt;AVERAGE(B30,C30),GEKB!$D$11:$D$30)),GEKB!$D$11:$D$30),1))</f>
-        <v>+III</v>
-      </c>
-      <c r="H30" s="9">
-        <f t="array" ref="H30">INDEX(DA!$K$50:$K$71,IFERROR(MATCH(MIN(IF(DA!$D$50:$D$71&gt;AVERAGE(B30,C30),DA!$D$50:$D$71)),DA!$D$50:$D$71),1))</f>
-        <v>0</v>
-      </c>
-      <c r="I30" s="9" t="str">
-        <f t="array" ref="I30">INDEX(STKWp!$K$11:$K$30,IFERROR(MATCH(MIN(IF(STKWp!$D$11:$D$30&gt;AVERAGE(B30,C30),STKWp!$D$11:$D$30)),STKWp!$D$11:$D$30),1))</f>
-        <v>+III</v>
+        <f t="array" ref="G30">INDEX(STBI!$O$11:$O$30,IFERROR(MATCH(MIN(IF(STBI!$D$11:$D$30&gt;AVERAGE(B30,C30),STBI!$D$11:$D$30)),STBI!$D$11:$D$30),1))</f>
+        <v>+III</v>
+      </c>
+      <c r="H30" s="9" t="str">
+        <f t="array" ref="H30">INDEX(GEKB!$K$11:$K$30,IFERROR(MATCH(MIN(IF(GEKB!$D$11:$D$30&gt;AVERAGE(B30,C30),GEKB!$D$11:$D$30)),GEKB!$D$11:$D$30),1))</f>
+        <v>+III</v>
+      </c>
+      <c r="I30" s="9">
+        <f t="array" ref="I30">INDEX(DA!$K$50:$K$71,IFERROR(MATCH(MIN(IF(DA!$D$50:$D$71&gt;AVERAGE(B30,C30),DA!$D$50:$D$71)),DA!$D$50:$D$71),1))</f>
+        <v>0</v>
       </c>
       <c r="J30" s="9" t="str">
-        <f t="array" ref="J30">INDEX(BSKW!$K$11:$K$30,IFERROR(MATCH(MIN(IF(BSKW!$D$11:$D$30&gt;AVERAGE(B30,C30),BSKW!$D$11:$D$30)),BSKW!$D$11:$D$30),1))</f>
-        <v>+III</v>
-      </c>
-      <c r="K30" s="12" t="str">
-        <f t="array" ref="K30">INDEX(HTKW!$K$11:$K$30,IFERROR(MATCH(MIN(IF(HTKW!$D$11:$D$30&gt;AVERAGE(B30,C30),HTKW!$D$11:$D$30)),HTKW!$D$11:$D$30),1))</f>
-        <v>+III</v>
-      </c>
-    </row>
-    <row r="31" spans="2:11" x14ac:dyDescent="0.25">
+        <f t="array" ref="J30">INDEX(STKWp!$K$11:$K$30,IFERROR(MATCH(MIN(IF(STKWp!$D$11:$D$30&gt;AVERAGE(B30,C30),STKWp!$D$11:$D$30)),STKWp!$D$11:$D$30),1))</f>
+        <v>+III</v>
+      </c>
+      <c r="K30" s="9" t="str">
+        <f t="array" ref="K30">INDEX(BSKW!$K$11:$K$30,IFERROR(MATCH(MIN(IF(BSKW!$D$11:$D$30&gt;AVERAGE(B30,C30),BSKW!$D$11:$D$30)),BSKW!$D$11:$D$30),1))</f>
+        <v>+III</v>
+      </c>
+      <c r="L30" s="12" t="str">
+        <f t="array" ref="L30">INDEX(HTKW!$K$11:$K$30,IFERROR(MATCH(MIN(IF(HTKW!$D$11:$D$30&gt;AVERAGE(B30,C30),HTKW!$D$11:$D$30)),HTKW!$D$11:$D$30),1))</f>
+        <v>+III</v>
+      </c>
+    </row>
+    <row r="31" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B31" s="8">
         <v>4.38</v>
       </c>
@@ -3652,36 +3771,40 @@
         <f t="shared" si="0"/>
         <v>+0</v>
       </c>
-      <c r="E31" s="9" t="str">
-        <f t="array" ref="E31">INDEX(STPH!$O$11:$O$30,IFERROR(MATCH(MIN(IF(STPH!$D$11:$D$30&gt;AVERAGE(B31,C31),STPH!$D$11:$D$30)),STPH!$D$11:$D$30),1))</f>
-        <v>+III</v>
+      <c r="E31" s="23" t="str">
+        <f t="shared" si="1"/>
+        <v>+0</v>
       </c>
       <c r="F31" s="9" t="str">
-        <f t="array" ref="F31">INDEX(STBI!$O$11:$O$30,IFERROR(MATCH(MIN(IF(STBI!$D$11:$D$30&gt;AVERAGE(B31,C31),STBI!$D$11:$D$30)),STBI!$D$11:$D$30),1))</f>
+        <f t="array" ref="F31">INDEX(STPH!$O$11:$O$30,IFERROR(MATCH(MIN(IF(STPH!$D$11:$D$30&gt;AVERAGE(B31,C31),STPH!$D$11:$D$30)),STPH!$D$11:$D$30),1))</f>
         <v>+III</v>
       </c>
       <c r="G31" s="9" t="str">
-        <f t="array" ref="G31">INDEX(GEKB!$K$11:$K$30,IFERROR(MATCH(MIN(IF(GEKB!$D$11:$D$30&gt;AVERAGE(B31,C31),GEKB!$D$11:$D$30)),GEKB!$D$11:$D$30),1))</f>
-        <v>+III</v>
-      </c>
-      <c r="H31" s="9">
-        <f t="array" ref="H31">INDEX(DA!$K$50:$K$71,IFERROR(MATCH(MIN(IF(DA!$D$50:$D$71&gt;AVERAGE(B31,C31),DA!$D$50:$D$71)),DA!$D$50:$D$71),1))</f>
-        <v>0</v>
-      </c>
-      <c r="I31" s="9" t="str">
-        <f t="array" ref="I31">INDEX(STKWp!$K$11:$K$30,IFERROR(MATCH(MIN(IF(STKWp!$D$11:$D$30&gt;AVERAGE(B31,C31),STKWp!$D$11:$D$30)),STKWp!$D$11:$D$30),1))</f>
-        <v>+III</v>
+        <f t="array" ref="G31">INDEX(STBI!$O$11:$O$30,IFERROR(MATCH(MIN(IF(STBI!$D$11:$D$30&gt;AVERAGE(B31,C31),STBI!$D$11:$D$30)),STBI!$D$11:$D$30),1))</f>
+        <v>+III</v>
+      </c>
+      <c r="H31" s="9" t="str">
+        <f t="array" ref="H31">INDEX(GEKB!$K$11:$K$30,IFERROR(MATCH(MIN(IF(GEKB!$D$11:$D$30&gt;AVERAGE(B31,C31),GEKB!$D$11:$D$30)),GEKB!$D$11:$D$30),1))</f>
+        <v>+III</v>
+      </c>
+      <c r="I31" s="9">
+        <f t="array" ref="I31">INDEX(DA!$K$50:$K$71,IFERROR(MATCH(MIN(IF(DA!$D$50:$D$71&gt;AVERAGE(B31,C31),DA!$D$50:$D$71)),DA!$D$50:$D$71),1))</f>
+        <v>0</v>
       </c>
       <c r="J31" s="9" t="str">
-        <f t="array" ref="J31">INDEX(BSKW!$K$11:$K$30,IFERROR(MATCH(MIN(IF(BSKW!$D$11:$D$30&gt;AVERAGE(B31,C31),BSKW!$D$11:$D$30)),BSKW!$D$11:$D$30),1))</f>
-        <v>+III</v>
-      </c>
-      <c r="K31" s="12" t="str">
-        <f t="array" ref="K31">INDEX(HTKW!$K$11:$K$30,IFERROR(MATCH(MIN(IF(HTKW!$D$11:$D$30&gt;AVERAGE(B31,C31),HTKW!$D$11:$D$30)),HTKW!$D$11:$D$30),1))</f>
-        <v>+III</v>
-      </c>
-    </row>
-    <row r="32" spans="2:11" x14ac:dyDescent="0.25">
+        <f t="array" ref="J31">INDEX(STKWp!$K$11:$K$30,IFERROR(MATCH(MIN(IF(STKWp!$D$11:$D$30&gt;AVERAGE(B31,C31),STKWp!$D$11:$D$30)),STKWp!$D$11:$D$30),1))</f>
+        <v>+III</v>
+      </c>
+      <c r="K31" s="9" t="str">
+        <f t="array" ref="K31">INDEX(BSKW!$K$11:$K$30,IFERROR(MATCH(MIN(IF(BSKW!$D$11:$D$30&gt;AVERAGE(B31,C31),BSKW!$D$11:$D$30)),BSKW!$D$11:$D$30),1))</f>
+        <v>+III</v>
+      </c>
+      <c r="L31" s="12" t="str">
+        <f t="array" ref="L31">INDEX(HTKW!$K$11:$K$30,IFERROR(MATCH(MIN(IF(HTKW!$D$11:$D$30&gt;AVERAGE(B31,C31),HTKW!$D$11:$D$30)),HTKW!$D$11:$D$30),1))</f>
+        <v>+III</v>
+      </c>
+    </row>
+    <row r="32" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B32" s="8">
         <v>4.5129999999999999</v>
       </c>
@@ -3692,36 +3815,40 @@
         <f t="shared" si="0"/>
         <v>+0</v>
       </c>
-      <c r="E32" s="9" t="str">
-        <f t="array" ref="E32">INDEX(STPH!$O$11:$O$30,IFERROR(MATCH(MIN(IF(STPH!$D$11:$D$30&gt;AVERAGE(B32,C32),STPH!$D$11:$D$30)),STPH!$D$11:$D$30),1))</f>
-        <v>+III</v>
+      <c r="E32" s="23" t="str">
+        <f t="shared" si="1"/>
+        <v>+0</v>
       </c>
       <c r="F32" s="9" t="str">
-        <f t="array" ref="F32">INDEX(STBI!$O$11:$O$30,IFERROR(MATCH(MIN(IF(STBI!$D$11:$D$30&gt;AVERAGE(B32,C32),STBI!$D$11:$D$30)),STBI!$D$11:$D$30),1))</f>
+        <f t="array" ref="F32">INDEX(STPH!$O$11:$O$30,IFERROR(MATCH(MIN(IF(STPH!$D$11:$D$30&gt;AVERAGE(B32,C32),STPH!$D$11:$D$30)),STPH!$D$11:$D$30),1))</f>
         <v>+III</v>
       </c>
       <c r="G32" s="9" t="str">
-        <f t="array" ref="G32">INDEX(GEKB!$K$11:$K$30,IFERROR(MATCH(MIN(IF(GEKB!$D$11:$D$30&gt;AVERAGE(B32,C32),GEKB!$D$11:$D$30)),GEKB!$D$11:$D$30),1))</f>
-        <v>+III</v>
-      </c>
-      <c r="H32" s="9">
-        <f t="array" ref="H32">INDEX(DA!$K$50:$K$71,IFERROR(MATCH(MIN(IF(DA!$D$50:$D$71&gt;AVERAGE(B32,C32),DA!$D$50:$D$71)),DA!$D$50:$D$71),1))</f>
-        <v>0</v>
-      </c>
-      <c r="I32" s="9" t="str">
-        <f t="array" ref="I32">INDEX(STKWp!$K$11:$K$30,IFERROR(MATCH(MIN(IF(STKWp!$D$11:$D$30&gt;AVERAGE(B32,C32),STKWp!$D$11:$D$30)),STKWp!$D$11:$D$30),1))</f>
-        <v>+III</v>
+        <f t="array" ref="G32">INDEX(STBI!$O$11:$O$30,IFERROR(MATCH(MIN(IF(STBI!$D$11:$D$30&gt;AVERAGE(B32,C32),STBI!$D$11:$D$30)),STBI!$D$11:$D$30),1))</f>
+        <v>+III</v>
+      </c>
+      <c r="H32" s="9" t="str">
+        <f t="array" ref="H32">INDEX(GEKB!$K$11:$K$30,IFERROR(MATCH(MIN(IF(GEKB!$D$11:$D$30&gt;AVERAGE(B32,C32),GEKB!$D$11:$D$30)),GEKB!$D$11:$D$30),1))</f>
+        <v>+III</v>
+      </c>
+      <c r="I32" s="9">
+        <f t="array" ref="I32">INDEX(DA!$K$50:$K$71,IFERROR(MATCH(MIN(IF(DA!$D$50:$D$71&gt;AVERAGE(B32,C32),DA!$D$50:$D$71)),DA!$D$50:$D$71),1))</f>
+        <v>0</v>
       </c>
       <c r="J32" s="9" t="str">
-        <f t="array" ref="J32">INDEX(BSKW!$K$11:$K$30,IFERROR(MATCH(MIN(IF(BSKW!$D$11:$D$30&gt;AVERAGE(B32,C32),BSKW!$D$11:$D$30)),BSKW!$D$11:$D$30),1))</f>
-        <v>+III</v>
-      </c>
-      <c r="K32" s="12" t="str">
-        <f t="array" ref="K32">INDEX(HTKW!$K$11:$K$30,IFERROR(MATCH(MIN(IF(HTKW!$D$11:$D$30&gt;AVERAGE(B32,C32),HTKW!$D$11:$D$30)),HTKW!$D$11:$D$30),1))</f>
-        <v>+III</v>
-      </c>
-    </row>
-    <row r="33" spans="2:11" x14ac:dyDescent="0.25">
+        <f t="array" ref="J32">INDEX(STKWp!$K$11:$K$30,IFERROR(MATCH(MIN(IF(STKWp!$D$11:$D$30&gt;AVERAGE(B32,C32),STKWp!$D$11:$D$30)),STKWp!$D$11:$D$30),1))</f>
+        <v>+III</v>
+      </c>
+      <c r="K32" s="9" t="str">
+        <f t="array" ref="K32">INDEX(BSKW!$K$11:$K$30,IFERROR(MATCH(MIN(IF(BSKW!$D$11:$D$30&gt;AVERAGE(B32,C32),BSKW!$D$11:$D$30)),BSKW!$D$11:$D$30),1))</f>
+        <v>+III</v>
+      </c>
+      <c r="L32" s="12" t="str">
+        <f t="array" ref="L32">INDEX(HTKW!$K$11:$K$30,IFERROR(MATCH(MIN(IF(HTKW!$D$11:$D$30&gt;AVERAGE(B32,C32),HTKW!$D$11:$D$30)),HTKW!$D$11:$D$30),1))</f>
+        <v>+III</v>
+      </c>
+    </row>
+    <row r="33" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B33" s="8">
         <v>4.6340000000000003</v>
       </c>
@@ -3732,36 +3859,40 @@
         <f t="shared" si="0"/>
         <v>+0</v>
       </c>
-      <c r="E33" s="9" t="str">
-        <f t="array" ref="E33">INDEX(STPH!$O$11:$O$30,IFERROR(MATCH(MIN(IF(STPH!$D$11:$D$30&gt;AVERAGE(B33,C33),STPH!$D$11:$D$30)),STPH!$D$11:$D$30),1))</f>
-        <v>+III</v>
+      <c r="E33" s="23" t="str">
+        <f t="shared" si="1"/>
+        <v>+0</v>
       </c>
       <c r="F33" s="9" t="str">
-        <f t="array" ref="F33">INDEX(STBI!$O$11:$O$30,IFERROR(MATCH(MIN(IF(STBI!$D$11:$D$30&gt;AVERAGE(B33,C33),STBI!$D$11:$D$30)),STBI!$D$11:$D$30),1))</f>
+        <f t="array" ref="F33">INDEX(STPH!$O$11:$O$30,IFERROR(MATCH(MIN(IF(STPH!$D$11:$D$30&gt;AVERAGE(B33,C33),STPH!$D$11:$D$30)),STPH!$D$11:$D$30),1))</f>
         <v>+III</v>
       </c>
       <c r="G33" s="9" t="str">
-        <f t="array" ref="G33">INDEX(GEKB!$K$11:$K$30,IFERROR(MATCH(MIN(IF(GEKB!$D$11:$D$30&gt;AVERAGE(B33,C33),GEKB!$D$11:$D$30)),GEKB!$D$11:$D$30),1))</f>
-        <v>+III</v>
-      </c>
-      <c r="H33" s="9">
-        <f t="array" ref="H33">INDEX(DA!$K$50:$K$71,IFERROR(MATCH(MIN(IF(DA!$D$50:$D$71&gt;AVERAGE(B33,C33),DA!$D$50:$D$71)),DA!$D$50:$D$71),1))</f>
-        <v>0</v>
-      </c>
-      <c r="I33" s="9" t="str">
-        <f t="array" ref="I33">INDEX(STKWp!$K$11:$K$30,IFERROR(MATCH(MIN(IF(STKWp!$D$11:$D$30&gt;AVERAGE(B33,C33),STKWp!$D$11:$D$30)),STKWp!$D$11:$D$30),1))</f>
-        <v>+III</v>
+        <f t="array" ref="G33">INDEX(STBI!$O$11:$O$30,IFERROR(MATCH(MIN(IF(STBI!$D$11:$D$30&gt;AVERAGE(B33,C33),STBI!$D$11:$D$30)),STBI!$D$11:$D$30),1))</f>
+        <v>+III</v>
+      </c>
+      <c r="H33" s="9" t="str">
+        <f t="array" ref="H33">INDEX(GEKB!$K$11:$K$30,IFERROR(MATCH(MIN(IF(GEKB!$D$11:$D$30&gt;AVERAGE(B33,C33),GEKB!$D$11:$D$30)),GEKB!$D$11:$D$30),1))</f>
+        <v>+III</v>
+      </c>
+      <c r="I33" s="9">
+        <f t="array" ref="I33">INDEX(DA!$K$50:$K$71,IFERROR(MATCH(MIN(IF(DA!$D$50:$D$71&gt;AVERAGE(B33,C33),DA!$D$50:$D$71)),DA!$D$50:$D$71),1))</f>
+        <v>0</v>
       </c>
       <c r="J33" s="9" t="str">
-        <f t="array" ref="J33">INDEX(BSKW!$K$11:$K$30,IFERROR(MATCH(MIN(IF(BSKW!$D$11:$D$30&gt;AVERAGE(B33,C33),BSKW!$D$11:$D$30)),BSKW!$D$11:$D$30),1))</f>
-        <v>+III</v>
-      </c>
-      <c r="K33" s="12" t="str">
-        <f t="array" ref="K33">INDEX(HTKW!$K$11:$K$30,IFERROR(MATCH(MIN(IF(HTKW!$D$11:$D$30&gt;AVERAGE(B33,C33),HTKW!$D$11:$D$30)),HTKW!$D$11:$D$30),1))</f>
-        <v>+III</v>
-      </c>
-    </row>
-    <row r="34" spans="2:11" x14ac:dyDescent="0.25">
+        <f t="array" ref="J33">INDEX(STKWp!$K$11:$K$30,IFERROR(MATCH(MIN(IF(STKWp!$D$11:$D$30&gt;AVERAGE(B33,C33),STKWp!$D$11:$D$30)),STKWp!$D$11:$D$30),1))</f>
+        <v>+III</v>
+      </c>
+      <c r="K33" s="9" t="str">
+        <f t="array" ref="K33">INDEX(BSKW!$K$11:$K$30,IFERROR(MATCH(MIN(IF(BSKW!$D$11:$D$30&gt;AVERAGE(B33,C33),BSKW!$D$11:$D$30)),BSKW!$D$11:$D$30),1))</f>
+        <v>+III</v>
+      </c>
+      <c r="L33" s="12" t="str">
+        <f t="array" ref="L33">INDEX(HTKW!$K$11:$K$30,IFERROR(MATCH(MIN(IF(HTKW!$D$11:$D$30&gt;AVERAGE(B33,C33),HTKW!$D$11:$D$30)),HTKW!$D$11:$D$30),1))</f>
+        <v>+III</v>
+      </c>
+    </row>
+    <row r="34" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B34" s="8">
         <v>4.7480000000000002</v>
       </c>
@@ -3772,36 +3903,40 @@
         <f t="shared" si="0"/>
         <v>+0</v>
       </c>
-      <c r="E34" s="9" t="str">
-        <f t="array" ref="E34">INDEX(STPH!$O$11:$O$30,IFERROR(MATCH(MIN(IF(STPH!$D$11:$D$30&gt;AVERAGE(B34,C34),STPH!$D$11:$D$30)),STPH!$D$11:$D$30),1))</f>
-        <v>+III</v>
+      <c r="E34" s="23" t="str">
+        <f t="shared" si="1"/>
+        <v>+0</v>
       </c>
       <c r="F34" s="9" t="str">
-        <f t="array" ref="F34">INDEX(STBI!$O$11:$O$30,IFERROR(MATCH(MIN(IF(STBI!$D$11:$D$30&gt;AVERAGE(B34,C34),STBI!$D$11:$D$30)),STBI!$D$11:$D$30),1))</f>
+        <f t="array" ref="F34">INDEX(STPH!$O$11:$O$30,IFERROR(MATCH(MIN(IF(STPH!$D$11:$D$30&gt;AVERAGE(B34,C34),STPH!$D$11:$D$30)),STPH!$D$11:$D$30),1))</f>
         <v>+III</v>
       </c>
       <c r="G34" s="9" t="str">
-        <f t="array" ref="G34">INDEX(GEKB!$K$11:$K$30,IFERROR(MATCH(MIN(IF(GEKB!$D$11:$D$30&gt;AVERAGE(B34,C34),GEKB!$D$11:$D$30)),GEKB!$D$11:$D$30),1))</f>
-        <v>+III</v>
-      </c>
-      <c r="H34" s="9">
-        <f t="array" ref="H34">INDEX(DA!$K$50:$K$71,IFERROR(MATCH(MIN(IF(DA!$D$50:$D$71&gt;AVERAGE(B34,C34),DA!$D$50:$D$71)),DA!$D$50:$D$71),1))</f>
-        <v>0</v>
-      </c>
-      <c r="I34" s="9" t="str">
-        <f t="array" ref="I34">INDEX(STKWp!$K$11:$K$30,IFERROR(MATCH(MIN(IF(STKWp!$D$11:$D$30&gt;AVERAGE(B34,C34),STKWp!$D$11:$D$30)),STKWp!$D$11:$D$30),1))</f>
-        <v>+III</v>
+        <f t="array" ref="G34">INDEX(STBI!$O$11:$O$30,IFERROR(MATCH(MIN(IF(STBI!$D$11:$D$30&gt;AVERAGE(B34,C34),STBI!$D$11:$D$30)),STBI!$D$11:$D$30),1))</f>
+        <v>+III</v>
+      </c>
+      <c r="H34" s="9" t="str">
+        <f t="array" ref="H34">INDEX(GEKB!$K$11:$K$30,IFERROR(MATCH(MIN(IF(GEKB!$D$11:$D$30&gt;AVERAGE(B34,C34),GEKB!$D$11:$D$30)),GEKB!$D$11:$D$30),1))</f>
+        <v>+III</v>
+      </c>
+      <c r="I34" s="9">
+        <f t="array" ref="I34">INDEX(DA!$K$50:$K$71,IFERROR(MATCH(MIN(IF(DA!$D$50:$D$71&gt;AVERAGE(B34,C34),DA!$D$50:$D$71)),DA!$D$50:$D$71),1))</f>
+        <v>0</v>
       </c>
       <c r="J34" s="9" t="str">
-        <f t="array" ref="J34">INDEX(BSKW!$K$11:$K$30,IFERROR(MATCH(MIN(IF(BSKW!$D$11:$D$30&gt;AVERAGE(B34,C34),BSKW!$D$11:$D$30)),BSKW!$D$11:$D$30),1))</f>
-        <v>+III</v>
-      </c>
-      <c r="K34" s="12" t="str">
-        <f t="array" ref="K34">INDEX(HTKW!$K$11:$K$30,IFERROR(MATCH(MIN(IF(HTKW!$D$11:$D$30&gt;AVERAGE(B34,C34),HTKW!$D$11:$D$30)),HTKW!$D$11:$D$30),1))</f>
-        <v>+III</v>
-      </c>
-    </row>
-    <row r="35" spans="2:11" x14ac:dyDescent="0.25">
+        <f t="array" ref="J34">INDEX(STKWp!$K$11:$K$30,IFERROR(MATCH(MIN(IF(STKWp!$D$11:$D$30&gt;AVERAGE(B34,C34),STKWp!$D$11:$D$30)),STKWp!$D$11:$D$30),1))</f>
+        <v>+III</v>
+      </c>
+      <c r="K34" s="9" t="str">
+        <f t="array" ref="K34">INDEX(BSKW!$K$11:$K$30,IFERROR(MATCH(MIN(IF(BSKW!$D$11:$D$30&gt;AVERAGE(B34,C34),BSKW!$D$11:$D$30)),BSKW!$D$11:$D$30),1))</f>
+        <v>+III</v>
+      </c>
+      <c r="L34" s="12" t="str">
+        <f t="array" ref="L34">INDEX(HTKW!$K$11:$K$30,IFERROR(MATCH(MIN(IF(HTKW!$D$11:$D$30&gt;AVERAGE(B34,C34),HTKW!$D$11:$D$30)),HTKW!$D$11:$D$30),1))</f>
+        <v>+III</v>
+      </c>
+    </row>
+    <row r="35" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B35" s="8">
         <v>4.8609999999999998</v>
       </c>
@@ -3812,36 +3947,40 @@
         <f t="shared" si="0"/>
         <v>+0</v>
       </c>
-      <c r="E35" s="9" t="str">
-        <f t="array" ref="E35">INDEX(STPH!$O$11:$O$30,IFERROR(MATCH(MIN(IF(STPH!$D$11:$D$30&gt;AVERAGE(B35,C35),STPH!$D$11:$D$30)),STPH!$D$11:$D$30),1))</f>
-        <v>+III</v>
+      <c r="E35" s="23" t="str">
+        <f t="shared" si="1"/>
+        <v>+0</v>
       </c>
       <c r="F35" s="9" t="str">
-        <f t="array" ref="F35">INDEX(STBI!$O$11:$O$30,IFERROR(MATCH(MIN(IF(STBI!$D$11:$D$30&gt;AVERAGE(B35,C35),STBI!$D$11:$D$30)),STBI!$D$11:$D$30),1))</f>
+        <f t="array" ref="F35">INDEX(STPH!$O$11:$O$30,IFERROR(MATCH(MIN(IF(STPH!$D$11:$D$30&gt;AVERAGE(B35,C35),STPH!$D$11:$D$30)),STPH!$D$11:$D$30),1))</f>
         <v>+III</v>
       </c>
       <c r="G35" s="9" t="str">
-        <f t="array" ref="G35">INDEX(GEKB!$K$11:$K$30,IFERROR(MATCH(MIN(IF(GEKB!$D$11:$D$30&gt;AVERAGE(B35,C35),GEKB!$D$11:$D$30)),GEKB!$D$11:$D$30),1))</f>
-        <v>+III</v>
-      </c>
-      <c r="H35" s="9">
-        <f t="array" ref="H35">INDEX(DA!$K$50:$K$71,IFERROR(MATCH(MIN(IF(DA!$D$50:$D$71&gt;AVERAGE(B35,C35),DA!$D$50:$D$71)),DA!$D$50:$D$71),1))</f>
-        <v>0</v>
-      </c>
-      <c r="I35" s="9" t="str">
-        <f t="array" ref="I35">INDEX(STKWp!$K$11:$K$30,IFERROR(MATCH(MIN(IF(STKWp!$D$11:$D$30&gt;AVERAGE(B35,C35),STKWp!$D$11:$D$30)),STKWp!$D$11:$D$30),1))</f>
-        <v>+III</v>
+        <f t="array" ref="G35">INDEX(STBI!$O$11:$O$30,IFERROR(MATCH(MIN(IF(STBI!$D$11:$D$30&gt;AVERAGE(B35,C35),STBI!$D$11:$D$30)),STBI!$D$11:$D$30),1))</f>
+        <v>+III</v>
+      </c>
+      <c r="H35" s="9" t="str">
+        <f t="array" ref="H35">INDEX(GEKB!$K$11:$K$30,IFERROR(MATCH(MIN(IF(GEKB!$D$11:$D$30&gt;AVERAGE(B35,C35),GEKB!$D$11:$D$30)),GEKB!$D$11:$D$30),1))</f>
+        <v>+III</v>
+      </c>
+      <c r="I35" s="9">
+        <f t="array" ref="I35">INDEX(DA!$K$50:$K$71,IFERROR(MATCH(MIN(IF(DA!$D$50:$D$71&gt;AVERAGE(B35,C35),DA!$D$50:$D$71)),DA!$D$50:$D$71),1))</f>
+        <v>0</v>
       </c>
       <c r="J35" s="9" t="str">
-        <f t="array" ref="J35">INDEX(BSKW!$K$11:$K$30,IFERROR(MATCH(MIN(IF(BSKW!$D$11:$D$30&gt;AVERAGE(B35,C35),BSKW!$D$11:$D$30)),BSKW!$D$11:$D$30),1))</f>
-        <v>+III</v>
-      </c>
-      <c r="K35" s="12" t="str">
-        <f t="array" ref="K35">INDEX(HTKW!$K$11:$K$30,IFERROR(MATCH(MIN(IF(HTKW!$D$11:$D$30&gt;AVERAGE(B35,C35),HTKW!$D$11:$D$30)),HTKW!$D$11:$D$30),1))</f>
-        <v>+III</v>
-      </c>
-    </row>
-    <row r="36" spans="2:11" x14ac:dyDescent="0.25">
+        <f t="array" ref="J35">INDEX(STKWp!$K$11:$K$30,IFERROR(MATCH(MIN(IF(STKWp!$D$11:$D$30&gt;AVERAGE(B35,C35),STKWp!$D$11:$D$30)),STKWp!$D$11:$D$30),1))</f>
+        <v>+III</v>
+      </c>
+      <c r="K35" s="9" t="str">
+        <f t="array" ref="K35">INDEX(BSKW!$K$11:$K$30,IFERROR(MATCH(MIN(IF(BSKW!$D$11:$D$30&gt;AVERAGE(B35,C35),BSKW!$D$11:$D$30)),BSKW!$D$11:$D$30),1))</f>
+        <v>+III</v>
+      </c>
+      <c r="L35" s="12" t="str">
+        <f t="array" ref="L35">INDEX(HTKW!$K$11:$K$30,IFERROR(MATCH(MIN(IF(HTKW!$D$11:$D$30&gt;AVERAGE(B35,C35),HTKW!$D$11:$D$30)),HTKW!$D$11:$D$30),1))</f>
+        <v>+III</v>
+      </c>
+    </row>
+    <row r="36" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B36" s="8">
         <v>4.9749999999999996</v>
       </c>
@@ -3852,36 +3991,40 @@
         <f t="shared" si="0"/>
         <v>+0</v>
       </c>
-      <c r="E36" s="9" t="str">
-        <f t="array" ref="E36">INDEX(STPH!$O$11:$O$30,IFERROR(MATCH(MIN(IF(STPH!$D$11:$D$30&gt;AVERAGE(B36,C36),STPH!$D$11:$D$30)),STPH!$D$11:$D$30),1))</f>
-        <v>+III</v>
+      <c r="E36" s="23" t="str">
+        <f t="shared" si="1"/>
+        <v>+0</v>
       </c>
       <c r="F36" s="9" t="str">
-        <f t="array" ref="F36">INDEX(STBI!$O$11:$O$30,IFERROR(MATCH(MIN(IF(STBI!$D$11:$D$30&gt;AVERAGE(B36,C36),STBI!$D$11:$D$30)),STBI!$D$11:$D$30),1))</f>
+        <f t="array" ref="F36">INDEX(STPH!$O$11:$O$30,IFERROR(MATCH(MIN(IF(STPH!$D$11:$D$30&gt;AVERAGE(B36,C36),STPH!$D$11:$D$30)),STPH!$D$11:$D$30),1))</f>
         <v>+III</v>
       </c>
       <c r="G36" s="9" t="str">
-        <f t="array" ref="G36">INDEX(GEKB!$K$11:$K$30,IFERROR(MATCH(MIN(IF(GEKB!$D$11:$D$30&gt;AVERAGE(B36,C36),GEKB!$D$11:$D$30)),GEKB!$D$11:$D$30),1))</f>
-        <v>+III</v>
-      </c>
-      <c r="H36" s="9">
-        <f t="array" ref="H36">INDEX(DA!$K$50:$K$71,IFERROR(MATCH(MIN(IF(DA!$D$50:$D$71&gt;AVERAGE(B36,C36),DA!$D$50:$D$71)),DA!$D$50:$D$71),1))</f>
-        <v>0</v>
-      </c>
-      <c r="I36" s="9" t="str">
-        <f t="array" ref="I36">INDEX(STKWp!$K$11:$K$30,IFERROR(MATCH(MIN(IF(STKWp!$D$11:$D$30&gt;AVERAGE(B36,C36),STKWp!$D$11:$D$30)),STKWp!$D$11:$D$30),1))</f>
-        <v>+III</v>
+        <f t="array" ref="G36">INDEX(STBI!$O$11:$O$30,IFERROR(MATCH(MIN(IF(STBI!$D$11:$D$30&gt;AVERAGE(B36,C36),STBI!$D$11:$D$30)),STBI!$D$11:$D$30),1))</f>
+        <v>+III</v>
+      </c>
+      <c r="H36" s="9" t="str">
+        <f t="array" ref="H36">INDEX(GEKB!$K$11:$K$30,IFERROR(MATCH(MIN(IF(GEKB!$D$11:$D$30&gt;AVERAGE(B36,C36),GEKB!$D$11:$D$30)),GEKB!$D$11:$D$30),1))</f>
+        <v>+III</v>
+      </c>
+      <c r="I36" s="9">
+        <f t="array" ref="I36">INDEX(DA!$K$50:$K$71,IFERROR(MATCH(MIN(IF(DA!$D$50:$D$71&gt;AVERAGE(B36,C36),DA!$D$50:$D$71)),DA!$D$50:$D$71),1))</f>
+        <v>0</v>
       </c>
       <c r="J36" s="9" t="str">
-        <f t="array" ref="J36">INDEX(BSKW!$K$11:$K$30,IFERROR(MATCH(MIN(IF(BSKW!$D$11:$D$30&gt;AVERAGE(B36,C36),BSKW!$D$11:$D$30)),BSKW!$D$11:$D$30),1))</f>
-        <v>+III</v>
-      </c>
-      <c r="K36" s="12" t="str">
-        <f t="array" ref="K36">INDEX(HTKW!$K$11:$K$30,IFERROR(MATCH(MIN(IF(HTKW!$D$11:$D$30&gt;AVERAGE(B36,C36),HTKW!$D$11:$D$30)),HTKW!$D$11:$D$30),1))</f>
-        <v>+III</v>
-      </c>
-    </row>
-    <row r="37" spans="2:11" x14ac:dyDescent="0.25">
+        <f t="array" ref="J36">INDEX(STKWp!$K$11:$K$30,IFERROR(MATCH(MIN(IF(STKWp!$D$11:$D$30&gt;AVERAGE(B36,C36),STKWp!$D$11:$D$30)),STKWp!$D$11:$D$30),1))</f>
+        <v>+III</v>
+      </c>
+      <c r="K36" s="9" t="str">
+        <f t="array" ref="K36">INDEX(BSKW!$K$11:$K$30,IFERROR(MATCH(MIN(IF(BSKW!$D$11:$D$30&gt;AVERAGE(B36,C36),BSKW!$D$11:$D$30)),BSKW!$D$11:$D$30),1))</f>
+        <v>+III</v>
+      </c>
+      <c r="L36" s="12" t="str">
+        <f t="array" ref="L36">INDEX(HTKW!$K$11:$K$30,IFERROR(MATCH(MIN(IF(HTKW!$D$11:$D$30&gt;AVERAGE(B36,C36),HTKW!$D$11:$D$30)),HTKW!$D$11:$D$30),1))</f>
+        <v>+III</v>
+      </c>
+    </row>
+    <row r="37" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B37" s="8">
         <v>5.0910000000000002</v>
       </c>
@@ -3892,36 +4035,40 @@
         <f t="shared" si="0"/>
         <v>+0</v>
       </c>
-      <c r="E37" s="9" t="str">
-        <f t="array" ref="E37">INDEX(STPH!$O$11:$O$30,IFERROR(MATCH(MIN(IF(STPH!$D$11:$D$30&gt;AVERAGE(B37,C37),STPH!$D$11:$D$30)),STPH!$D$11:$D$30),1))</f>
-        <v>+III</v>
+      <c r="E37" s="23" t="str">
+        <f t="shared" si="1"/>
+        <v>+0</v>
       </c>
       <c r="F37" s="9" t="str">
-        <f t="array" ref="F37">INDEX(STBI!$O$11:$O$30,IFERROR(MATCH(MIN(IF(STBI!$D$11:$D$30&gt;AVERAGE(B37,C37),STBI!$D$11:$D$30)),STBI!$D$11:$D$30),1))</f>
+        <f t="array" ref="F37">INDEX(STPH!$O$11:$O$30,IFERROR(MATCH(MIN(IF(STPH!$D$11:$D$30&gt;AVERAGE(B37,C37),STPH!$D$11:$D$30)),STPH!$D$11:$D$30),1))</f>
         <v>+III</v>
       </c>
       <c r="G37" s="9" t="str">
-        <f t="array" ref="G37">INDEX(GEKB!$K$11:$K$30,IFERROR(MATCH(MIN(IF(GEKB!$D$11:$D$30&gt;AVERAGE(B37,C37),GEKB!$D$11:$D$30)),GEKB!$D$11:$D$30),1))</f>
-        <v>+III</v>
-      </c>
-      <c r="H37" s="9">
-        <f t="array" ref="H37">INDEX(DA!$K$50:$K$71,IFERROR(MATCH(MIN(IF(DA!$D$50:$D$71&gt;AVERAGE(B37,C37),DA!$D$50:$D$71)),DA!$D$50:$D$71),1))</f>
-        <v>0</v>
-      </c>
-      <c r="I37" s="9" t="str">
-        <f t="array" ref="I37">INDEX(STKWp!$K$11:$K$30,IFERROR(MATCH(MIN(IF(STKWp!$D$11:$D$30&gt;AVERAGE(B37,C37),STKWp!$D$11:$D$30)),STKWp!$D$11:$D$30),1))</f>
-        <v>+III</v>
+        <f t="array" ref="G37">INDEX(STBI!$O$11:$O$30,IFERROR(MATCH(MIN(IF(STBI!$D$11:$D$30&gt;AVERAGE(B37,C37),STBI!$D$11:$D$30)),STBI!$D$11:$D$30),1))</f>
+        <v>+III</v>
+      </c>
+      <c r="H37" s="9" t="str">
+        <f t="array" ref="H37">INDEX(GEKB!$K$11:$K$30,IFERROR(MATCH(MIN(IF(GEKB!$D$11:$D$30&gt;AVERAGE(B37,C37),GEKB!$D$11:$D$30)),GEKB!$D$11:$D$30),1))</f>
+        <v>+III</v>
+      </c>
+      <c r="I37" s="9">
+        <f t="array" ref="I37">INDEX(DA!$K$50:$K$71,IFERROR(MATCH(MIN(IF(DA!$D$50:$D$71&gt;AVERAGE(B37,C37),DA!$D$50:$D$71)),DA!$D$50:$D$71),1))</f>
+        <v>0</v>
       </c>
       <c r="J37" s="9" t="str">
-        <f t="array" ref="J37">INDEX(BSKW!$K$11:$K$30,IFERROR(MATCH(MIN(IF(BSKW!$D$11:$D$30&gt;AVERAGE(B37,C37),BSKW!$D$11:$D$30)),BSKW!$D$11:$D$30),1))</f>
-        <v>+III</v>
-      </c>
-      <c r="K37" s="12" t="str">
-        <f t="array" ref="K37">INDEX(HTKW!$K$11:$K$30,IFERROR(MATCH(MIN(IF(HTKW!$D$11:$D$30&gt;AVERAGE(B37,C37),HTKW!$D$11:$D$30)),HTKW!$D$11:$D$30),1))</f>
-        <v>+III</v>
-      </c>
-    </row>
-    <row r="38" spans="2:11" x14ac:dyDescent="0.25">
+        <f t="array" ref="J37">INDEX(STKWp!$K$11:$K$30,IFERROR(MATCH(MIN(IF(STKWp!$D$11:$D$30&gt;AVERAGE(B37,C37),STKWp!$D$11:$D$30)),STKWp!$D$11:$D$30),1))</f>
+        <v>+III</v>
+      </c>
+      <c r="K37" s="9" t="str">
+        <f t="array" ref="K37">INDEX(BSKW!$K$11:$K$30,IFERROR(MATCH(MIN(IF(BSKW!$D$11:$D$30&gt;AVERAGE(B37,C37),BSKW!$D$11:$D$30)),BSKW!$D$11:$D$30),1))</f>
+        <v>+III</v>
+      </c>
+      <c r="L37" s="12" t="str">
+        <f t="array" ref="L37">INDEX(HTKW!$K$11:$K$30,IFERROR(MATCH(MIN(IF(HTKW!$D$11:$D$30&gt;AVERAGE(B37,C37),HTKW!$D$11:$D$30)),HTKW!$D$11:$D$30),1))</f>
+        <v>+III</v>
+      </c>
+    </row>
+    <row r="38" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B38" s="8">
         <v>5.2140000000000004</v>
       </c>
@@ -3932,36 +4079,40 @@
         <f t="shared" si="0"/>
         <v>+0</v>
       </c>
-      <c r="E38" s="9" t="str">
-        <f t="array" ref="E38">INDEX(STPH!$O$11:$O$30,IFERROR(MATCH(MIN(IF(STPH!$D$11:$D$30&gt;AVERAGE(B38,C38),STPH!$D$11:$D$30)),STPH!$D$11:$D$30),1))</f>
-        <v>+III</v>
+      <c r="E38" s="23" t="str">
+        <f t="shared" si="1"/>
+        <v>+0</v>
       </c>
       <c r="F38" s="9" t="str">
-        <f t="array" ref="F38">INDEX(STBI!$O$11:$O$30,IFERROR(MATCH(MIN(IF(STBI!$D$11:$D$30&gt;AVERAGE(B38,C38),STBI!$D$11:$D$30)),STBI!$D$11:$D$30),1))</f>
+        <f t="array" ref="F38">INDEX(STPH!$O$11:$O$30,IFERROR(MATCH(MIN(IF(STPH!$D$11:$D$30&gt;AVERAGE(B38,C38),STPH!$D$11:$D$30)),STPH!$D$11:$D$30),1))</f>
         <v>+III</v>
       </c>
       <c r="G38" s="9" t="str">
-        <f t="array" ref="G38">INDEX(GEKB!$K$11:$K$30,IFERROR(MATCH(MIN(IF(GEKB!$D$11:$D$30&gt;AVERAGE(B38,C38),GEKB!$D$11:$D$30)),GEKB!$D$11:$D$30),1))</f>
-        <v>+III</v>
-      </c>
-      <c r="H38" s="9">
-        <f t="array" ref="H38">INDEX(DA!$K$50:$K$71,IFERROR(MATCH(MIN(IF(DA!$D$50:$D$71&gt;AVERAGE(B38,C38),DA!$D$50:$D$71)),DA!$D$50:$D$71),1))</f>
-        <v>0</v>
-      </c>
-      <c r="I38" s="9" t="str">
-        <f t="array" ref="I38">INDEX(STKWp!$K$11:$K$30,IFERROR(MATCH(MIN(IF(STKWp!$D$11:$D$30&gt;AVERAGE(B38,C38),STKWp!$D$11:$D$30)),STKWp!$D$11:$D$30),1))</f>
-        <v>+III</v>
+        <f t="array" ref="G38">INDEX(STBI!$O$11:$O$30,IFERROR(MATCH(MIN(IF(STBI!$D$11:$D$30&gt;AVERAGE(B38,C38),STBI!$D$11:$D$30)),STBI!$D$11:$D$30),1))</f>
+        <v>+III</v>
+      </c>
+      <c r="H38" s="9" t="str">
+        <f t="array" ref="H38">INDEX(GEKB!$K$11:$K$30,IFERROR(MATCH(MIN(IF(GEKB!$D$11:$D$30&gt;AVERAGE(B38,C38),GEKB!$D$11:$D$30)),GEKB!$D$11:$D$30),1))</f>
+        <v>+III</v>
+      </c>
+      <c r="I38" s="9">
+        <f t="array" ref="I38">INDEX(DA!$K$50:$K$71,IFERROR(MATCH(MIN(IF(DA!$D$50:$D$71&gt;AVERAGE(B38,C38),DA!$D$50:$D$71)),DA!$D$50:$D$71),1))</f>
+        <v>0</v>
       </c>
       <c r="J38" s="9" t="str">
-        <f t="array" ref="J38">INDEX(BSKW!$K$11:$K$30,IFERROR(MATCH(MIN(IF(BSKW!$D$11:$D$30&gt;AVERAGE(B38,C38),BSKW!$D$11:$D$30)),BSKW!$D$11:$D$30),1))</f>
-        <v>+III</v>
-      </c>
-      <c r="K38" s="12" t="str">
-        <f t="array" ref="K38">INDEX(HTKW!$K$11:$K$30,IFERROR(MATCH(MIN(IF(HTKW!$D$11:$D$30&gt;AVERAGE(B38,C38),HTKW!$D$11:$D$30)),HTKW!$D$11:$D$30),1))</f>
-        <v>+III</v>
-      </c>
-    </row>
-    <row r="39" spans="2:11" x14ac:dyDescent="0.25">
+        <f t="array" ref="J38">INDEX(STKWp!$K$11:$K$30,IFERROR(MATCH(MIN(IF(STKWp!$D$11:$D$30&gt;AVERAGE(B38,C38),STKWp!$D$11:$D$30)),STKWp!$D$11:$D$30),1))</f>
+        <v>+III</v>
+      </c>
+      <c r="K38" s="9" t="str">
+        <f t="array" ref="K38">INDEX(BSKW!$K$11:$K$30,IFERROR(MATCH(MIN(IF(BSKW!$D$11:$D$30&gt;AVERAGE(B38,C38),BSKW!$D$11:$D$30)),BSKW!$D$11:$D$30),1))</f>
+        <v>+III</v>
+      </c>
+      <c r="L38" s="12" t="str">
+        <f t="array" ref="L38">INDEX(HTKW!$K$11:$K$30,IFERROR(MATCH(MIN(IF(HTKW!$D$11:$D$30&gt;AVERAGE(B38,C38),HTKW!$D$11:$D$30)),HTKW!$D$11:$D$30),1))</f>
+        <v>+III</v>
+      </c>
+    </row>
+    <row r="39" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B39" s="8">
         <v>5.3390000000000004</v>
       </c>
@@ -3972,36 +4123,40 @@
         <f t="shared" si="0"/>
         <v>+0</v>
       </c>
-      <c r="E39" s="9" t="str">
-        <f t="array" ref="E39">INDEX(STPH!$O$11:$O$30,IFERROR(MATCH(MIN(IF(STPH!$D$11:$D$30&gt;AVERAGE(B39,C39),STPH!$D$11:$D$30)),STPH!$D$11:$D$30),1))</f>
-        <v>+III</v>
+      <c r="E39" s="23" t="str">
+        <f t="shared" si="1"/>
+        <v>+0</v>
       </c>
       <c r="F39" s="9" t="str">
-        <f t="array" ref="F39">INDEX(STBI!$O$11:$O$30,IFERROR(MATCH(MIN(IF(STBI!$D$11:$D$30&gt;AVERAGE(B39,C39),STBI!$D$11:$D$30)),STBI!$D$11:$D$30),1))</f>
+        <f t="array" ref="F39">INDEX(STPH!$O$11:$O$30,IFERROR(MATCH(MIN(IF(STPH!$D$11:$D$30&gt;AVERAGE(B39,C39),STPH!$D$11:$D$30)),STPH!$D$11:$D$30),1))</f>
         <v>+III</v>
       </c>
       <c r="G39" s="9" t="str">
-        <f t="array" ref="G39">INDEX(GEKB!$K$11:$K$30,IFERROR(MATCH(MIN(IF(GEKB!$D$11:$D$30&gt;AVERAGE(B39,C39),GEKB!$D$11:$D$30)),GEKB!$D$11:$D$30),1))</f>
-        <v>+III</v>
-      </c>
-      <c r="H39" s="9">
-        <f t="array" ref="H39">INDEX(DA!$K$50:$K$71,IFERROR(MATCH(MIN(IF(DA!$D$50:$D$71&gt;AVERAGE(B39,C39),DA!$D$50:$D$71)),DA!$D$50:$D$71),1))</f>
-        <v>0</v>
-      </c>
-      <c r="I39" s="9" t="str">
-        <f t="array" ref="I39">INDEX(STKWp!$K$11:$K$30,IFERROR(MATCH(MIN(IF(STKWp!$D$11:$D$30&gt;AVERAGE(B39,C39),STKWp!$D$11:$D$30)),STKWp!$D$11:$D$30),1))</f>
-        <v>+III</v>
+        <f t="array" ref="G39">INDEX(STBI!$O$11:$O$30,IFERROR(MATCH(MIN(IF(STBI!$D$11:$D$30&gt;AVERAGE(B39,C39),STBI!$D$11:$D$30)),STBI!$D$11:$D$30),1))</f>
+        <v>+III</v>
+      </c>
+      <c r="H39" s="9" t="str">
+        <f t="array" ref="H39">INDEX(GEKB!$K$11:$K$30,IFERROR(MATCH(MIN(IF(GEKB!$D$11:$D$30&gt;AVERAGE(B39,C39),GEKB!$D$11:$D$30)),GEKB!$D$11:$D$30),1))</f>
+        <v>+III</v>
+      </c>
+      <c r="I39" s="9">
+        <f t="array" ref="I39">INDEX(DA!$K$50:$K$71,IFERROR(MATCH(MIN(IF(DA!$D$50:$D$71&gt;AVERAGE(B39,C39),DA!$D$50:$D$71)),DA!$D$50:$D$71),1))</f>
+        <v>0</v>
       </c>
       <c r="J39" s="9" t="str">
-        <f t="array" ref="J39">INDEX(BSKW!$K$11:$K$30,IFERROR(MATCH(MIN(IF(BSKW!$D$11:$D$30&gt;AVERAGE(B39,C39),BSKW!$D$11:$D$30)),BSKW!$D$11:$D$30),1))</f>
-        <v>+III</v>
-      </c>
-      <c r="K39" s="12" t="str">
-        <f t="array" ref="K39">INDEX(HTKW!$K$11:$K$30,IFERROR(MATCH(MIN(IF(HTKW!$D$11:$D$30&gt;AVERAGE(B39,C39),HTKW!$D$11:$D$30)),HTKW!$D$11:$D$30),1))</f>
-        <v>+III</v>
-      </c>
-    </row>
-    <row r="40" spans="2:11" x14ac:dyDescent="0.25">
+        <f t="array" ref="J39">INDEX(STKWp!$K$11:$K$30,IFERROR(MATCH(MIN(IF(STKWp!$D$11:$D$30&gt;AVERAGE(B39,C39),STKWp!$D$11:$D$30)),STKWp!$D$11:$D$30),1))</f>
+        <v>+III</v>
+      </c>
+      <c r="K39" s="9" t="str">
+        <f t="array" ref="K39">INDEX(BSKW!$K$11:$K$30,IFERROR(MATCH(MIN(IF(BSKW!$D$11:$D$30&gt;AVERAGE(B39,C39),BSKW!$D$11:$D$30)),BSKW!$D$11:$D$30),1))</f>
+        <v>+III</v>
+      </c>
+      <c r="L39" s="12" t="str">
+        <f t="array" ref="L39">INDEX(HTKW!$K$11:$K$30,IFERROR(MATCH(MIN(IF(HTKW!$D$11:$D$30&gt;AVERAGE(B39,C39),HTKW!$D$11:$D$30)),HTKW!$D$11:$D$30),1))</f>
+        <v>+III</v>
+      </c>
+    </row>
+    <row r="40" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B40" s="8">
         <v>5.4950000000000001</v>
       </c>
@@ -4012,844 +4167,914 @@
         <f t="shared" si="0"/>
         <v>+0</v>
       </c>
-      <c r="E40" s="9" t="str">
-        <f t="array" ref="E40">INDEX(STPH!$O$11:$O$30,IFERROR(MATCH(MIN(IF(STPH!$D$11:$D$30&gt;AVERAGE(B40,C40),STPH!$D$11:$D$30)),STPH!$D$11:$D$30),1))</f>
-        <v>+III</v>
+      <c r="E40" s="23" t="str">
+        <f t="shared" si="1"/>
+        <v>+0</v>
       </c>
       <c r="F40" s="9" t="str">
-        <f t="array" ref="F40">INDEX(STBI!$O$11:$O$30,IFERROR(MATCH(MIN(IF(STBI!$D$11:$D$30&gt;AVERAGE(B40,C40),STBI!$D$11:$D$30)),STBI!$D$11:$D$30),1))</f>
+        <f t="array" ref="F40">INDEX(STPH!$O$11:$O$30,IFERROR(MATCH(MIN(IF(STPH!$D$11:$D$30&gt;AVERAGE(B40,C40),STPH!$D$11:$D$30)),STPH!$D$11:$D$30),1))</f>
         <v>+III</v>
       </c>
       <c r="G40" s="9" t="str">
-        <f t="array" ref="G40">INDEX(GEKB!$K$11:$K$30,IFERROR(MATCH(MIN(IF(GEKB!$D$11:$D$30&gt;AVERAGE(B40,C40),GEKB!$D$11:$D$30)),GEKB!$D$11:$D$30),1))</f>
-        <v>+III</v>
-      </c>
-      <c r="H40" s="9">
-        <f t="array" ref="H40">INDEX(DA!$K$50:$K$71,IFERROR(MATCH(MIN(IF(DA!$D$50:$D$71&gt;AVERAGE(B40,C40),DA!$D$50:$D$71)),DA!$D$50:$D$71),1))</f>
-        <v>0</v>
-      </c>
-      <c r="I40" s="9" t="str">
-        <f t="array" ref="I40">INDEX(STKWp!$K$11:$K$30,IFERROR(MATCH(MIN(IF(STKWp!$D$11:$D$30&gt;AVERAGE(B40,C40),STKWp!$D$11:$D$30)),STKWp!$D$11:$D$30),1))</f>
-        <v>+III</v>
+        <f t="array" ref="G40">INDEX(STBI!$O$11:$O$30,IFERROR(MATCH(MIN(IF(STBI!$D$11:$D$30&gt;AVERAGE(B40,C40),STBI!$D$11:$D$30)),STBI!$D$11:$D$30),1))</f>
+        <v>+III</v>
+      </c>
+      <c r="H40" s="9" t="str">
+        <f t="array" ref="H40">INDEX(GEKB!$K$11:$K$30,IFERROR(MATCH(MIN(IF(GEKB!$D$11:$D$30&gt;AVERAGE(B40,C40),GEKB!$D$11:$D$30)),GEKB!$D$11:$D$30),1))</f>
+        <v>+III</v>
+      </c>
+      <c r="I40" s="9">
+        <f t="array" ref="I40">INDEX(DA!$K$50:$K$71,IFERROR(MATCH(MIN(IF(DA!$D$50:$D$71&gt;AVERAGE(B40,C40),DA!$D$50:$D$71)),DA!$D$50:$D$71),1))</f>
+        <v>0</v>
       </c>
       <c r="J40" s="9" t="str">
-        <f t="array" ref="J40">INDEX(BSKW!$K$11:$K$30,IFERROR(MATCH(MIN(IF(BSKW!$D$11:$D$30&gt;AVERAGE(B40,C40),BSKW!$D$11:$D$30)),BSKW!$D$11:$D$30),1))</f>
-        <v>+III</v>
-      </c>
-      <c r="K40" s="12" t="str">
-        <f t="array" ref="K40">INDEX(HTKW!$K$11:$K$30,IFERROR(MATCH(MIN(IF(HTKW!$D$11:$D$30&gt;AVERAGE(B40,C40),HTKW!$D$11:$D$30)),HTKW!$D$11:$D$30),1))</f>
-        <v>+III</v>
-      </c>
-    </row>
-    <row r="41" spans="2:11" x14ac:dyDescent="0.25">
+        <f t="array" ref="J40">INDEX(STKWp!$K$11:$K$30,IFERROR(MATCH(MIN(IF(STKWp!$D$11:$D$30&gt;AVERAGE(B40,C40),STKWp!$D$11:$D$30)),STKWp!$D$11:$D$30),1))</f>
+        <v>+III</v>
+      </c>
+      <c r="K40" s="9" t="str">
+        <f t="array" ref="K40">INDEX(BSKW!$K$11:$K$30,IFERROR(MATCH(MIN(IF(BSKW!$D$11:$D$30&gt;AVERAGE(B40,C40),BSKW!$D$11:$D$30)),BSKW!$D$11:$D$30),1))</f>
+        <v>+III</v>
+      </c>
+      <c r="L40" s="12" t="str">
+        <f t="array" ref="L40">INDEX(HTKW!$K$11:$K$30,IFERROR(MATCH(MIN(IF(HTKW!$D$11:$D$30&gt;AVERAGE(B40,C40),HTKW!$D$11:$D$30)),HTKW!$D$11:$D$30),1))</f>
+        <v>+III</v>
+      </c>
+    </row>
+    <row r="41" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B41" s="8"/>
       <c r="C41" s="9"/>
       <c r="D41" s="23"/>
-      <c r="E41" s="9"/>
+      <c r="E41" s="23"/>
       <c r="F41" s="9"/>
       <c r="G41" s="9"/>
       <c r="H41" s="9"/>
       <c r="I41" s="9"/>
       <c r="J41" s="9"/>
-      <c r="K41" s="12"/>
-    </row>
-    <row r="42" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="K41" s="9"/>
+      <c r="L41" s="12"/>
+    </row>
+    <row r="42" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B42" s="8"/>
       <c r="C42" s="9"/>
       <c r="D42" s="23"/>
-      <c r="E42" s="9"/>
+      <c r="E42" s="23"/>
       <c r="F42" s="9"/>
       <c r="G42" s="9"/>
       <c r="H42" s="9"/>
       <c r="I42" s="9"/>
       <c r="J42" s="9"/>
-      <c r="K42" s="12"/>
-    </row>
-    <row r="43" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="K42" s="9"/>
+      <c r="L42" s="12"/>
+    </row>
+    <row r="43" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B43" s="8"/>
       <c r="C43" s="9"/>
       <c r="D43" s="23"/>
-      <c r="E43" s="9"/>
+      <c r="E43" s="23"/>
       <c r="F43" s="9"/>
       <c r="G43" s="9"/>
       <c r="H43" s="9"/>
       <c r="I43" s="9"/>
       <c r="J43" s="9"/>
-      <c r="K43" s="12"/>
-    </row>
-    <row r="44" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="K43" s="9"/>
+      <c r="L43" s="12"/>
+    </row>
+    <row r="44" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B44" s="8"/>
       <c r="C44" s="9"/>
       <c r="D44" s="23"/>
-      <c r="E44" s="9"/>
+      <c r="E44" s="23"/>
       <c r="F44" s="9"/>
       <c r="G44" s="9"/>
       <c r="H44" s="9"/>
       <c r="I44" s="9"/>
       <c r="J44" s="9"/>
-      <c r="K44" s="12"/>
-    </row>
-    <row r="45" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="K44" s="9"/>
+      <c r="L44" s="12"/>
+    </row>
+    <row r="45" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B45" s="8"/>
       <c r="C45" s="9"/>
       <c r="D45" s="23"/>
-      <c r="E45" s="9"/>
+      <c r="E45" s="23"/>
       <c r="F45" s="9"/>
       <c r="G45" s="9"/>
       <c r="H45" s="9"/>
       <c r="I45" s="9"/>
       <c r="J45" s="9"/>
-      <c r="K45" s="12"/>
-    </row>
-    <row r="46" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="K45" s="9"/>
+      <c r="L45" s="12"/>
+    </row>
+    <row r="46" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B46" s="8"/>
       <c r="C46" s="9"/>
       <c r="D46" s="23"/>
-      <c r="E46" s="9"/>
+      <c r="E46" s="23"/>
       <c r="F46" s="9"/>
       <c r="G46" s="9"/>
       <c r="H46" s="9"/>
       <c r="I46" s="9"/>
       <c r="J46" s="9"/>
-      <c r="K46" s="12"/>
-    </row>
-    <row r="47" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="K46" s="9"/>
+      <c r="L46" s="12"/>
+    </row>
+    <row r="47" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B47" s="8"/>
       <c r="C47" s="9"/>
       <c r="D47" s="23"/>
-      <c r="E47" s="9"/>
+      <c r="E47" s="23"/>
       <c r="F47" s="9"/>
       <c r="G47" s="9"/>
       <c r="H47" s="9"/>
       <c r="I47" s="9"/>
       <c r="J47" s="9"/>
-      <c r="K47" s="12"/>
-    </row>
-    <row r="48" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="K47" s="9"/>
+      <c r="L47" s="12"/>
+    </row>
+    <row r="48" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B48" s="8"/>
       <c r="C48" s="9"/>
       <c r="D48" s="23"/>
-      <c r="E48" s="9"/>
+      <c r="E48" s="23"/>
       <c r="F48" s="9"/>
       <c r="G48" s="9"/>
       <c r="H48" s="9"/>
       <c r="I48" s="9"/>
       <c r="J48" s="9"/>
-      <c r="K48" s="12"/>
-    </row>
-    <row r="49" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="K48" s="9"/>
+      <c r="L48" s="12"/>
+    </row>
+    <row r="49" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B49" s="8"/>
       <c r="C49" s="9"/>
       <c r="D49" s="23"/>
-      <c r="E49" s="9"/>
+      <c r="E49" s="23"/>
       <c r="F49" s="9"/>
       <c r="G49" s="9"/>
       <c r="H49" s="9"/>
       <c r="I49" s="9"/>
       <c r="J49" s="9"/>
-      <c r="K49" s="12"/>
-    </row>
-    <row r="50" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="K49" s="9"/>
+      <c r="L49" s="12"/>
+    </row>
+    <row r="50" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B50" s="8"/>
       <c r="C50" s="9"/>
       <c r="D50" s="23"/>
-      <c r="E50" s="9"/>
+      <c r="E50" s="23"/>
       <c r="F50" s="9"/>
       <c r="G50" s="9"/>
       <c r="H50" s="9"/>
       <c r="I50" s="9"/>
       <c r="J50" s="9"/>
-      <c r="K50" s="12"/>
-    </row>
-    <row r="51" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="K50" s="9"/>
+      <c r="L50" s="12"/>
+    </row>
+    <row r="51" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B51" s="8"/>
       <c r="C51" s="9"/>
       <c r="D51" s="23"/>
-      <c r="E51" s="9"/>
+      <c r="E51" s="23"/>
       <c r="F51" s="9"/>
       <c r="G51" s="9"/>
       <c r="H51" s="9"/>
       <c r="I51" s="9"/>
       <c r="J51" s="9"/>
-      <c r="K51" s="12"/>
-    </row>
-    <row r="52" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="K51" s="9"/>
+      <c r="L51" s="12"/>
+    </row>
+    <row r="52" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B52" s="8"/>
       <c r="C52" s="9"/>
       <c r="D52" s="23"/>
-      <c r="E52" s="9"/>
+      <c r="E52" s="23"/>
       <c r="F52" s="9"/>
       <c r="G52" s="9"/>
       <c r="H52" s="9"/>
       <c r="I52" s="9"/>
       <c r="J52" s="9"/>
-      <c r="K52" s="12"/>
-    </row>
-    <row r="53" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="K52" s="9"/>
+      <c r="L52" s="12"/>
+    </row>
+    <row r="53" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B53" s="8"/>
       <c r="C53" s="9"/>
       <c r="D53" s="23"/>
-      <c r="E53" s="9"/>
+      <c r="E53" s="23"/>
       <c r="F53" s="9"/>
       <c r="G53" s="9"/>
       <c r="H53" s="9"/>
       <c r="I53" s="9"/>
       <c r="J53" s="9"/>
-      <c r="K53" s="12"/>
-    </row>
-    <row r="54" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="K53" s="9"/>
+      <c r="L53" s="12"/>
+    </row>
+    <row r="54" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B54" s="8"/>
       <c r="C54" s="9"/>
       <c r="D54" s="23"/>
-      <c r="E54" s="9"/>
+      <c r="E54" s="23"/>
       <c r="F54" s="9"/>
       <c r="G54" s="9"/>
       <c r="H54" s="9"/>
       <c r="I54" s="9"/>
       <c r="J54" s="9"/>
-      <c r="K54" s="12"/>
-    </row>
-    <row r="55" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="K54" s="9"/>
+      <c r="L54" s="12"/>
+    </row>
+    <row r="55" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B55" s="8"/>
       <c r="C55" s="9"/>
       <c r="D55" s="23"/>
-      <c r="E55" s="9"/>
+      <c r="E55" s="23"/>
       <c r="F55" s="9"/>
       <c r="G55" s="9"/>
       <c r="H55" s="9"/>
       <c r="I55" s="9"/>
       <c r="J55" s="9"/>
-      <c r="K55" s="12"/>
-    </row>
-    <row r="56" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="K55" s="9"/>
+      <c r="L55" s="12"/>
+    </row>
+    <row r="56" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B56" s="8"/>
       <c r="C56" s="9"/>
       <c r="D56" s="23"/>
-      <c r="E56" s="9"/>
+      <c r="E56" s="23"/>
       <c r="F56" s="9"/>
       <c r="G56" s="9"/>
       <c r="H56" s="9"/>
       <c r="I56" s="9"/>
       <c r="J56" s="9"/>
-      <c r="K56" s="12"/>
-    </row>
-    <row r="57" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="K56" s="9"/>
+      <c r="L56" s="12"/>
+    </row>
+    <row r="57" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B57" s="8"/>
       <c r="C57" s="9"/>
       <c r="D57" s="23"/>
-      <c r="E57" s="9"/>
+      <c r="E57" s="23"/>
       <c r="F57" s="9"/>
       <c r="G57" s="9"/>
       <c r="H57" s="9"/>
       <c r="I57" s="9"/>
       <c r="J57" s="9"/>
-      <c r="K57" s="12"/>
-    </row>
-    <row r="58" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="K57" s="9"/>
+      <c r="L57" s="12"/>
+    </row>
+    <row r="58" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B58" s="8"/>
       <c r="C58" s="9"/>
       <c r="D58" s="23"/>
-      <c r="E58" s="9"/>
+      <c r="E58" s="23"/>
       <c r="F58" s="9"/>
       <c r="G58" s="9"/>
       <c r="H58" s="9"/>
       <c r="I58" s="9"/>
       <c r="J58" s="9"/>
-      <c r="K58" s="12"/>
-    </row>
-    <row r="59" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="K58" s="9"/>
+      <c r="L58" s="12"/>
+    </row>
+    <row r="59" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B59" s="8"/>
       <c r="C59" s="9"/>
       <c r="D59" s="23"/>
-      <c r="E59" s="9"/>
+      <c r="E59" s="23"/>
       <c r="F59" s="9"/>
       <c r="G59" s="9"/>
       <c r="H59" s="9"/>
       <c r="I59" s="9"/>
       <c r="J59" s="9"/>
-      <c r="K59" s="12"/>
-    </row>
-    <row r="60" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="K59" s="9"/>
+      <c r="L59" s="12"/>
+    </row>
+    <row r="60" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B60" s="8"/>
       <c r="C60" s="9"/>
       <c r="D60" s="23"/>
-      <c r="E60" s="9"/>
+      <c r="E60" s="23"/>
       <c r="F60" s="9"/>
       <c r="G60" s="9"/>
       <c r="H60" s="9"/>
       <c r="I60" s="9"/>
       <c r="J60" s="9"/>
-      <c r="K60" s="12"/>
-    </row>
-    <row r="61" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="K60" s="9"/>
+      <c r="L60" s="12"/>
+    </row>
+    <row r="61" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B61" s="8"/>
       <c r="C61" s="9"/>
       <c r="D61" s="23"/>
-      <c r="E61" s="9"/>
+      <c r="E61" s="23"/>
       <c r="F61" s="9"/>
       <c r="G61" s="9"/>
       <c r="H61" s="9"/>
       <c r="I61" s="9"/>
       <c r="J61" s="9"/>
-      <c r="K61" s="12"/>
-    </row>
-    <row r="62" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="K61" s="9"/>
+      <c r="L61" s="12"/>
+    </row>
+    <row r="62" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B62" s="8"/>
       <c r="C62" s="9"/>
       <c r="D62" s="23"/>
-      <c r="E62" s="9"/>
+      <c r="E62" s="23"/>
       <c r="F62" s="9"/>
       <c r="G62" s="9"/>
       <c r="H62" s="9"/>
       <c r="I62" s="9"/>
       <c r="J62" s="9"/>
-      <c r="K62" s="12"/>
-    </row>
-    <row r="63" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="K62" s="9"/>
+      <c r="L62" s="12"/>
+    </row>
+    <row r="63" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B63" s="8"/>
       <c r="C63" s="9"/>
       <c r="D63" s="23"/>
-      <c r="E63" s="9"/>
+      <c r="E63" s="23"/>
       <c r="F63" s="9"/>
       <c r="G63" s="9"/>
       <c r="H63" s="9"/>
       <c r="I63" s="9"/>
       <c r="J63" s="9"/>
-      <c r="K63" s="12"/>
-    </row>
-    <row r="64" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="K63" s="9"/>
+      <c r="L63" s="12"/>
+    </row>
+    <row r="64" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B64" s="8"/>
       <c r="C64" s="9"/>
       <c r="D64" s="23"/>
-      <c r="E64" s="9"/>
+      <c r="E64" s="23"/>
       <c r="F64" s="9"/>
       <c r="G64" s="9"/>
       <c r="H64" s="9"/>
       <c r="I64" s="9"/>
       <c r="J64" s="9"/>
-      <c r="K64" s="12"/>
-    </row>
-    <row r="65" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="K64" s="9"/>
+      <c r="L64" s="12"/>
+    </row>
+    <row r="65" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B65" s="8"/>
       <c r="C65" s="9"/>
       <c r="D65" s="23"/>
-      <c r="E65" s="9"/>
+      <c r="E65" s="23"/>
       <c r="F65" s="9"/>
       <c r="G65" s="9"/>
       <c r="H65" s="9"/>
       <c r="I65" s="9"/>
       <c r="J65" s="9"/>
-      <c r="K65" s="12"/>
-    </row>
-    <row r="66" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="K65" s="9"/>
+      <c r="L65" s="12"/>
+    </row>
+    <row r="66" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B66" s="8"/>
       <c r="C66" s="9"/>
       <c r="D66" s="23"/>
-      <c r="E66" s="9"/>
+      <c r="E66" s="23"/>
       <c r="F66" s="9"/>
       <c r="G66" s="9"/>
       <c r="H66" s="9"/>
       <c r="I66" s="9"/>
       <c r="J66" s="9"/>
-      <c r="K66" s="12"/>
-    </row>
-    <row r="67" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="K66" s="9"/>
+      <c r="L66" s="12"/>
+    </row>
+    <row r="67" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B67" s="8"/>
       <c r="C67" s="9"/>
       <c r="D67" s="23"/>
-      <c r="E67" s="9"/>
+      <c r="E67" s="23"/>
       <c r="F67" s="9"/>
       <c r="G67" s="9"/>
       <c r="H67" s="9"/>
       <c r="I67" s="9"/>
       <c r="J67" s="9"/>
-      <c r="K67" s="12"/>
-    </row>
-    <row r="68" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="K67" s="9"/>
+      <c r="L67" s="12"/>
+    </row>
+    <row r="68" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B68" s="8"/>
       <c r="C68" s="9"/>
       <c r="D68" s="23"/>
-      <c r="E68" s="9"/>
+      <c r="E68" s="23"/>
       <c r="F68" s="9"/>
       <c r="G68" s="9"/>
       <c r="H68" s="9"/>
       <c r="I68" s="9"/>
       <c r="J68" s="9"/>
-      <c r="K68" s="12"/>
-    </row>
-    <row r="69" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="K68" s="9"/>
+      <c r="L68" s="12"/>
+    </row>
+    <row r="69" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B69" s="8"/>
       <c r="C69" s="9"/>
       <c r="D69" s="23"/>
-      <c r="E69" s="9"/>
+      <c r="E69" s="23"/>
       <c r="F69" s="9"/>
       <c r="G69" s="9"/>
       <c r="H69" s="9"/>
       <c r="I69" s="9"/>
       <c r="J69" s="9"/>
-      <c r="K69" s="12"/>
-    </row>
-    <row r="70" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="K69" s="9"/>
+      <c r="L69" s="12"/>
+    </row>
+    <row r="70" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B70" s="8"/>
       <c r="C70" s="9"/>
       <c r="D70" s="23"/>
-      <c r="E70" s="9"/>
+      <c r="E70" s="23"/>
       <c r="F70" s="9"/>
       <c r="G70" s="9"/>
       <c r="H70" s="9"/>
       <c r="I70" s="9"/>
       <c r="J70" s="9"/>
-      <c r="K70" s="12"/>
-    </row>
-    <row r="71" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="K70" s="9"/>
+      <c r="L70" s="12"/>
+    </row>
+    <row r="71" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B71" s="8"/>
       <c r="C71" s="9"/>
       <c r="D71" s="23"/>
-      <c r="E71" s="9"/>
+      <c r="E71" s="23"/>
       <c r="F71" s="9"/>
       <c r="G71" s="9"/>
       <c r="H71" s="9"/>
       <c r="I71" s="9"/>
       <c r="J71" s="9"/>
-      <c r="K71" s="12"/>
-    </row>
-    <row r="72" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="K71" s="9"/>
+      <c r="L71" s="12"/>
+    </row>
+    <row r="72" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B72" s="8"/>
       <c r="C72" s="9"/>
       <c r="D72" s="23"/>
-      <c r="E72" s="9"/>
+      <c r="E72" s="23"/>
       <c r="F72" s="9"/>
       <c r="G72" s="9"/>
       <c r="H72" s="9"/>
       <c r="I72" s="9"/>
       <c r="J72" s="9"/>
-      <c r="K72" s="12"/>
-    </row>
-    <row r="73" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="K72" s="9"/>
+      <c r="L72" s="12"/>
+    </row>
+    <row r="73" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B73" s="8"/>
       <c r="C73" s="9"/>
       <c r="D73" s="23"/>
-      <c r="E73" s="9"/>
+      <c r="E73" s="23"/>
       <c r="F73" s="9"/>
       <c r="G73" s="9"/>
       <c r="H73" s="9"/>
       <c r="I73" s="9"/>
       <c r="J73" s="9"/>
-      <c r="K73" s="12"/>
-    </row>
-    <row r="74" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="K73" s="9"/>
+      <c r="L73" s="12"/>
+    </row>
+    <row r="74" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B74" s="8"/>
       <c r="C74" s="9"/>
       <c r="D74" s="23"/>
-      <c r="E74" s="9"/>
+      <c r="E74" s="23"/>
       <c r="F74" s="9"/>
       <c r="G74" s="9"/>
       <c r="H74" s="9"/>
       <c r="I74" s="9"/>
       <c r="J74" s="9"/>
-      <c r="K74" s="12"/>
-    </row>
-    <row r="75" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="K74" s="9"/>
+      <c r="L74" s="12"/>
+    </row>
+    <row r="75" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B75" s="8"/>
       <c r="C75" s="9"/>
       <c r="D75" s="23"/>
-      <c r="E75" s="9"/>
+      <c r="E75" s="23"/>
       <c r="F75" s="9"/>
       <c r="G75" s="9"/>
       <c r="H75" s="9"/>
       <c r="I75" s="9"/>
       <c r="J75" s="9"/>
-      <c r="K75" s="12"/>
-    </row>
-    <row r="76" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="K75" s="9"/>
+      <c r="L75" s="12"/>
+    </row>
+    <row r="76" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B76" s="8"/>
       <c r="C76" s="9"/>
       <c r="D76" s="23"/>
-      <c r="E76" s="9"/>
+      <c r="E76" s="23"/>
       <c r="F76" s="9"/>
       <c r="G76" s="9"/>
       <c r="H76" s="9"/>
       <c r="I76" s="9"/>
       <c r="J76" s="9"/>
-      <c r="K76" s="12"/>
-    </row>
-    <row r="77" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="K76" s="9"/>
+      <c r="L76" s="12"/>
+    </row>
+    <row r="77" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B77" s="8"/>
       <c r="C77" s="9"/>
       <c r="D77" s="23"/>
-      <c r="E77" s="9"/>
+      <c r="E77" s="23"/>
       <c r="F77" s="9"/>
       <c r="G77" s="9"/>
       <c r="H77" s="9"/>
       <c r="I77" s="9"/>
       <c r="J77" s="9"/>
-      <c r="K77" s="12"/>
-    </row>
-    <row r="78" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="K77" s="9"/>
+      <c r="L77" s="12"/>
+    </row>
+    <row r="78" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B78" s="8"/>
       <c r="C78" s="9"/>
       <c r="D78" s="23"/>
-      <c r="E78" s="9"/>
+      <c r="E78" s="23"/>
       <c r="F78" s="9"/>
       <c r="G78" s="9"/>
       <c r="H78" s="9"/>
       <c r="I78" s="9"/>
       <c r="J78" s="9"/>
-      <c r="K78" s="12"/>
-    </row>
-    <row r="79" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="K78" s="9"/>
+      <c r="L78" s="12"/>
+    </row>
+    <row r="79" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B79" s="8"/>
       <c r="C79" s="9"/>
       <c r="D79" s="23"/>
-      <c r="E79" s="9"/>
+      <c r="E79" s="23"/>
       <c r="F79" s="9"/>
       <c r="G79" s="9"/>
       <c r="H79" s="9"/>
       <c r="I79" s="9"/>
       <c r="J79" s="9"/>
-      <c r="K79" s="12"/>
-    </row>
-    <row r="80" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="K79" s="9"/>
+      <c r="L79" s="12"/>
+    </row>
+    <row r="80" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B80" s="8"/>
       <c r="C80" s="9"/>
       <c r="D80" s="23"/>
-      <c r="E80" s="9"/>
+      <c r="E80" s="23"/>
       <c r="F80" s="9"/>
       <c r="G80" s="9"/>
       <c r="H80" s="9"/>
       <c r="I80" s="9"/>
       <c r="J80" s="9"/>
-      <c r="K80" s="12"/>
-    </row>
-    <row r="81" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="K80" s="9"/>
+      <c r="L80" s="12"/>
+    </row>
+    <row r="81" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B81" s="8"/>
       <c r="C81" s="9"/>
       <c r="D81" s="23"/>
-      <c r="E81" s="9"/>
+      <c r="E81" s="23"/>
       <c r="F81" s="9"/>
       <c r="G81" s="9"/>
       <c r="H81" s="9"/>
       <c r="I81" s="9"/>
       <c r="J81" s="9"/>
-      <c r="K81" s="12"/>
-    </row>
-    <row r="82" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="K81" s="9"/>
+      <c r="L81" s="12"/>
+    </row>
+    <row r="82" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B82" s="8"/>
       <c r="C82" s="9"/>
       <c r="D82" s="23"/>
-      <c r="E82" s="9"/>
+      <c r="E82" s="23"/>
       <c r="F82" s="9"/>
       <c r="G82" s="9"/>
       <c r="H82" s="9"/>
       <c r="I82" s="9"/>
       <c r="J82" s="9"/>
-      <c r="K82" s="12"/>
-    </row>
-    <row r="83" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="K82" s="9"/>
+      <c r="L82" s="12"/>
+    </row>
+    <row r="83" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B83" s="8"/>
       <c r="C83" s="9"/>
       <c r="D83" s="23"/>
-      <c r="E83" s="9"/>
+      <c r="E83" s="23"/>
       <c r="F83" s="9"/>
       <c r="G83" s="9"/>
       <c r="H83" s="9"/>
       <c r="I83" s="9"/>
       <c r="J83" s="9"/>
-      <c r="K83" s="12"/>
-    </row>
-    <row r="84" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="K83" s="9"/>
+      <c r="L83" s="12"/>
+    </row>
+    <row r="84" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B84" s="8"/>
       <c r="C84" s="9"/>
       <c r="D84" s="23"/>
-      <c r="E84" s="9"/>
+      <c r="E84" s="23"/>
       <c r="F84" s="9"/>
       <c r="G84" s="9"/>
       <c r="H84" s="9"/>
       <c r="I84" s="9"/>
       <c r="J84" s="9"/>
-      <c r="K84" s="12"/>
-    </row>
-    <row r="85" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="K84" s="9"/>
+      <c r="L84" s="12"/>
+    </row>
+    <row r="85" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B85" s="8"/>
       <c r="C85" s="9"/>
       <c r="D85" s="23"/>
-      <c r="E85" s="9"/>
+      <c r="E85" s="23"/>
       <c r="F85" s="9"/>
       <c r="G85" s="9"/>
       <c r="H85" s="9"/>
       <c r="I85" s="9"/>
       <c r="J85" s="9"/>
-      <c r="K85" s="12"/>
-    </row>
-    <row r="86" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="K85" s="9"/>
+      <c r="L85" s="12"/>
+    </row>
+    <row r="86" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B86" s="8"/>
       <c r="C86" s="9"/>
       <c r="D86" s="23"/>
-      <c r="E86" s="9"/>
+      <c r="E86" s="23"/>
       <c r="F86" s="9"/>
       <c r="G86" s="9"/>
       <c r="H86" s="9"/>
       <c r="I86" s="9"/>
       <c r="J86" s="9"/>
-      <c r="K86" s="12"/>
-    </row>
-    <row r="87" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="K86" s="9"/>
+      <c r="L86" s="12"/>
+    </row>
+    <row r="87" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B87" s="8"/>
       <c r="C87" s="9"/>
       <c r="D87" s="23"/>
-      <c r="E87" s="9"/>
+      <c r="E87" s="23"/>
       <c r="F87" s="9"/>
       <c r="G87" s="9"/>
       <c r="H87" s="9"/>
       <c r="I87" s="9"/>
       <c r="J87" s="9"/>
-      <c r="K87" s="12"/>
-    </row>
-    <row r="88" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="K87" s="9"/>
+      <c r="L87" s="12"/>
+    </row>
+    <row r="88" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B88" s="8"/>
       <c r="C88" s="9"/>
       <c r="D88" s="23"/>
-      <c r="E88" s="9"/>
+      <c r="E88" s="23"/>
       <c r="F88" s="9"/>
       <c r="G88" s="9"/>
       <c r="H88" s="9"/>
       <c r="I88" s="9"/>
       <c r="J88" s="9"/>
-      <c r="K88" s="12"/>
-    </row>
-    <row r="89" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="K88" s="9"/>
+      <c r="L88" s="12"/>
+    </row>
+    <row r="89" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B89" s="8"/>
       <c r="C89" s="9"/>
       <c r="D89" s="23"/>
-      <c r="E89" s="9"/>
+      <c r="E89" s="23"/>
       <c r="F89" s="9"/>
       <c r="G89" s="9"/>
       <c r="H89" s="9"/>
       <c r="I89" s="9"/>
       <c r="J89" s="9"/>
-      <c r="K89" s="12"/>
-    </row>
-    <row r="90" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="K89" s="9"/>
+      <c r="L89" s="12"/>
+    </row>
+    <row r="90" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B90" s="8"/>
       <c r="C90" s="9"/>
       <c r="D90" s="23"/>
-      <c r="E90" s="9"/>
+      <c r="E90" s="23"/>
       <c r="F90" s="9"/>
       <c r="G90" s="9"/>
       <c r="H90" s="9"/>
       <c r="I90" s="9"/>
       <c r="J90" s="9"/>
-      <c r="K90" s="12"/>
-    </row>
-    <row r="91" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="K90" s="9"/>
+      <c r="L90" s="12"/>
+    </row>
+    <row r="91" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B91" s="8"/>
       <c r="C91" s="9"/>
       <c r="D91" s="23"/>
-      <c r="E91" s="9"/>
+      <c r="E91" s="23"/>
       <c r="F91" s="9"/>
       <c r="G91" s="9"/>
       <c r="H91" s="9"/>
       <c r="I91" s="9"/>
       <c r="J91" s="9"/>
-      <c r="K91" s="12"/>
-    </row>
-    <row r="92" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="K91" s="9"/>
+      <c r="L91" s="12"/>
+    </row>
+    <row r="92" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B92" s="8"/>
       <c r="C92" s="9"/>
       <c r="D92" s="23"/>
-      <c r="E92" s="9"/>
+      <c r="E92" s="23"/>
       <c r="F92" s="9"/>
       <c r="G92" s="9"/>
       <c r="H92" s="9"/>
       <c r="I92" s="9"/>
       <c r="J92" s="9"/>
-      <c r="K92" s="12"/>
-    </row>
-    <row r="93" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="K92" s="9"/>
+      <c r="L92" s="12"/>
+    </row>
+    <row r="93" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B93" s="8"/>
       <c r="C93" s="9"/>
       <c r="D93" s="23"/>
-      <c r="E93" s="9"/>
+      <c r="E93" s="23"/>
       <c r="F93" s="9"/>
       <c r="G93" s="9"/>
       <c r="H93" s="9"/>
       <c r="I93" s="9"/>
       <c r="J93" s="9"/>
-      <c r="K93" s="12"/>
-    </row>
-    <row r="94" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="K93" s="9"/>
+      <c r="L93" s="12"/>
+    </row>
+    <row r="94" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B94" s="8"/>
       <c r="C94" s="9"/>
       <c r="D94" s="23"/>
-      <c r="E94" s="9"/>
+      <c r="E94" s="23"/>
       <c r="F94" s="9"/>
       <c r="G94" s="9"/>
       <c r="H94" s="9"/>
       <c r="I94" s="9"/>
       <c r="J94" s="9"/>
-      <c r="K94" s="12"/>
-    </row>
-    <row r="95" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="K94" s="9"/>
+      <c r="L94" s="12"/>
+    </row>
+    <row r="95" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B95" s="8"/>
       <c r="C95" s="9"/>
       <c r="D95" s="23"/>
-      <c r="E95" s="9"/>
+      <c r="E95" s="23"/>
       <c r="F95" s="9"/>
       <c r="G95" s="9"/>
       <c r="H95" s="9"/>
       <c r="I95" s="9"/>
       <c r="J95" s="9"/>
-      <c r="K95" s="12"/>
-    </row>
-    <row r="96" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="K95" s="9"/>
+      <c r="L95" s="12"/>
+    </row>
+    <row r="96" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B96" s="8"/>
       <c r="C96" s="9"/>
       <c r="D96" s="23"/>
-      <c r="E96" s="9"/>
+      <c r="E96" s="23"/>
       <c r="F96" s="9"/>
       <c r="G96" s="9"/>
       <c r="H96" s="9"/>
       <c r="I96" s="9"/>
       <c r="J96" s="9"/>
-      <c r="K96" s="12"/>
-    </row>
-    <row r="97" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="K96" s="9"/>
+      <c r="L96" s="12"/>
+    </row>
+    <row r="97" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B97" s="8"/>
       <c r="C97" s="9"/>
       <c r="D97" s="23"/>
-      <c r="E97" s="9"/>
+      <c r="E97" s="23"/>
       <c r="F97" s="9"/>
       <c r="G97" s="9"/>
       <c r="H97" s="9"/>
       <c r="I97" s="9"/>
       <c r="J97" s="9"/>
-      <c r="K97" s="12"/>
-    </row>
-    <row r="98" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="K97" s="9"/>
+      <c r="L97" s="12"/>
+    </row>
+    <row r="98" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B98" s="8"/>
       <c r="C98" s="9"/>
       <c r="D98" s="23"/>
-      <c r="E98" s="9"/>
+      <c r="E98" s="23"/>
       <c r="F98" s="9"/>
       <c r="G98" s="9"/>
       <c r="H98" s="9"/>
       <c r="I98" s="9"/>
       <c r="J98" s="9"/>
-      <c r="K98" s="12"/>
-    </row>
-    <row r="99" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="K98" s="9"/>
+      <c r="L98" s="12"/>
+    </row>
+    <row r="99" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B99" s="8"/>
       <c r="C99" s="9"/>
       <c r="D99" s="23"/>
-      <c r="E99" s="9"/>
+      <c r="E99" s="23"/>
       <c r="F99" s="9"/>
       <c r="G99" s="9"/>
       <c r="H99" s="9"/>
       <c r="I99" s="9"/>
       <c r="J99" s="9"/>
-      <c r="K99" s="12"/>
-    </row>
-    <row r="100" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="K99" s="9"/>
+      <c r="L99" s="12"/>
+    </row>
+    <row r="100" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B100" s="8"/>
       <c r="C100" s="9"/>
       <c r="D100" s="23"/>
-      <c r="E100" s="9"/>
+      <c r="E100" s="23"/>
       <c r="F100" s="9"/>
       <c r="G100" s="9"/>
       <c r="H100" s="9"/>
       <c r="I100" s="9"/>
       <c r="J100" s="9"/>
-      <c r="K100" s="12"/>
-    </row>
-    <row r="101" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="K100" s="9"/>
+      <c r="L100" s="12"/>
+    </row>
+    <row r="101" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B101" s="8"/>
       <c r="C101" s="9"/>
       <c r="D101" s="23"/>
-      <c r="E101" s="9"/>
+      <c r="E101" s="23"/>
       <c r="F101" s="9"/>
       <c r="G101" s="9"/>
       <c r="H101" s="9"/>
       <c r="I101" s="9"/>
       <c r="J101" s="9"/>
-      <c r="K101" s="12"/>
-    </row>
-    <row r="102" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="K101" s="9"/>
+      <c r="L101" s="12"/>
+    </row>
+    <row r="102" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B102" s="8"/>
       <c r="C102" s="9"/>
       <c r="D102" s="23"/>
-      <c r="E102" s="9"/>
+      <c r="E102" s="23"/>
       <c r="F102" s="9"/>
       <c r="G102" s="9"/>
       <c r="H102" s="9"/>
       <c r="I102" s="9"/>
       <c r="J102" s="9"/>
-      <c r="K102" s="12"/>
-    </row>
-    <row r="103" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="K102" s="9"/>
+      <c r="L102" s="12"/>
+    </row>
+    <row r="103" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B103" s="8"/>
       <c r="C103" s="9"/>
       <c r="D103" s="23"/>
-      <c r="E103" s="9"/>
+      <c r="E103" s="23"/>
       <c r="F103" s="9"/>
       <c r="G103" s="9"/>
       <c r="H103" s="9"/>
       <c r="I103" s="9"/>
       <c r="J103" s="9"/>
-      <c r="K103" s="12"/>
-    </row>
-    <row r="104" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="K103" s="9"/>
+      <c r="L103" s="12"/>
+    </row>
+    <row r="104" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B104" s="8"/>
       <c r="C104" s="9"/>
       <c r="D104" s="23"/>
-      <c r="E104" s="9"/>
+      <c r="E104" s="23"/>
       <c r="F104" s="9"/>
       <c r="G104" s="9"/>
       <c r="H104" s="9"/>
       <c r="I104" s="9"/>
       <c r="J104" s="9"/>
-      <c r="K104" s="12"/>
-    </row>
-    <row r="105" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="K104" s="9"/>
+      <c r="L104" s="12"/>
+    </row>
+    <row r="105" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B105" s="8"/>
       <c r="C105" s="9"/>
       <c r="D105" s="23"/>
-      <c r="E105" s="9"/>
+      <c r="E105" s="23"/>
       <c r="F105" s="9"/>
       <c r="G105" s="9"/>
       <c r="H105" s="9"/>
       <c r="I105" s="9"/>
       <c r="J105" s="9"/>
-      <c r="K105" s="12"/>
-    </row>
-    <row r="106" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="K105" s="9"/>
+      <c r="L105" s="12"/>
+    </row>
+    <row r="106" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B106" s="13"/>
       <c r="C106" s="14"/>
       <c r="D106" s="24"/>
-      <c r="E106" s="14"/>
+      <c r="E106" s="24"/>
       <c r="F106" s="14"/>
       <c r="G106" s="14"/>
       <c r="H106" s="14"/>
       <c r="I106" s="14"/>
       <c r="J106" s="14"/>
-      <c r="K106" s="17"/>
-    </row>
-    <row r="107" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="K106" s="14"/>
+      <c r="L106" s="17"/>
+    </row>
+    <row r="107" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B107" s="9"/>
       <c r="C107" s="9"/>
     </row>
-    <row r="108" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="108" spans="2:12" x14ac:dyDescent="0.25">
       <c r="C108" s="9"/>
     </row>
-    <row r="109" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="109" spans="2:12" x14ac:dyDescent="0.25">
       <c r="C109" s="9"/>
     </row>
-    <row r="110" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="110" spans="2:12" x14ac:dyDescent="0.25">
       <c r="C110" s="9"/>
     </row>
-    <row r="111" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="111" spans="2:12" x14ac:dyDescent="0.25">
       <c r="C111" s="9"/>
     </row>
-    <row r="112" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="112" spans="2:12" x14ac:dyDescent="0.25">
       <c r="C112" s="9"/>
     </row>
     <row r="113" spans="3:3" x14ac:dyDescent="0.25">
@@ -4934,7 +5159,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{69CBD9B7-2F4E-4E0F-B0DE-0C76068107FF}">
   <dimension ref="A2:F33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>

</xml_diff>